<commit_message>
matrix e grafo de citacoes
</commit_message>
<xml_diff>
--- a/Experiment01_Resumo/Resumo_Exp01.xlsx
+++ b/Experiment01_Resumo/Resumo_Exp01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" firstSheet="7" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="507">
   <si>
     <t>Database search</t>
   </si>
@@ -1598,9 +1598,6 @@
     <t>basili2007a</t>
   </si>
   <si>
-    <t>münch2013b</t>
-  </si>
-  <si>
     <t>basili2007b</t>
   </si>
   <si>
@@ -1638,6 +1635,30 @@
   </si>
   <si>
     <t>mccoy1998a</t>
+  </si>
+  <si>
+    <t>debou2000a</t>
+  </si>
+  <si>
+    <t>hinley1995a</t>
+  </si>
+  <si>
+    <t>messnarz1999a</t>
+  </si>
+  <si>
+    <t>waina2001a</t>
+  </si>
+  <si>
+    <t>Não encontrado na Scopus</t>
+  </si>
+  <si>
+    <t>Não encontrado na Scopus. Nome deveria ser basili2014</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>münch2013c</t>
   </si>
 </sst>
 </file>
@@ -1736,7 +1757,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1872,6 +1893,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2324,7 +2351,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="233">
+  <cellXfs count="237">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2665,9 +2692,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -2787,6 +2811,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2922,7 +2947,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2943,7 +2968,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -3012,7 +3047,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3268,12 +3302,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="209728800"/>
-        <c:axId val="209728408"/>
+        <c:axId val="210937608"/>
+        <c:axId val="210933688"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="209728800"/>
+        <c:axId val="210937608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3305,7 +3339,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3366,7 +3399,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209728408"/>
+        <c:crossAx val="210933688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3374,7 +3407,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209728408"/>
+        <c:axId val="210933688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3425,7 +3458,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209728800"/>
+        <c:crossAx val="210937608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3439,7 +3472,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3648,7 +3680,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3736,12 +3767,12 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:shape val="box"/>
-        <c:axId val="209729192"/>
-        <c:axId val="209729584"/>
+        <c:axId val="210934472"/>
+        <c:axId val="210934864"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="209729192"/>
+        <c:axId val="210934472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3770,7 +3801,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3831,7 +3861,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209729584"/>
+        <c:crossAx val="210934864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3839,7 +3869,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209729584"/>
+        <c:axId val="210934864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3868,7 +3898,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3923,7 +3952,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209729192"/>
+        <c:crossAx val="210934472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3937,7 +3966,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4122,7 +4150,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -4210,12 +4237,12 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:shape val="box"/>
-        <c:axId val="209726840"/>
-        <c:axId val="209731936"/>
+        <c:axId val="210936432"/>
+        <c:axId val="210935648"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="209726840"/>
+        <c:axId val="210936432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4244,7 +4271,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4305,7 +4331,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209731936"/>
+        <c:crossAx val="210935648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4313,7 +4339,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209731936"/>
+        <c:axId val="210935648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4342,7 +4368,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4397,7 +4422,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209726840"/>
+        <c:crossAx val="210936432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4411,7 +4436,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5186,12 +5210,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="209727624"/>
-        <c:axId val="209730760"/>
+        <c:axId val="210936040"/>
+        <c:axId val="210938392"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="209727624"/>
+        <c:axId val="210936040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5231,7 +5255,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209730760"/>
+        <c:crossAx val="210938392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5239,7 +5263,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209730760"/>
+        <c:axId val="210938392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5287,7 +5311,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209727624"/>
+        <c:crossAx val="210936040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5526,7 +5550,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -5597,8 +5620,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="210984632"/>
-        <c:axId val="210985024"/>
+        <c:axId val="292584800"/>
+        <c:axId val="292581272"/>
         <c:axId val="0"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -5768,7 +5791,7 @@
         </c:extLst>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="210984632"/>
+        <c:axId val="292584800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5800,7 +5823,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5867,7 +5889,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210985024"/>
+        <c:crossAx val="292581272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5875,7 +5897,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="210985024"/>
+        <c:axId val="292581272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5921,7 +5943,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5955,7 +5976,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="210984632"/>
+        <c:crossAx val="292584800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5969,7 +5990,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6270,8 +6290,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="210985416"/>
-        <c:axId val="210984240"/>
+        <c:axId val="292586760"/>
+        <c:axId val="292582448"/>
         <c:axId val="0"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -6441,7 +6461,7 @@
         </c:extLst>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="210985416"/>
+        <c:axId val="292586760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6539,7 +6559,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210984240"/>
+        <c:crossAx val="292582448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6547,7 +6567,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="210984240"/>
+        <c:axId val="292582448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6626,7 +6646,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="210985416"/>
+        <c:crossAx val="292586760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10537,7 +10557,7 @@
       </c>
       <c r="G3" s="48"/>
       <c r="H3" s="91"/>
-      <c r="I3" s="136" t="s">
+      <c r="I3" s="135" t="s">
         <v>329</v>
       </c>
       <c r="J3" s="85" t="s">
@@ -10604,10 +10624,10 @@
       <c r="K5" s="91"/>
     </row>
     <row r="6" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="153" t="s">
+      <c r="A6" s="152" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="139" t="s">
+      <c r="B6" s="138" t="s">
         <v>33</v>
       </c>
       <c r="C6" s="18" t="s">
@@ -10660,7 +10680,7 @@
       <c r="K7" s="91"/>
     </row>
     <row r="8" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="153" t="s">
+      <c r="A8" s="152" t="s">
         <v>39</v>
       </c>
       <c r="B8" s="129" t="s">
@@ -10693,7 +10713,7 @@
       <c r="B9" s="129" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="139" t="s">
+      <c r="C9" s="138" t="s">
         <v>124</v>
       </c>
       <c r="D9" s="94">
@@ -10936,7 +10956,7 @@
       <c r="K17" s="91"/>
     </row>
     <row r="18" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="153" t="s">
+      <c r="A18" s="152" t="s">
         <v>49</v>
       </c>
       <c r="B18" s="129" t="s">
@@ -11012,7 +11032,7 @@
       </c>
       <c r="G20" s="48"/>
       <c r="H20" s="91"/>
-      <c r="I20" s="136" t="s">
+      <c r="I20" s="135" t="s">
         <v>329</v>
       </c>
       <c r="J20" s="85" t="s">
@@ -11029,7 +11049,7 @@
       <c r="B21" s="130" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="139" t="s">
+      <c r="C21" s="138" t="s">
         <v>85</v>
       </c>
       <c r="D21" s="94">
@@ -11101,7 +11121,7 @@
       </c>
       <c r="G23" s="48"/>
       <c r="H23" s="91"/>
-      <c r="I23" s="136" t="s">
+      <c r="I23" s="135" t="s">
         <v>329</v>
       </c>
       <c r="J23" s="85" t="s">
@@ -11141,23 +11161,23 @@
       <c r="K24" s="91"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E25" s="161" t="s">
+      <c r="E25" s="160" t="s">
         <v>81</v>
       </c>
-      <c r="F25" s="162">
+      <c r="F25" s="161">
         <f>SUM(F3:F24)</f>
         <v>464</v>
       </c>
-      <c r="G25" s="163">
+      <c r="G25" s="162">
         <f>SUM(G3:G24)</f>
         <v>13</v>
       </c>
-      <c r="H25" s="161">
+      <c r="H25" s="160">
         <f>SUM(H3:H24)</f>
         <v>4</v>
       </c>
-      <c r="I25" s="163"/>
-      <c r="J25" s="138"/>
+      <c r="I25" s="162"/>
+      <c r="J25" s="137"/>
     </row>
     <row r="28" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
@@ -11210,7 +11230,7 @@
       <c r="A2" s="79" t="s">
         <v>248</v>
       </c>
-      <c r="B2" s="142" t="s">
+      <c r="B2" s="141" t="s">
         <v>330</v>
       </c>
     </row>
@@ -11234,7 +11254,7 @@
       <c r="A5" s="79" t="s">
         <v>332</v>
       </c>
-      <c r="B5" s="141" t="s">
+      <c r="B5" s="140" t="s">
         <v>275</v>
       </c>
     </row>
@@ -11254,7 +11274,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
@@ -11288,40 +11308,40 @@
       <c r="L1" s="228"/>
     </row>
     <row r="2" spans="1:12" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="143" t="s">
+      <c r="A2" s="142" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="143" t="s">
+      <c r="B2" s="142" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="144" t="s">
+      <c r="C2" s="143" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="143" t="s">
+      <c r="D2" s="142" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="143" t="s">
+      <c r="E2" s="142" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="143" t="s">
+      <c r="F2" s="142" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="143" t="s">
+      <c r="G2" s="142" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="143" t="s">
+      <c r="H2" s="142" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="143" t="s">
+      <c r="I2" s="142" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="143" t="s">
+      <c r="J2" s="142" t="s">
         <v>35</v>
       </c>
-      <c r="K2" s="143" t="s">
+      <c r="K2" s="142" t="s">
         <v>36</v>
       </c>
-      <c r="L2" s="143" t="s">
+      <c r="L2" s="142" t="s">
         <v>37</v>
       </c>
     </row>
@@ -11329,17 +11349,17 @@
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="135" t="s">
+      <c r="B3" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="135" t="s">
+      <c r="C3" s="134" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="135" t="s">
+      <c r="H3" s="134" t="s">
         <v>18</v>
       </c>
       <c r="I3" s="128" t="s">
@@ -11631,19 +11651,19 @@
       <c r="A13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="135" t="s">
+      <c r="B13" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="135" t="s">
+      <c r="C13" s="134" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="135" t="s">
+      <c r="G13" s="134" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="135" t="s">
+      <c r="H13" s="134" t="s">
         <v>18</v>
       </c>
       <c r="I13" s="129" t="s">
@@ -11853,17 +11873,17 @@
       <c r="A20" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="135" t="s">
+      <c r="B20" s="134" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="135" t="s">
+      <c r="F20" s="134" t="s">
         <v>19</v>
       </c>
       <c r="G20" s="2"/>
-      <c r="H20" s="135" t="s">
+      <c r="H20" s="134" t="s">
         <v>18</v>
       </c>
       <c r="I20" s="130" t="s">
@@ -11913,17 +11933,17 @@
       <c r="A22" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="135" t="s">
+      <c r="B22" s="134" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="135" t="s">
+      <c r="F22" s="134" t="s">
         <v>19</v>
       </c>
       <c r="G22" s="2"/>
-      <c r="H22" s="135" t="s">
+      <c r="H22" s="134" t="s">
         <v>18</v>
       </c>
       <c r="I22" s="130" t="s">
@@ -11943,17 +11963,17 @@
       <c r="A23" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="135" t="s">
+      <c r="B23" s="134" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="135" t="s">
+      <c r="F23" s="134" t="s">
         <v>19</v>
       </c>
       <c r="G23" s="2"/>
-      <c r="H23" s="135" t="s">
+      <c r="H23" s="134" t="s">
         <v>18</v>
       </c>
       <c r="I23" s="130" t="s">
@@ -12003,7 +12023,7 @@
       <c r="L25" s="92"/>
     </row>
     <row r="26" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="135"/>
+      <c r="A26" s="134"/>
       <c r="B26" s="229" t="s">
         <v>334</v>
       </c>
@@ -12045,7 +12065,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="90" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="164" t="s">
+      <c r="A1" s="163" t="s">
         <v>349</v>
       </c>
     </row>
@@ -12078,84 +12098,84 @@
       <c r="A7" s="18" t="s">
         <v>343</v>
       </c>
-      <c r="B7" s="140"/>
-      <c r="C7" s="140"/>
-      <c r="D7" s="140"/>
-      <c r="E7" s="140"/>
-      <c r="F7" s="140"/>
-      <c r="G7" s="140"/>
+      <c r="B7" s="139"/>
+      <c r="C7" s="139"/>
+      <c r="D7" s="139"/>
+      <c r="E7" s="139"/>
+      <c r="F7" s="139"/>
+      <c r="G7" s="139"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="148"/>
-      <c r="B8" s="148"/>
-      <c r="C8" s="148"/>
-      <c r="D8" s="148"/>
-      <c r="E8" s="148"/>
-      <c r="F8" s="148"/>
-      <c r="G8" s="148"/>
+      <c r="A8" s="147"/>
+      <c r="B8" s="147"/>
+      <c r="C8" s="147"/>
+      <c r="D8" s="147"/>
+      <c r="E8" s="147"/>
+      <c r="F8" s="147"/>
+      <c r="G8" s="147"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="148"/>
-      <c r="B9" s="148"/>
-      <c r="C9" s="148"/>
-      <c r="D9" s="148"/>
-      <c r="E9" s="148"/>
-      <c r="F9" s="148"/>
-      <c r="G9" s="148"/>
+      <c r="A9" s="147"/>
+      <c r="B9" s="147"/>
+      <c r="C9" s="147"/>
+      <c r="D9" s="147"/>
+      <c r="E9" s="147"/>
+      <c r="F9" s="147"/>
+      <c r="G9" s="147"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="148"/>
-      <c r="B10" s="148"/>
-      <c r="C10" s="148"/>
-      <c r="D10" s="148"/>
-      <c r="E10" s="148"/>
-      <c r="F10" s="148"/>
-      <c r="G10" s="148"/>
+      <c r="A10" s="147"/>
+      <c r="B10" s="147"/>
+      <c r="C10" s="147"/>
+      <c r="D10" s="147"/>
+      <c r="E10" s="147"/>
+      <c r="F10" s="147"/>
+      <c r="G10" s="147"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="148"/>
-      <c r="B11" s="148"/>
-      <c r="C11" s="148"/>
-      <c r="D11" s="148"/>
-      <c r="E11" s="148"/>
-      <c r="F11" s="148"/>
-      <c r="G11" s="148"/>
+      <c r="A11" s="147"/>
+      <c r="B11" s="147"/>
+      <c r="C11" s="147"/>
+      <c r="D11" s="147"/>
+      <c r="E11" s="147"/>
+      <c r="F11" s="147"/>
+      <c r="G11" s="147"/>
     </row>
     <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="148"/>
-      <c r="B12" s="148"/>
-      <c r="C12" s="148"/>
-      <c r="D12" s="148"/>
-      <c r="E12" s="148"/>
-      <c r="F12" s="148"/>
-      <c r="G12" s="148"/>
+      <c r="A12" s="147"/>
+      <c r="B12" s="147"/>
+      <c r="C12" s="147"/>
+      <c r="D12" s="147"/>
+      <c r="E12" s="147"/>
+      <c r="F12" s="147"/>
+      <c r="G12" s="147"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="148"/>
-      <c r="B13" s="148"/>
-      <c r="C13" s="148"/>
-      <c r="D13" s="148"/>
-      <c r="E13" s="148"/>
-      <c r="F13" s="148"/>
-      <c r="G13" s="148"/>
+      <c r="A13" s="147"/>
+      <c r="B13" s="147"/>
+      <c r="C13" s="147"/>
+      <c r="D13" s="147"/>
+      <c r="E13" s="147"/>
+      <c r="F13" s="147"/>
+      <c r="G13" s="147"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="148"/>
-      <c r="B14" s="148"/>
-      <c r="C14" s="148"/>
-      <c r="D14" s="148"/>
-      <c r="E14" s="148"/>
-      <c r="F14" s="148"/>
-      <c r="G14" s="148"/>
+      <c r="A14" s="147"/>
+      <c r="B14" s="147"/>
+      <c r="C14" s="147"/>
+      <c r="D14" s="147"/>
+      <c r="E14" s="147"/>
+      <c r="F14" s="147"/>
+      <c r="G14" s="147"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="148"/>
-      <c r="B15" s="148"/>
-      <c r="C15" s="148"/>
-      <c r="D15" s="148"/>
-      <c r="E15" s="148"/>
-      <c r="F15" s="148"/>
-      <c r="G15" s="148"/>
+      <c r="A15" s="147"/>
+      <c r="B15" s="147"/>
+      <c r="C15" s="147"/>
+      <c r="D15" s="147"/>
+      <c r="E15" s="147"/>
+      <c r="F15" s="147"/>
+      <c r="G15" s="147"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -12168,7 +12188,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12192,18 +12212,18 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" s="150" t="s">
+      <c r="A3" s="149" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="149" t="s">
+      <c r="B3" s="148" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="151" t="s">
+      <c r="A4" s="150" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="152"/>
+      <c r="B4" s="151"/>
     </row>
     <row r="5" spans="1:2" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
@@ -12287,7 +12307,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -12667,22 +12687,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="81" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="67.5703125" customWidth="1"/>
+    <col min="2" max="2" width="77.5703125" customWidth="1"/>
     <col min="3" max="3" width="57.140625" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" style="3" customWidth="1"/>
     <col min="5" max="5" width="41.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="195" t="s">
         <v>126</v>
       </c>
@@ -12690,8 +12711,9 @@
       <c r="C1" s="195"/>
       <c r="D1" s="195"/>
       <c r="E1" s="195"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="195"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>123</v>
       </c>
@@ -12707,9 +12729,12 @@
       <c r="E2" s="21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="133" t="s">
+      <c r="F2" s="21" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="132" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="131" t="s">
@@ -12718,15 +12743,18 @@
       <c r="C3" s="131" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="133" t="s">
+      <c r="D3" s="132" t="s">
         <v>25</v>
       </c>
       <c r="E3" s="19" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="133" t="s">
+      <c r="F3" s="91" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="132" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="131" t="s">
@@ -12735,15 +12763,18 @@
       <c r="C4" s="131" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="133">
+      <c r="D4" s="132">
         <v>2007</v>
       </c>
       <c r="E4" s="19" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="133" t="s">
+      <c r="F4" s="91" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="132" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="131" t="s">
@@ -12752,15 +12783,18 @@
       <c r="C5" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="133">
+      <c r="D5" s="132">
         <v>2008</v>
       </c>
       <c r="E5" s="19" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="133" t="s">
+      <c r="F5" s="91" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="132" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -12769,15 +12803,16 @@
       <c r="C6" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="133">
+      <c r="D6" s="132">
         <v>2015</v>
       </c>
       <c r="E6" s="19" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="133" t="s">
+      <c r="F6" s="91"/>
+    </row>
+    <row r="7" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="132" t="s">
         <v>38</v>
       </c>
       <c r="B7" s="131" t="s">
@@ -12786,15 +12821,16 @@
       <c r="C7" s="131" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="133">
+      <c r="D7" s="132">
         <v>2011</v>
       </c>
       <c r="E7" s="19" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="133" t="s">
+      <c r="F7" s="91"/>
+    </row>
+    <row r="8" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="132" t="s">
         <v>39</v>
       </c>
       <c r="B8" s="131" t="s">
@@ -12803,15 +12839,16 @@
       <c r="C8" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="133">
+      <c r="D8" s="132">
         <v>2010</v>
       </c>
       <c r="E8" s="19" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="133" t="s">
+      <c r="F8" s="91"/>
+    </row>
+    <row r="9" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="132" t="s">
         <v>40</v>
       </c>
       <c r="B9" s="131" t="s">
@@ -12820,32 +12857,34 @@
       <c r="C9" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="D9" s="133">
+      <c r="D9" s="132">
         <v>2009</v>
       </c>
       <c r="E9" s="19" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="133" t="s">
+      <c r="F9" s="91"/>
+    </row>
+    <row r="10" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="132" t="s">
         <v>41</v>
       </c>
       <c r="B10" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="132" t="s">
+      <c r="C10" s="131" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="133">
+      <c r="D10" s="132">
         <v>2010</v>
       </c>
       <c r="E10" s="19" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="133" t="s">
+      <c r="F10" s="91"/>
+    </row>
+    <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="132" t="s">
         <v>42</v>
       </c>
       <c r="B11" s="131" t="s">
@@ -12854,15 +12893,16 @@
       <c r="C11" s="131" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="133">
+      <c r="D11" s="132">
         <v>2010</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="133" t="s">
+      <c r="F11" s="91"/>
+    </row>
+    <row r="12" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="132" t="s">
         <v>43</v>
       </c>
       <c r="B12" s="131" t="s">
@@ -12871,15 +12911,16 @@
       <c r="C12" s="131" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="133">
+      <c r="D12" s="132">
         <v>1999</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="133" t="s">
+      <c r="F12" s="91"/>
+    </row>
+    <row r="13" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="132" t="s">
         <v>44</v>
       </c>
       <c r="B13" s="131" t="s">
@@ -12888,15 +12929,16 @@
       <c r="C13" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="133">
+      <c r="D13" s="132">
         <v>2005</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="133" t="s">
+      <c r="F13" s="91"/>
+    </row>
+    <row r="14" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="132" t="s">
         <v>45</v>
       </c>
       <c r="B14" s="131" t="s">
@@ -12905,15 +12947,16 @@
       <c r="C14" s="131" t="s">
         <v>71</v>
       </c>
-      <c r="D14" s="133">
+      <c r="D14" s="132">
         <v>2008</v>
       </c>
       <c r="E14" s="20" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="133" t="s">
+      <c r="F14" s="91"/>
+    </row>
+    <row r="15" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="132" t="s">
         <v>46</v>
       </c>
       <c r="B15" s="131" t="s">
@@ -12922,15 +12965,16 @@
       <c r="C15" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="133">
+      <c r="D15" s="132">
         <v>2011</v>
       </c>
       <c r="E15" s="19" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="133" t="s">
+      <c r="F15" s="91"/>
+    </row>
+    <row r="16" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="132" t="s">
         <v>47</v>
       </c>
       <c r="B16" s="131" t="s">
@@ -12939,15 +12983,16 @@
       <c r="C16" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="D16" s="133">
+      <c r="D16" s="132">
         <v>2009</v>
       </c>
       <c r="E16" s="19" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="133" t="s">
+      <c r="F16" s="91"/>
+    </row>
+    <row r="17" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="132" t="s">
         <v>48</v>
       </c>
       <c r="B17" s="131" t="s">
@@ -12956,15 +13001,16 @@
       <c r="C17" s="131" t="s">
         <v>61</v>
       </c>
-      <c r="D17" s="133">
+      <c r="D17" s="132">
         <v>1997</v>
       </c>
       <c r="E17" s="19" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="133" t="s">
+      <c r="F17" s="91"/>
+    </row>
+    <row r="18" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="132" t="s">
         <v>49</v>
       </c>
       <c r="B18" s="131" t="s">
@@ -12973,15 +13019,16 @@
       <c r="C18" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="133">
+      <c r="D18" s="132">
         <v>2010</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="133" t="s">
+      <c r="F18" s="91"/>
+    </row>
+    <row r="19" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="132" t="s">
         <v>50</v>
       </c>
       <c r="B19" s="20" t="s">
@@ -12990,15 +13037,16 @@
       <c r="C19" s="131" t="s">
         <v>80</v>
       </c>
-      <c r="D19" s="133">
+      <c r="D19" s="132">
         <v>2005</v>
       </c>
       <c r="E19" s="19" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="133" t="s">
+      <c r="F19" s="91"/>
+    </row>
+    <row r="20" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="132" t="s">
         <v>51</v>
       </c>
       <c r="B20" s="20" t="s">
@@ -13007,15 +13055,16 @@
       <c r="C20" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="D20" s="133">
+      <c r="D20" s="132">
         <v>2011</v>
       </c>
       <c r="E20" s="19" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="133" t="s">
+      <c r="F20" s="91"/>
+    </row>
+    <row r="21" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="132" t="s">
         <v>52</v>
       </c>
       <c r="B21" s="20" t="s">
@@ -13024,15 +13073,16 @@
       <c r="C21" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="D21" s="133">
+      <c r="D21" s="132">
         <v>2008</v>
       </c>
       <c r="E21" s="19" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="133" t="s">
+      <c r="F21" s="91"/>
+    </row>
+    <row r="22" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="132" t="s">
         <v>53</v>
       </c>
       <c r="B22" s="20" t="s">
@@ -13041,15 +13091,16 @@
       <c r="C22" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="D22" s="133">
+      <c r="D22" s="132">
         <v>2015</v>
       </c>
       <c r="E22" s="19" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="133" t="s">
+      <c r="F22" s="91"/>
+    </row>
+    <row r="23" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="132" t="s">
         <v>54</v>
       </c>
       <c r="B23" s="20" t="s">
@@ -13058,15 +13109,16 @@
       <c r="C23" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="D23" s="133">
+      <c r="D23" s="132">
         <v>2000</v>
       </c>
       <c r="E23" s="19" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="133" t="s">
+      <c r="F23" s="91"/>
+    </row>
+    <row r="24" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="132" t="s">
         <v>55</v>
       </c>
       <c r="B24" s="20" t="s">
@@ -13075,27 +13127,28 @@
       <c r="C24" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="D24" s="133">
+      <c r="D24" s="132">
         <v>2010</v>
       </c>
       <c r="E24" s="19" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="145" t="s">
+      <c r="F24" s="91"/>
+    </row>
+    <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="144" t="s">
         <v>125</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="134"/>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="133"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -13105,8 +13158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S54"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13283,19 +13336,19 @@
       <c r="D12" s="210"/>
     </row>
     <row r="13" spans="1:19" s="77" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="146" t="s">
+      <c r="A13" s="145" t="s">
         <v>274</v>
       </c>
-      <c r="B13" s="137" t="s">
+      <c r="B13" s="136" t="s">
         <v>272</v>
       </c>
-      <c r="C13" s="137" t="s">
+      <c r="C13" s="136" t="s">
         <v>273</v>
       </c>
       <c r="D13" s="211"/>
     </row>
     <row r="14" spans="1:19" s="77" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="147" t="s">
+      <c r="A14" s="146" t="s">
         <v>340</v>
       </c>
       <c r="B14" s="94" t="s">
@@ -13393,7 +13446,7 @@
       <c r="F19" s="72">
         <v>0.77</v>
       </c>
-      <c r="G19" s="232">
+      <c r="G19" s="179">
         <f>HARMEAN(E19,F19)</f>
         <v>3.326556543837357E-2</v>
       </c>
@@ -13417,7 +13470,7 @@
       <c r="F20" s="72">
         <v>0.41</v>
       </c>
-      <c r="G20" s="232">
+      <c r="G20" s="179">
         <f t="shared" ref="G20:G24" si="0">HARMEAN(E20,F20)</f>
         <v>4.3556581986143185E-2</v>
       </c>
@@ -13441,7 +13494,7 @@
       <c r="F21" s="72">
         <v>0.59</v>
       </c>
-      <c r="G21" s="232">
+      <c r="G21" s="179">
         <f t="shared" si="0"/>
         <v>5.5282714054927309E-2</v>
       </c>
@@ -13465,7 +13518,7 @@
       <c r="F22" s="72">
         <v>0.5</v>
       </c>
-      <c r="G22" s="232">
+      <c r="G22" s="179">
         <f t="shared" si="0"/>
         <v>8.2568807339449546E-2</v>
       </c>
@@ -13489,7 +13542,7 @@
       <c r="F23" s="72">
         <v>0.59</v>
       </c>
-      <c r="G23" s="232">
+      <c r="G23" s="179">
         <f t="shared" si="0"/>
         <v>6.608E-2</v>
       </c>
@@ -13513,7 +13566,7 @@
       <c r="F24" s="72">
         <v>0.54</v>
       </c>
-      <c r="G24" s="232">
+      <c r="G24" s="179">
         <f t="shared" si="0"/>
         <v>6.9254766031195833E-2</v>
       </c>
@@ -13789,11 +13842,11 @@
       <c r="C48" s="126">
         <v>0.59</v>
       </c>
-      <c r="D48" s="176">
+      <c r="D48" s="175">
         <f>2*((B48*C48)/(B48+C48))</f>
         <v>5.3827240375283081E-2</v>
       </c>
-      <c r="E48" s="232">
+      <c r="E48" s="179">
         <f>HARMEAN(B48,C48)</f>
         <v>5.3827240375283081E-2</v>
       </c>
@@ -13805,14 +13858,14 @@
       <c r="B49" s="126">
         <v>1.67E-2</v>
       </c>
-      <c r="C49" s="175">
+      <c r="C49" s="174">
         <v>0.77270000000000005</v>
       </c>
-      <c r="D49" s="176">
+      <c r="D49" s="175">
         <f t="shared" ref="D49:D54" si="1">2*((B49*C49)/(B49+C49))</f>
         <v>3.2693412718520394E-2</v>
       </c>
-      <c r="E49" s="232">
+      <c r="E49" s="179">
         <f t="shared" ref="E49:E54" si="2">HARMEAN(B49,C49)</f>
         <v>3.2693412718520394E-2</v>
       </c>
@@ -13827,11 +13880,11 @@
       <c r="C50" s="126">
         <v>0.40899999999999997</v>
       </c>
-      <c r="D50" s="176">
+      <c r="D50" s="175">
         <f t="shared" si="1"/>
         <v>4.3730155056699832E-2</v>
       </c>
-      <c r="E50" s="232">
+      <c r="E50" s="179">
         <f t="shared" si="2"/>
         <v>4.3730155056699839E-2</v>
       </c>
@@ -13846,11 +13899,11 @@
       <c r="C51" s="126">
         <v>0.59</v>
       </c>
-      <c r="D51" s="176">
+      <c r="D51" s="175">
         <f t="shared" si="1"/>
         <v>5.5827547230744394E-2</v>
       </c>
-      <c r="E51" s="232">
+      <c r="E51" s="179">
         <f t="shared" si="2"/>
         <v>5.5827547230744394E-2</v>
       </c>
@@ -13865,11 +13918,11 @@
       <c r="C52" s="126">
         <v>0.5</v>
       </c>
-      <c r="D52" s="176">
+      <c r="D52" s="175">
         <f>2*((B52*C52)/(B52+C52))</f>
         <v>8.2063521204332662E-2</v>
       </c>
-      <c r="E52" s="232">
+      <c r="E52" s="179">
         <f t="shared" si="2"/>
         <v>8.2063521204332662E-2</v>
       </c>
@@ -13884,11 +13937,11 @@
       <c r="C53" s="126">
         <v>0.59</v>
       </c>
-      <c r="D53" s="176">
+      <c r="D53" s="175">
         <f t="shared" si="1"/>
         <v>6.6258198688209882E-2</v>
       </c>
-      <c r="E53" s="232">
+      <c r="E53" s="179">
         <f t="shared" si="2"/>
         <v>6.6258198688209896E-2</v>
       </c>
@@ -13903,11 +13956,11 @@
       <c r="C54" s="126">
         <v>0.54</v>
       </c>
-      <c r="D54" s="176">
+      <c r="D54" s="175">
         <f t="shared" si="1"/>
         <v>6.9254766031195833E-2</v>
       </c>
-      <c r="E54" s="232">
+      <c r="E54" s="179">
         <f t="shared" si="2"/>
         <v>6.9254766031195833E-2</v>
       </c>
@@ -13945,7 +13998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V48"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -13976,25 +14029,25 @@
       <c r="G1" s="217"/>
     </row>
     <row r="2" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="159" t="s">
+      <c r="A2" s="158" t="s">
         <v>177</v>
       </c>
-      <c r="B2" s="159" t="s">
+      <c r="B2" s="158" t="s">
         <v>178</v>
       </c>
-      <c r="C2" s="160" t="s">
+      <c r="C2" s="159" t="s">
         <v>179</v>
       </c>
-      <c r="D2" s="160" t="s">
+      <c r="D2" s="159" t="s">
         <v>180</v>
       </c>
-      <c r="E2" s="159" t="s">
+      <c r="E2" s="158" t="s">
         <v>208</v>
       </c>
-      <c r="F2" s="159" t="s">
+      <c r="F2" s="158" t="s">
         <v>224</v>
       </c>
-      <c r="G2" s="159" t="s">
+      <c r="G2" s="158" t="s">
         <v>344</v>
       </c>
       <c r="I2" s="216" t="s">
@@ -14027,7 +14080,7 @@
       <c r="A4" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="154" t="s">
+      <c r="B4" s="153" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="49"/>
@@ -14035,10 +14088,10 @@
       <c r="E4" s="49">
         <v>20</v>
       </c>
-      <c r="F4" s="158" t="s">
+      <c r="F4" s="157" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="154" t="s">
+      <c r="G4" s="153" t="s">
         <v>209</v>
       </c>
       <c r="I4" s="52" t="s">
@@ -14053,7 +14106,7 @@
       <c r="A5" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="154" t="s">
+      <c r="B5" s="153" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="49"/>
@@ -14061,10 +14114,10 @@
       <c r="E5" s="49">
         <v>24</v>
       </c>
-      <c r="F5" s="158" t="s">
+      <c r="F5" s="157" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="158" t="s">
+      <c r="G5" s="157" t="s">
         <v>210</v>
       </c>
       <c r="I5" s="59" t="s">
@@ -14101,7 +14154,7 @@
       <c r="A7" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="154" t="s">
+      <c r="B7" s="153" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="49"/>
@@ -14109,10 +14162,10 @@
       <c r="E7" s="49">
         <v>11</v>
       </c>
-      <c r="F7" s="158" t="s">
+      <c r="F7" s="157" t="s">
         <v>56</v>
       </c>
-      <c r="G7" s="154" t="s">
+      <c r="G7" s="153" t="s">
         <v>211</v>
       </c>
       <c r="I7" s="58" t="s">
@@ -14165,7 +14218,7 @@
       <c r="A10" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="154" t="s">
+      <c r="B10" s="153" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="49"/>
@@ -14173,10 +14226,10 @@
       <c r="E10" s="70">
         <v>44</v>
       </c>
-      <c r="F10" s="158" t="s">
+      <c r="F10" s="157" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="154" t="s">
+      <c r="G10" s="153" t="s">
         <v>212</v>
       </c>
       <c r="I10" s="55" t="s">
@@ -14261,7 +14314,7 @@
       <c r="A14" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="154" t="s">
+      <c r="B14" s="153" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="49"/>
@@ -14269,10 +14322,10 @@
       <c r="E14" s="49">
         <v>14</v>
       </c>
-      <c r="F14" s="158" t="s">
+      <c r="F14" s="157" t="s">
         <v>70</v>
       </c>
-      <c r="G14" s="154" t="s">
+      <c r="G14" s="153" t="s">
         <v>213</v>
       </c>
       <c r="I14" s="104" t="s">
@@ -14289,7 +14342,7 @@
       <c r="A15" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="154" t="s">
+      <c r="B15" s="153" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="49"/>
@@ -14297,10 +14350,10 @@
       <c r="E15" s="49">
         <v>8</v>
       </c>
-      <c r="F15" s="158" t="s">
+      <c r="F15" s="157" t="s">
         <v>72</v>
       </c>
-      <c r="G15" s="154" t="s">
+      <c r="G15" s="153" t="s">
         <v>214</v>
       </c>
       <c r="I15" s="104" t="s">
@@ -14317,7 +14370,7 @@
       <c r="A16" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="154" t="s">
+      <c r="B16" s="153" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="49"/>
@@ -14325,10 +14378,10 @@
       <c r="E16" s="49">
         <v>27</v>
       </c>
-      <c r="F16" s="158" t="s">
+      <c r="F16" s="157" t="s">
         <v>74</v>
       </c>
-      <c r="G16" s="154" t="s">
+      <c r="G16" s="153" t="s">
         <v>215</v>
       </c>
       <c r="I16" s="119" t="s">
@@ -14345,7 +14398,7 @@
       <c r="A17" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="154" t="s">
+      <c r="B17" s="153" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="49"/>
@@ -14353,10 +14406,10 @@
       <c r="E17" s="49">
         <v>14</v>
       </c>
-      <c r="F17" s="158" t="s">
+      <c r="F17" s="157" t="s">
         <v>76</v>
       </c>
-      <c r="G17" s="154" t="s">
+      <c r="G17" s="153" t="s">
         <v>216</v>
       </c>
     </row>
@@ -14514,7 +14567,7 @@
       <c r="B25" s="49"/>
       <c r="C25" s="49"/>
       <c r="D25" s="49"/>
-      <c r="E25" s="154">
+      <c r="E25" s="153">
         <f>SUM(E3:E24)</f>
         <v>162</v>
       </c>
@@ -14532,7 +14585,7 @@
       <c r="B26" s="91"/>
       <c r="C26" s="91"/>
       <c r="D26" s="91"/>
-      <c r="E26" s="158" t="s">
+      <c r="E26" s="157" t="s">
         <v>314</v>
       </c>
       <c r="F26" s="114"/>
@@ -14559,12 +14612,12 @@
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A28" s="155" t="s">
+      <c r="A28" s="154" t="s">
         <v>312</v>
       </c>
-      <c r="B28" s="156"/>
-      <c r="C28" s="156"/>
-      <c r="D28" s="157"/>
+      <c r="B28" s="155"/>
+      <c r="C28" s="155"/>
+      <c r="D28" s="156"/>
       <c r="I28" s="110" t="s">
         <v>294</v>
       </c>
@@ -14772,7 +14825,7 @@
   <dimension ref="A1:V48"/>
   <sheetViews>
     <sheetView topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14808,25 +14861,25 @@
       <c r="G1" s="217"/>
     </row>
     <row r="2" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="159" t="s">
+      <c r="A2" s="158" t="s">
         <v>177</v>
       </c>
-      <c r="B2" s="159" t="s">
+      <c r="B2" s="158" t="s">
         <v>178</v>
       </c>
-      <c r="C2" s="160" t="s">
+      <c r="C2" s="159" t="s">
         <v>179</v>
       </c>
-      <c r="D2" s="160" t="s">
+      <c r="D2" s="159" t="s">
         <v>180</v>
       </c>
-      <c r="E2" s="159" t="s">
+      <c r="E2" s="158" t="s">
         <v>208</v>
       </c>
-      <c r="F2" s="159" t="s">
+      <c r="F2" s="158" t="s">
         <v>224</v>
       </c>
-      <c r="G2" s="159" t="s">
+      <c r="G2" s="158" t="s">
         <v>344</v>
       </c>
       <c r="I2" s="216" t="s">
@@ -14834,16 +14887,16 @@
       </c>
       <c r="J2" s="216"/>
       <c r="K2" s="216"/>
-      <c r="O2" s="171" t="s">
+      <c r="O2" s="170" t="s">
         <v>351</v>
       </c>
-      <c r="P2" s="172" t="s">
+      <c r="P2" s="171" t="s">
         <v>465</v>
       </c>
-      <c r="Q2" s="172" t="s">
+      <c r="Q2" s="171" t="s">
         <v>352</v>
       </c>
-      <c r="R2" s="173" t="s">
+      <c r="R2" s="172" t="s">
         <v>353</v>
       </c>
     </row>
@@ -14866,7 +14919,7 @@
         <v>22</v>
       </c>
       <c r="K3" s="61"/>
-      <c r="O3" s="166" t="s">
+      <c r="O3" s="165" t="s">
         <v>244</v>
       </c>
       <c r="P3" s="91" t="s">
@@ -14875,7 +14928,7 @@
       <c r="Q3" s="91" t="s">
         <v>356</v>
       </c>
-      <c r="R3" s="167" t="s">
+      <c r="R3" s="166" t="s">
         <v>356</v>
       </c>
     </row>
@@ -14883,7 +14936,7 @@
       <c r="A4" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="154" t="s">
+      <c r="B4" s="153" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="94"/>
@@ -14891,10 +14944,10 @@
       <c r="E4" s="94">
         <v>20</v>
       </c>
-      <c r="F4" s="158" t="s">
+      <c r="F4" s="157" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="154" t="s">
+      <c r="G4" s="153" t="s">
         <v>209</v>
       </c>
       <c r="I4" s="95" t="s">
@@ -14904,20 +14957,20 @@
         <v>17</v>
       </c>
       <c r="K4" s="48"/>
-      <c r="O4" s="166" t="s">
+      <c r="O4" s="165" t="s">
         <v>245</v>
       </c>
       <c r="P4" s="91" t="s">
         <v>354</v>
       </c>
       <c r="Q4" s="91"/>
-      <c r="R4" s="167"/>
+      <c r="R4" s="166"/>
     </row>
     <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="154" t="s">
+      <c r="B5" s="153" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="94"/>
@@ -14925,10 +14978,10 @@
       <c r="E5" s="94">
         <v>24</v>
       </c>
-      <c r="F5" s="158" t="s">
+      <c r="F5" s="157" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="158" t="s">
+      <c r="G5" s="157" t="s">
         <v>210</v>
       </c>
       <c r="I5" s="59" t="s">
@@ -14938,14 +14991,14 @@
         <v>8</v>
       </c>
       <c r="K5" s="48"/>
-      <c r="O5" s="166" t="s">
+      <c r="O5" s="165" t="s">
         <v>246</v>
       </c>
       <c r="P5" s="91" t="s">
         <v>354</v>
       </c>
       <c r="Q5" s="91"/>
-      <c r="R5" s="167"/>
+      <c r="R5" s="166"/>
     </row>
     <row r="6" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="36" t="s">
@@ -14968,20 +15021,20 @@
         <v>14</v>
       </c>
       <c r="K6" s="48"/>
-      <c r="O6" s="168" t="s">
+      <c r="O6" s="167" t="s">
         <v>247</v>
       </c>
-      <c r="P6" s="169" t="s">
+      <c r="P6" s="168" t="s">
         <v>354</v>
       </c>
-      <c r="Q6" s="169"/>
-      <c r="R6" s="170"/>
+      <c r="Q6" s="168"/>
+      <c r="R6" s="169"/>
     </row>
     <row r="7" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="154" t="s">
+      <c r="B7" s="153" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="94"/>
@@ -14989,10 +15042,10 @@
       <c r="E7" s="94">
         <v>11</v>
       </c>
-      <c r="F7" s="158" t="s">
+      <c r="F7" s="157" t="s">
         <v>56</v>
       </c>
-      <c r="G7" s="154" t="s">
+      <c r="G7" s="153" t="s">
         <v>211</v>
       </c>
       <c r="I7" s="58" t="s">
@@ -15045,7 +15098,7 @@
       <c r="A10" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="154" t="s">
+      <c r="B10" s="153" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="94"/>
@@ -15053,10 +15106,10 @@
       <c r="E10" s="70">
         <v>44</v>
       </c>
-      <c r="F10" s="158" t="s">
+      <c r="F10" s="157" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="154" t="s">
+      <c r="G10" s="153" t="s">
         <v>212</v>
       </c>
       <c r="I10" s="55" t="s">
@@ -15111,7 +15164,7 @@
       <c r="J12" s="62" t="s">
         <v>300</v>
       </c>
-      <c r="K12" s="165" t="s">
+      <c r="K12" s="164" t="s">
         <v>220</v>
       </c>
     </row>
@@ -15133,7 +15186,7 @@
       <c r="J13" s="62" t="s">
         <v>218</v>
       </c>
-      <c r="K13" s="165" t="s">
+      <c r="K13" s="164" t="s">
         <v>204</v>
       </c>
     </row>
@@ -15141,7 +15194,7 @@
       <c r="A14" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="154" t="s">
+      <c r="B14" s="153" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="94"/>
@@ -15149,10 +15202,10 @@
       <c r="E14" s="94">
         <v>14</v>
       </c>
-      <c r="F14" s="158" t="s">
+      <c r="F14" s="157" t="s">
         <v>70</v>
       </c>
-      <c r="G14" s="154" t="s">
+      <c r="G14" s="153" t="s">
         <v>213</v>
       </c>
       <c r="I14" s="104" t="s">
@@ -15161,7 +15214,7 @@
       <c r="J14" s="98" t="s">
         <v>299</v>
       </c>
-      <c r="K14" s="165" t="s">
+      <c r="K14" s="164" t="s">
         <v>221</v>
       </c>
     </row>
@@ -15169,7 +15222,7 @@
       <c r="A15" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="154" t="s">
+      <c r="B15" s="153" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="94"/>
@@ -15177,10 +15230,10 @@
       <c r="E15" s="94">
         <v>8</v>
       </c>
-      <c r="F15" s="158" t="s">
+      <c r="F15" s="157" t="s">
         <v>72</v>
       </c>
-      <c r="G15" s="154" t="s">
+      <c r="G15" s="153" t="s">
         <v>214</v>
       </c>
       <c r="I15" s="104" t="s">
@@ -15189,7 +15242,7 @@
       <c r="J15" s="98" t="s">
         <v>298</v>
       </c>
-      <c r="K15" s="165" t="s">
+      <c r="K15" s="164" t="s">
         <v>204</v>
       </c>
     </row>
@@ -15197,7 +15250,7 @@
       <c r="A16" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="154" t="s">
+      <c r="B16" s="153" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="94"/>
@@ -15205,10 +15258,10 @@
       <c r="E16" s="94">
         <v>27</v>
       </c>
-      <c r="F16" s="158" t="s">
+      <c r="F16" s="157" t="s">
         <v>74</v>
       </c>
-      <c r="G16" s="154" t="s">
+      <c r="G16" s="153" t="s">
         <v>215</v>
       </c>
       <c r="I16" s="119" t="s">
@@ -15225,7 +15278,7 @@
       <c r="A17" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="154" t="s">
+      <c r="B17" s="153" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="94"/>
@@ -15233,10 +15286,10 @@
       <c r="E17" s="94">
         <v>14</v>
       </c>
-      <c r="F17" s="158" t="s">
+      <c r="F17" s="157" t="s">
         <v>76</v>
       </c>
-      <c r="G17" s="154" t="s">
+      <c r="G17" s="153" t="s">
         <v>216</v>
       </c>
     </row>
@@ -15394,7 +15447,7 @@
       <c r="B25" s="94"/>
       <c r="C25" s="94"/>
       <c r="D25" s="94"/>
-      <c r="E25" s="154">
+      <c r="E25" s="153">
         <f>SUM(E3:E24)</f>
         <v>162</v>
       </c>
@@ -15412,7 +15465,7 @@
       <c r="B26" s="91"/>
       <c r="C26" s="91"/>
       <c r="D26" s="91"/>
-      <c r="E26" s="158" t="s">
+      <c r="E26" s="157" t="s">
         <v>314</v>
       </c>
       <c r="F26" s="114"/>
@@ -15439,12 +15492,12 @@
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A28" s="155" t="s">
+      <c r="A28" s="154" t="s">
         <v>312</v>
       </c>
-      <c r="B28" s="156"/>
-      <c r="C28" s="156"/>
-      <c r="D28" s="157"/>
+      <c r="B28" s="155"/>
+      <c r="C28" s="155"/>
+      <c r="D28" s="156"/>
       <c r="I28" s="110" t="s">
         <v>294</v>
       </c>
@@ -15517,7 +15570,7 @@
       <c r="A33" s="84" t="s">
         <v>182</v>
       </c>
-      <c r="B33" s="165" t="s">
+      <c r="B33" s="164" t="s">
         <v>222</v>
       </c>
       <c r="I33" s="43" t="s">
@@ -15531,7 +15584,7 @@
       <c r="A34" s="100" t="s">
         <v>183</v>
       </c>
-      <c r="B34" s="165" t="s">
+      <c r="B34" s="164" t="s">
         <v>223</v>
       </c>
       <c r="I34" s="44" t="s">
@@ -15639,22 +15692,23 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="65.140625" customWidth="1"/>
+    <col min="2" max="2" width="48.5703125" customWidth="1"/>
     <col min="3" max="3" width="46.28515625" customWidth="1"/>
     <col min="5" max="5" width="30.5703125" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" style="3" customWidth="1"/>
     <col min="7" max="8" width="9.140625" style="3"/>
+    <col min="9" max="9" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="225" t="s">
         <v>464</v>
       </c>
@@ -15665,38 +15719,46 @@
       <c r="F1" s="225"/>
       <c r="G1" s="225"/>
       <c r="H1" s="225"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="174" t="s">
+      <c r="I1" s="225"/>
+      <c r="J1" s="225"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="173" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="174" t="s">
+      <c r="B2" s="173" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="174" t="s">
+      <c r="C2" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="174" t="s">
+      <c r="D2" s="173" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="174" t="s">
+      <c r="E2" s="173" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="174" t="s">
+      <c r="F2" s="173" t="s">
         <v>474</v>
       </c>
-      <c r="G2" s="174" t="s">
+      <c r="G2" s="173" t="s">
         <v>146</v>
       </c>
-      <c r="H2" s="174" t="s">
+      <c r="H2" s="173" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="179" t="s">
+      <c r="I2" s="173" t="s">
+        <v>164</v>
+      </c>
+      <c r="J2" s="234" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="178" t="s">
         <v>359</v>
       </c>
-      <c r="B3" s="177" t="s">
+      <c r="B3" s="176" t="s">
         <v>399</v>
       </c>
       <c r="C3" s="18" t="s">
@@ -15708,15 +15770,21 @@
       <c r="E3" s="18" t="s">
         <v>357</v>
       </c>
-      <c r="F3" s="34"/>
+      <c r="F3" s="34" t="s">
+        <v>501</v>
+      </c>
       <c r="G3" s="94"/>
       <c r="H3" s="94"/>
-    </row>
-    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="179" t="s">
+      <c r="I3" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="J3" s="232"/>
+    </row>
+    <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="178" t="s">
         <v>360</v>
       </c>
-      <c r="B4" s="177" t="s">
+      <c r="B4" s="176" t="s">
         <v>363</v>
       </c>
       <c r="C4" s="18" t="s">
@@ -15735,12 +15803,13 @@
         <v>12</v>
       </c>
       <c r="H4" s="94"/>
-    </row>
-    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="179" t="s">
+      <c r="I4" s="91"/>
+    </row>
+    <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="178" t="s">
         <v>364</v>
       </c>
-      <c r="B5" s="177" t="s">
+      <c r="B5" s="176" t="s">
         <v>367</v>
       </c>
       <c r="C5" s="18" t="s">
@@ -15759,12 +15828,13 @@
         <v>10</v>
       </c>
       <c r="H5" s="94"/>
-    </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="179" t="s">
+      <c r="I5" s="91"/>
+    </row>
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="178" t="s">
         <v>368</v>
       </c>
-      <c r="B6" s="177" t="s">
+      <c r="B6" s="176" t="s">
         <v>370</v>
       </c>
       <c r="C6" s="18" t="s">
@@ -15785,12 +15855,13 @@
       <c r="H6" s="53" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="179" t="s">
+      <c r="I6" s="91"/>
+    </row>
+    <row r="7" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="178" t="s">
         <v>372</v>
       </c>
-      <c r="B7" s="177" t="s">
+      <c r="B7" s="176" t="s">
         <v>374</v>
       </c>
       <c r="C7" s="18" t="s">
@@ -15809,12 +15880,13 @@
         <v>19</v>
       </c>
       <c r="H7" s="94"/>
-    </row>
-    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="179" t="s">
+      <c r="I7" s="91"/>
+    </row>
+    <row r="8" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="178" t="s">
         <v>378</v>
       </c>
-      <c r="B8" s="177" t="s">
+      <c r="B8" s="176" t="s">
         <v>478</v>
       </c>
       <c r="C8" s="18" t="s">
@@ -15833,12 +15905,13 @@
         <v>13</v>
       </c>
       <c r="H8" s="94"/>
-    </row>
-    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="179" t="s">
+      <c r="I8" s="91"/>
+    </row>
+    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="178" t="s">
         <v>379</v>
       </c>
-      <c r="B9" s="177" t="s">
+      <c r="B9" s="176" t="s">
         <v>382</v>
       </c>
       <c r="C9" s="18" t="s">
@@ -15850,15 +15923,21 @@
       <c r="E9" s="18" t="s">
         <v>380</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="235" t="s">
+        <v>500</v>
+      </c>
       <c r="G9" s="94"/>
       <c r="H9" s="94"/>
-    </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="179" t="s">
+      <c r="I9" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="J9" s="233"/>
+    </row>
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="178" t="s">
         <v>383</v>
       </c>
-      <c r="B10" s="177" t="s">
+      <c r="B10" s="176" t="s">
         <v>385</v>
       </c>
       <c r="C10" s="18" t="s">
@@ -15877,12 +15956,13 @@
         <v>26</v>
       </c>
       <c r="H10" s="94"/>
-    </row>
-    <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="179" t="s">
+      <c r="I10" s="91"/>
+    </row>
+    <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="178" t="s">
         <v>387</v>
       </c>
-      <c r="B11" s="177" t="s">
+      <c r="B11" s="176" t="s">
         <v>390</v>
       </c>
       <c r="C11" s="18" t="s">
@@ -15901,12 +15981,13 @@
         <v>21</v>
       </c>
       <c r="H11" s="94"/>
-    </row>
-    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="179" t="s">
+      <c r="I11" s="91"/>
+    </row>
+    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="178" t="s">
         <v>391</v>
       </c>
-      <c r="B12" s="177" t="s">
+      <c r="B12" s="176" t="s">
         <v>393</v>
       </c>
       <c r="C12" s="18" t="s">
@@ -15918,15 +15999,21 @@
       <c r="E12" s="18" t="s">
         <v>392</v>
       </c>
-      <c r="F12" s="178"/>
+      <c r="F12" s="177" t="s">
+        <v>499</v>
+      </c>
       <c r="G12" s="94"/>
       <c r="H12" s="94"/>
-    </row>
-    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="179" t="s">
+      <c r="I12" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="J12" s="232"/>
+    </row>
+    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="178" t="s">
         <v>395</v>
       </c>
-      <c r="B13" s="177" t="s">
+      <c r="B13" s="176" t="s">
         <v>398</v>
       </c>
       <c r="C13" s="18" t="s">
@@ -15945,12 +16032,13 @@
         <v>18</v>
       </c>
       <c r="H13" s="94"/>
-    </row>
-    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="179" t="s">
+      <c r="I13" s="91"/>
+    </row>
+    <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="178" t="s">
         <v>400</v>
       </c>
-      <c r="B14" s="177" t="s">
+      <c r="B14" s="176" t="s">
         <v>402</v>
       </c>
       <c r="C14" s="18" t="s">
@@ -15969,12 +16057,13 @@
         <v>45</v>
       </c>
       <c r="H14" s="94"/>
-    </row>
-    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="179" t="s">
+      <c r="I14" s="91"/>
+    </row>
+    <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="178" t="s">
         <v>404</v>
       </c>
-      <c r="B15" s="177" t="s">
+      <c r="B15" s="176" t="s">
         <v>406</v>
       </c>
       <c r="C15" s="18" t="s">
@@ -15993,12 +16082,13 @@
         <v>28</v>
       </c>
       <c r="H15" s="94"/>
-    </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="179" t="s">
+      <c r="I15" s="91"/>
+    </row>
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="178" t="s">
         <v>407</v>
       </c>
-      <c r="B16" s="177" t="s">
+      <c r="B16" s="176" t="s">
         <v>409</v>
       </c>
       <c r="C16" s="18" t="s">
@@ -16017,12 +16107,13 @@
         <v>14</v>
       </c>
       <c r="H16" s="94"/>
-    </row>
-    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="179" t="s">
+      <c r="I16" s="91"/>
+    </row>
+    <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="178" t="s">
         <v>411</v>
       </c>
-      <c r="B17" s="177" t="s">
+      <c r="B17" s="176" t="s">
         <v>413</v>
       </c>
       <c r="C17" s="18" t="s">
@@ -16035,18 +16126,22 @@
         <v>412</v>
       </c>
       <c r="F17" s="29" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G17" s="94">
         <v>5</v>
       </c>
       <c r="H17" s="94"/>
-    </row>
-    <row r="18" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="179" t="s">
+      <c r="I17" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="J17" s="233"/>
+    </row>
+    <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="178" t="s">
         <v>415</v>
       </c>
-      <c r="B18" s="177" t="s">
+      <c r="B18" s="176" t="s">
         <v>419</v>
       </c>
       <c r="C18" s="18" t="s">
@@ -16065,12 +16160,13 @@
         <v>15</v>
       </c>
       <c r="H18" s="94"/>
-    </row>
-    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="179" t="s">
+      <c r="I18" s="91"/>
+    </row>
+    <row r="19" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="178" t="s">
         <v>417</v>
       </c>
-      <c r="B19" s="177" t="s">
+      <c r="B19" s="176" t="s">
         <v>421</v>
       </c>
       <c r="C19" s="18" t="s">
@@ -16083,16 +16179,20 @@
         <v>418</v>
       </c>
       <c r="F19" s="85" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G19" s="94"/>
       <c r="H19" s="94"/>
-    </row>
-    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="179" t="s">
+      <c r="I19" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="J19" s="232"/>
+    </row>
+    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="178" t="s">
         <v>423</v>
       </c>
-      <c r="B20" s="177" t="s">
+      <c r="B20" s="176" t="s">
         <v>466</v>
       </c>
       <c r="C20" s="18" t="s">
@@ -16105,18 +16205,19 @@
         <v>424</v>
       </c>
       <c r="F20" s="94" t="s">
-        <v>486</v>
+        <v>506</v>
       </c>
       <c r="G20" s="94">
         <v>31</v>
       </c>
       <c r="H20" s="94"/>
-    </row>
-    <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="179" t="s">
+      <c r="I20" s="91"/>
+    </row>
+    <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="178" t="s">
         <v>426</v>
       </c>
-      <c r="B21" s="177" t="s">
+      <c r="B21" s="176" t="s">
         <v>428</v>
       </c>
       <c r="C21" s="18" t="s">
@@ -16128,17 +16229,21 @@
       <c r="E21" s="18" t="s">
         <v>424</v>
       </c>
-      <c r="F21" s="34" t="s">
-        <v>497</v>
+      <c r="F21" s="29" t="s">
+        <v>496</v>
       </c>
       <c r="G21" s="94"/>
       <c r="H21" s="94"/>
-    </row>
-    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="179" t="s">
+      <c r="I21" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="J21" s="233"/>
+    </row>
+    <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="178" t="s">
         <v>429</v>
       </c>
-      <c r="B22" s="177" t="s">
+      <c r="B22" s="176" t="s">
         <v>431</v>
       </c>
       <c r="C22" s="18" t="s">
@@ -16151,18 +16256,19 @@
         <v>430</v>
       </c>
       <c r="F22" s="94" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G22" s="94">
         <v>7</v>
       </c>
       <c r="H22" s="94"/>
-    </row>
-    <row r="23" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="179" t="s">
+      <c r="I22" s="91"/>
+    </row>
+    <row r="23" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="178" t="s">
         <v>433</v>
       </c>
-      <c r="B23" s="177" t="s">
+      <c r="B23" s="176" t="s">
         <v>436</v>
       </c>
       <c r="C23" s="18" t="s">
@@ -16175,18 +16281,19 @@
         <v>434</v>
       </c>
       <c r="F23" s="94" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G23" s="94">
         <v>7</v>
       </c>
       <c r="H23" s="94"/>
-    </row>
-    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="179" t="s">
+      <c r="I23" s="91"/>
+    </row>
+    <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="178" t="s">
         <v>437</v>
       </c>
-      <c r="B24" s="177" t="s">
+      <c r="B24" s="176" t="s">
         <v>439</v>
       </c>
       <c r="C24" s="18" t="s">
@@ -16198,17 +16305,23 @@
       <c r="E24" s="18" t="s">
         <v>438</v>
       </c>
-      <c r="F24" s="34" t="s">
-        <v>496</v>
-      </c>
-      <c r="G24" s="94"/>
+      <c r="F24" s="29" t="s">
+        <v>495</v>
+      </c>
+      <c r="G24" s="94">
+        <v>14</v>
+      </c>
       <c r="H24" s="94"/>
-    </row>
-    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="179" t="s">
+      <c r="I24" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="J24" s="233"/>
+    </row>
+    <row r="25" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="178" t="s">
         <v>440</v>
       </c>
-      <c r="B25" s="177" t="s">
+      <c r="B25" s="176" t="s">
         <v>442</v>
       </c>
       <c r="C25" s="18" t="s">
@@ -16220,17 +16333,21 @@
       <c r="E25" s="18" t="s">
         <v>441</v>
       </c>
-      <c r="F25" s="34" t="s">
-        <v>495</v>
+      <c r="F25" s="235" t="s">
+        <v>494</v>
       </c>
       <c r="G25" s="94"/>
       <c r="H25" s="94"/>
-    </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="179" t="s">
+      <c r="I25" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="J25" s="233"/>
+    </row>
+    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="178" t="s">
         <v>444</v>
       </c>
-      <c r="B26" s="177" t="s">
+      <c r="B26" s="176" t="s">
         <v>445</v>
       </c>
       <c r="C26" s="18" t="s">
@@ -16243,18 +16360,19 @@
         <v>408</v>
       </c>
       <c r="F26" s="94" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="G26" s="94">
         <v>19</v>
       </c>
       <c r="H26" s="94"/>
-    </row>
-    <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="179" t="s">
+      <c r="I26" s="91"/>
+    </row>
+    <row r="27" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="178" t="s">
         <v>447</v>
       </c>
-      <c r="B27" s="177" t="s">
+      <c r="B27" s="176" t="s">
         <v>450</v>
       </c>
       <c r="C27" s="18" t="s">
@@ -16267,18 +16385,19 @@
         <v>448</v>
       </c>
       <c r="F27" s="29" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G27" s="94">
         <v>19</v>
       </c>
       <c r="H27" s="94"/>
-    </row>
-    <row r="28" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="179" t="s">
+      <c r="I27" s="91"/>
+    </row>
+    <row r="28" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="178" t="s">
         <v>451</v>
       </c>
-      <c r="B28" s="177" t="s">
+      <c r="B28" s="176" t="s">
         <v>467</v>
       </c>
       <c r="C28" s="18" t="s">
@@ -16291,18 +16410,19 @@
         <v>455</v>
       </c>
       <c r="F28" s="29" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="G28" s="94">
         <v>13</v>
       </c>
       <c r="H28" s="94"/>
-    </row>
-    <row r="29" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="179" t="s">
+      <c r="I28" s="91"/>
+    </row>
+    <row r="29" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="178" t="s">
         <v>452</v>
       </c>
-      <c r="B29" s="177" t="s">
+      <c r="B29" s="176" t="s">
         <v>458</v>
       </c>
       <c r="C29" s="18" t="s">
@@ -16314,17 +16434,23 @@
       <c r="E29" s="18" t="s">
         <v>457</v>
       </c>
-      <c r="F29" s="34" t="s">
-        <v>494</v>
-      </c>
-      <c r="G29" s="94"/>
+      <c r="F29" s="29" t="s">
+        <v>493</v>
+      </c>
+      <c r="G29" s="94">
+        <v>8</v>
+      </c>
       <c r="H29" s="94"/>
-    </row>
-    <row r="30" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="179" t="s">
+      <c r="I29" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="J29" s="233"/>
+    </row>
+    <row r="30" spans="1:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="178" t="s">
         <v>453</v>
       </c>
-      <c r="B30" s="177" t="s">
+      <c r="B30" s="176" t="s">
         <v>462</v>
       </c>
       <c r="C30" s="18" t="s">
@@ -16337,18 +16463,19 @@
         <v>460</v>
       </c>
       <c r="F30" s="29" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="G30" s="94">
         <v>13</v>
       </c>
       <c r="H30" s="94"/>
-    </row>
-    <row r="31" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A31" s="179" t="s">
+      <c r="I30" s="91"/>
+    </row>
+    <row r="31" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="178" t="s">
         <v>454</v>
       </c>
-      <c r="B31" s="177" t="s">
+      <c r="B31" s="176" t="s">
         <v>463</v>
       </c>
       <c r="C31" s="18" t="s">
@@ -16360,15 +16487,24 @@
       <c r="E31" s="18" t="s">
         <v>420</v>
       </c>
-      <c r="F31" s="34" t="s">
-        <v>493</v>
-      </c>
-      <c r="G31" s="94"/>
+      <c r="F31" s="29" t="s">
+        <v>492</v>
+      </c>
+      <c r="G31" s="94">
+        <v>10</v>
+      </c>
       <c r="H31" s="94"/>
+      <c r="I31" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="J31" s="233"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="236"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Validate antes do FSB - ok
</commit_message>
<xml_diff>
--- a/Experiment01_Resumo/Resumo_Exp01.xlsx
+++ b/Experiment01_Resumo/Resumo_Exp01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="526">
   <si>
     <t>Database search</t>
   </si>
@@ -1671,6 +1671,51 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>petersen2015a</t>
+  </si>
+  <si>
+    <t>barreto2010a</t>
+  </si>
+  <si>
+    <t>trienekens2009a</t>
+  </si>
+  <si>
+    <t>basili2010a</t>
+  </si>
+  <si>
+    <t>sommerville1999a</t>
+  </si>
+  <si>
+    <t>wang2005a</t>
+  </si>
+  <si>
+    <t>plösch2011a</t>
+  </si>
+  <si>
+    <t>mandić2010a</t>
+  </si>
+  <si>
+    <t>trienekens2005a</t>
+  </si>
+  <si>
+    <t>esfahani2011a</t>
+  </si>
+  <si>
+    <t>becker2008b</t>
+  </si>
+  <si>
+    <t>oConnor2015a</t>
+  </si>
+  <si>
+    <t>kautz2000a</t>
+  </si>
+  <si>
+    <t>mandić2010b</t>
+  </si>
+  <si>
+    <t>Análise da quantidade de seed set por biblioteca digital</t>
   </si>
 </sst>
 </file>
@@ -2357,7 +2402,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="235">
+  <cellXfs count="236">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2871,6 +2916,33 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2880,12 +2952,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2898,27 +2964,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2978,6 +3023,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3302,12 +3350,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="210404552"/>
-        <c:axId val="210407296"/>
+        <c:axId val="206411768"/>
+        <c:axId val="206408240"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="210404552"/>
+        <c:axId val="206411768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3399,7 +3447,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210407296"/>
+        <c:crossAx val="206408240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3407,7 +3455,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="210407296"/>
+        <c:axId val="206408240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3458,7 +3506,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210404552"/>
+        <c:crossAx val="206411768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3767,12 +3815,12 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:shape val="box"/>
-        <c:axId val="210406904"/>
-        <c:axId val="210405336"/>
+        <c:axId val="206409808"/>
+        <c:axId val="206410984"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="210406904"/>
+        <c:axId val="206409808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3861,7 +3909,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210405336"/>
+        <c:crossAx val="206410984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3869,7 +3917,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="210405336"/>
+        <c:axId val="206410984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3952,7 +4000,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210406904"/>
+        <c:crossAx val="206409808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4237,12 +4285,12 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:shape val="box"/>
-        <c:axId val="210411216"/>
-        <c:axId val="210403768"/>
+        <c:axId val="206409024"/>
+        <c:axId val="209227736"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="210411216"/>
+        <c:axId val="206409024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4331,7 +4379,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210403768"/>
+        <c:crossAx val="209227736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4339,7 +4387,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="210403768"/>
+        <c:axId val="209227736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4422,7 +4470,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210411216"/>
+        <c:crossAx val="206409024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5209,12 +5257,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="211879008"/>
-        <c:axId val="211879400"/>
+        <c:axId val="209229304"/>
+        <c:axId val="209225776"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="211879008"/>
+        <c:axId val="209229304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5254,7 +5302,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211879400"/>
+        <c:crossAx val="209225776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5262,7 +5310,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="211879400"/>
+        <c:axId val="209225776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5310,7 +5358,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211879008"/>
+        <c:crossAx val="209229304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5618,8 +5666,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="211880576"/>
-        <c:axId val="211884496"/>
+        <c:axId val="209226168"/>
+        <c:axId val="209226952"/>
         <c:axId val="0"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -5789,7 +5837,7 @@
         </c:extLst>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="211880576"/>
+        <c:axId val="209226168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5887,7 +5935,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211884496"/>
+        <c:crossAx val="209226952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5895,7 +5943,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="211884496"/>
+        <c:axId val="209226952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5974,7 +6022,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="211880576"/>
+        <c:crossAx val="209226168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6288,8 +6336,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="211880184"/>
-        <c:axId val="211885280"/>
+        <c:axId val="209223424"/>
+        <c:axId val="209229696"/>
         <c:axId val="0"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -6459,7 +6507,7 @@
         </c:extLst>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="211880184"/>
+        <c:axId val="209223424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6557,7 +6605,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211885280"/>
+        <c:crossAx val="209229696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6565,7 +6613,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="211885280"/>
+        <c:axId val="209229696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6644,7 +6692,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="211880184"/>
+        <c:crossAx val="209223424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10331,7 +10379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -11208,7 +11256,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -12688,7 +12736,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12698,7 +12746,7 @@
     <col min="3" max="3" width="57.140625" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" style="3" customWidth="1"/>
     <col min="5" max="5" width="41.5703125" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" style="81" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
@@ -12747,7 +12795,7 @@
       <c r="E3" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="91" t="s">
+      <c r="F3" s="48" t="s">
         <v>502</v>
       </c>
     </row>
@@ -12767,7 +12815,7 @@
       <c r="E4" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="F4" s="91" t="s">
+      <c r="F4" s="48" t="s">
         <v>209</v>
       </c>
     </row>
@@ -12787,7 +12835,7 @@
       <c r="E5" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="F5" s="91" t="s">
+      <c r="F5" s="48" t="s">
         <v>210</v>
       </c>
     </row>
@@ -12807,7 +12855,9 @@
       <c r="E6" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="F6" s="91"/>
+      <c r="F6" s="48" t="s">
+        <v>511</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="132" t="s">
@@ -12825,7 +12875,9 @@
       <c r="E7" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="F7" s="91"/>
+      <c r="F7" s="48" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="132" t="s">
@@ -12843,7 +12895,9 @@
       <c r="E8" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="F8" s="91"/>
+      <c r="F8" s="48" t="s">
+        <v>512</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="132" t="s">
@@ -12861,7 +12915,9 @@
       <c r="E9" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="F9" s="91"/>
+      <c r="F9" s="48" t="s">
+        <v>513</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="132" t="s">
@@ -12879,7 +12935,9 @@
       <c r="E10" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="F10" s="91"/>
+      <c r="F10" s="48" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="132" t="s">
@@ -12897,7 +12955,9 @@
       <c r="E11" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="F11" s="91"/>
+      <c r="F11" s="48" t="s">
+        <v>514</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="132" t="s">
@@ -12915,7 +12975,9 @@
       <c r="E12" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="F12" s="91"/>
+      <c r="F12" s="48" t="s">
+        <v>515</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="132" t="s">
@@ -12933,7 +12995,9 @@
       <c r="E13" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="F13" s="91"/>
+      <c r="F13" s="48" t="s">
+        <v>516</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="132" t="s">
@@ -12951,7 +13015,9 @@
       <c r="E14" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="F14" s="91"/>
+      <c r="F14" s="48" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="132" t="s">
@@ -12969,7 +13035,9 @@
       <c r="E15" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="F15" s="91"/>
+      <c r="F15" s="48" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="132" t="s">
@@ -12987,7 +13055,9 @@
       <c r="E16" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="F16" s="91"/>
+      <c r="F16" s="48" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="132" t="s">
@@ -13005,7 +13075,9 @@
       <c r="E17" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="F17" s="91"/>
+      <c r="F17" s="48" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="132" t="s">
@@ -13023,7 +13095,9 @@
       <c r="E18" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="F18" s="91"/>
+      <c r="F18" s="48" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="132" t="s">
@@ -13041,7 +13115,9 @@
       <c r="E19" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="F19" s="91"/>
+      <c r="F19" s="48" t="s">
+        <v>519</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="132" t="s">
@@ -13059,7 +13135,9 @@
       <c r="E20" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="F20" s="91"/>
+      <c r="F20" s="48" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="132" t="s">
@@ -13077,7 +13155,9 @@
       <c r="E21" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="F21" s="91"/>
+      <c r="F21" s="48" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="22" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="132" t="s">
@@ -13095,7 +13175,9 @@
       <c r="E22" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="F22" s="91"/>
+      <c r="F22" s="48" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="23" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="132" t="s">
@@ -13113,7 +13195,9 @@
       <c r="E23" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="F23" s="91"/>
+      <c r="F23" s="48" t="s">
+        <v>523</v>
+      </c>
     </row>
     <row r="24" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="132" t="s">
@@ -13131,7 +13215,9 @@
       <c r="E24" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="F24" s="91"/>
+      <c r="F24" s="48" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="144" t="s">
@@ -13172,43 +13258,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="199" t="s">
+      <c r="A1" s="208" t="s">
         <v>230</v>
       </c>
-      <c r="B1" s="200"/>
-      <c r="C1" s="200"/>
-      <c r="D1" s="200"/>
-      <c r="E1" s="200"/>
-      <c r="F1" s="200"/>
-      <c r="G1" s="200"/>
-      <c r="H1" s="200"/>
-      <c r="I1" s="200"/>
+      <c r="B1" s="209"/>
+      <c r="C1" s="209"/>
+      <c r="D1" s="209"/>
+      <c r="E1" s="209"/>
+      <c r="F1" s="209"/>
+      <c r="G1" s="209"/>
+      <c r="H1" s="209"/>
+      <c r="I1" s="209"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="202" t="s">
+      <c r="A2" s="207" t="s">
         <v>229</v>
       </c>
-      <c r="B2" s="202"/>
-      <c r="C2" s="202"/>
-      <c r="D2" s="202"/>
-      <c r="E2" s="202"/>
-      <c r="F2" s="202"/>
-      <c r="G2" s="202"/>
-      <c r="H2" s="202"/>
-      <c r="I2" s="202"/>
+      <c r="B2" s="207"/>
+      <c r="C2" s="207"/>
+      <c r="D2" s="207"/>
+      <c r="E2" s="207"/>
+      <c r="F2" s="207"/>
+      <c r="G2" s="207"/>
+      <c r="H2" s="207"/>
+      <c r="I2" s="207"/>
     </row>
     <row r="3" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="203" t="s">
+      <c r="A3" s="200" t="s">
         <v>337</v>
       </c>
-      <c r="B3" s="203"/>
-      <c r="C3" s="203"/>
-      <c r="D3" s="203"/>
-      <c r="E3" s="203"/>
-      <c r="F3" s="203"/>
-      <c r="G3" s="203"/>
-      <c r="H3" s="203"/>
-      <c r="I3" s="203"/>
+      <c r="B3" s="200"/>
+      <c r="C3" s="200"/>
+      <c r="D3" s="200"/>
+      <c r="E3" s="200"/>
+      <c r="F3" s="200"/>
+      <c r="G3" s="200"/>
+      <c r="H3" s="200"/>
+      <c r="I3" s="200"/>
       <c r="J3" s="71"/>
       <c r="K3" s="71"/>
       <c r="L3" s="71"/>
@@ -13221,12 +13307,12 @@
       <c r="S3" s="71"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="201" t="s">
+      <c r="A4" s="210" t="s">
         <v>253</v>
       </c>
-      <c r="B4" s="201"/>
-      <c r="C4" s="201"/>
-      <c r="D4" s="201"/>
+      <c r="B4" s="210"/>
+      <c r="C4" s="210"/>
+      <c r="D4" s="210"/>
     </row>
     <row r="5" spans="1:19" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="69" t="s">
@@ -13252,7 +13338,7 @@
       <c r="C6" s="49" t="s">
         <v>196</v>
       </c>
-      <c r="D6" s="212" t="s">
+      <c r="D6" s="204" t="s">
         <v>339</v>
       </c>
       <c r="E6" t="e">
@@ -13271,7 +13357,7 @@
       <c r="C7" s="49" t="s">
         <v>228</v>
       </c>
-      <c r="D7" s="213"/>
+      <c r="D7" s="205"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="78" t="s">
@@ -13283,7 +13369,7 @@
       <c r="C8" s="49" t="s">
         <v>235</v>
       </c>
-      <c r="D8" s="213"/>
+      <c r="D8" s="205"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="78" t="s">
@@ -13295,7 +13381,7 @@
       <c r="C9" s="49" t="s">
         <v>236</v>
       </c>
-      <c r="D9" s="213"/>
+      <c r="D9" s="205"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="78" t="s">
@@ -13307,7 +13393,7 @@
       <c r="C10" s="49" t="s">
         <v>237</v>
       </c>
-      <c r="D10" s="213"/>
+      <c r="D10" s="205"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="78" t="s">
@@ -13319,7 +13405,7 @@
       <c r="C11" s="49" t="s">
         <v>237</v>
       </c>
-      <c r="D11" s="213"/>
+      <c r="D11" s="205"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="78" t="s">
@@ -13331,7 +13417,7 @@
       <c r="C12" s="49" t="s">
         <v>266</v>
       </c>
-      <c r="D12" s="213"/>
+      <c r="D12" s="205"/>
     </row>
     <row r="13" spans="1:19" s="77" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="145" t="s">
@@ -13343,7 +13429,7 @@
       <c r="C13" s="136" t="s">
         <v>273</v>
       </c>
-      <c r="D13" s="214"/>
+      <c r="D13" s="206"/>
     </row>
     <row r="14" spans="1:19" s="77" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="146" t="s">
@@ -13360,30 +13446,30 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="202" t="s">
+      <c r="A15" s="207" t="s">
         <v>261</v>
       </c>
-      <c r="B15" s="202"/>
-      <c r="C15" s="202"/>
-      <c r="D15" s="202"/>
-      <c r="E15" s="202"/>
-      <c r="F15" s="202"/>
-      <c r="G15" s="202"/>
-      <c r="H15" s="202"/>
-      <c r="I15" s="202"/>
+      <c r="B15" s="207"/>
+      <c r="C15" s="207"/>
+      <c r="D15" s="207"/>
+      <c r="E15" s="207"/>
+      <c r="F15" s="207"/>
+      <c r="G15" s="207"/>
+      <c r="H15" s="207"/>
+      <c r="I15" s="207"/>
     </row>
     <row r="16" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="203" t="s">
+      <c r="A16" s="200" t="s">
         <v>238</v>
       </c>
-      <c r="B16" s="203"/>
-      <c r="C16" s="203"/>
-      <c r="D16" s="203"/>
-      <c r="E16" s="203"/>
-      <c r="F16" s="203"/>
-      <c r="G16" s="203"/>
-      <c r="H16" s="203"/>
-      <c r="I16" s="203"/>
+      <c r="B16" s="200"/>
+      <c r="C16" s="200"/>
+      <c r="D16" s="200"/>
+      <c r="E16" s="200"/>
+      <c r="F16" s="200"/>
+      <c r="G16" s="200"/>
+      <c r="H16" s="200"/>
+      <c r="I16" s="200"/>
       <c r="J16" s="71"/>
       <c r="K16" s="71"/>
       <c r="L16" s="71"/>
@@ -13396,14 +13482,14 @@
       <c r="S16" s="71"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="201" t="s">
+      <c r="A17" s="210" t="s">
         <v>259</v>
       </c>
-      <c r="B17" s="201"/>
-      <c r="C17" s="201"/>
-      <c r="D17" s="201"/>
-      <c r="E17" s="201"/>
-      <c r="F17" s="201"/>
+      <c r="B17" s="210"/>
+      <c r="C17" s="210"/>
+      <c r="D17" s="210"/>
+      <c r="E17" s="210"/>
+      <c r="F17" s="210"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="69" t="s">
@@ -13570,30 +13656,30 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="202" t="s">
+      <c r="A25" s="207" t="s">
         <v>260</v>
       </c>
-      <c r="B25" s="202"/>
-      <c r="C25" s="202"/>
-      <c r="D25" s="202"/>
-      <c r="E25" s="202"/>
-      <c r="F25" s="202"/>
-      <c r="G25" s="202"/>
-      <c r="H25" s="202"/>
-      <c r="I25" s="202"/>
+      <c r="B25" s="207"/>
+      <c r="C25" s="207"/>
+      <c r="D25" s="207"/>
+      <c r="E25" s="207"/>
+      <c r="F25" s="207"/>
+      <c r="G25" s="207"/>
+      <c r="H25" s="207"/>
+      <c r="I25" s="207"/>
     </row>
     <row r="26" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="203" t="s">
+      <c r="A26" s="200" t="s">
         <v>338</v>
       </c>
-      <c r="B26" s="203"/>
-      <c r="C26" s="203"/>
-      <c r="D26" s="203"/>
-      <c r="E26" s="203"/>
-      <c r="F26" s="203"/>
-      <c r="G26" s="203"/>
-      <c r="H26" s="203"/>
-      <c r="I26" s="203"/>
+      <c r="B26" s="200"/>
+      <c r="C26" s="200"/>
+      <c r="D26" s="200"/>
+      <c r="E26" s="200"/>
+      <c r="F26" s="200"/>
+      <c r="G26" s="200"/>
+      <c r="H26" s="200"/>
+      <c r="I26" s="200"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="69" t="s">
@@ -13605,12 +13691,12 @@
       <c r="C27" s="69" t="s">
         <v>201</v>
       </c>
-      <c r="D27" s="207" t="s">
+      <c r="D27" s="214" t="s">
         <v>292</v>
       </c>
-      <c r="E27" s="207"/>
-      <c r="F27" s="207"/>
-      <c r="G27" s="207"/>
+      <c r="E27" s="214"/>
+      <c r="F27" s="214"/>
+      <c r="G27" s="214"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="52" t="s">
@@ -13622,12 +13708,12 @@
       <c r="C28" s="72">
         <v>0.59</v>
       </c>
-      <c r="D28" s="209" t="s">
+      <c r="D28" s="201" t="s">
         <v>285</v>
       </c>
-      <c r="E28" s="210"/>
-      <c r="F28" s="210"/>
-      <c r="G28" s="211"/>
+      <c r="E28" s="202"/>
+      <c r="F28" s="202"/>
+      <c r="G28" s="203"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="52" t="s">
@@ -13639,12 +13725,12 @@
       <c r="C29" s="72">
         <v>0.77</v>
       </c>
-      <c r="D29" s="204" t="s">
+      <c r="D29" s="211" t="s">
         <v>286</v>
       </c>
-      <c r="E29" s="205"/>
-      <c r="F29" s="205"/>
-      <c r="G29" s="206"/>
+      <c r="E29" s="212"/>
+      <c r="F29" s="212"/>
+      <c r="G29" s="213"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="52" t="s">
@@ -13656,12 +13742,12 @@
       <c r="C30" s="72">
         <v>0.41</v>
       </c>
-      <c r="D30" s="204" t="s">
+      <c r="D30" s="211" t="s">
         <v>287</v>
       </c>
-      <c r="E30" s="205"/>
-      <c r="F30" s="205"/>
-      <c r="G30" s="206"/>
+      <c r="E30" s="212"/>
+      <c r="F30" s="212"/>
+      <c r="G30" s="213"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="52" t="s">
@@ -13673,12 +13759,12 @@
       <c r="C31" s="72">
         <v>0.59</v>
       </c>
-      <c r="D31" s="204" t="s">
+      <c r="D31" s="211" t="s">
         <v>289</v>
       </c>
-      <c r="E31" s="205"/>
-      <c r="F31" s="205"/>
-      <c r="G31" s="206"/>
+      <c r="E31" s="212"/>
+      <c r="F31" s="212"/>
+      <c r="G31" s="213"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="52" t="s">
@@ -13690,12 +13776,12 @@
       <c r="C32" s="72">
         <v>0.5</v>
       </c>
-      <c r="D32" s="204" t="s">
+      <c r="D32" s="211" t="s">
         <v>288</v>
       </c>
-      <c r="E32" s="205"/>
-      <c r="F32" s="205"/>
-      <c r="G32" s="206"/>
+      <c r="E32" s="212"/>
+      <c r="F32" s="212"/>
+      <c r="G32" s="213"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="52" t="s">
@@ -13707,12 +13793,12 @@
       <c r="C33" s="72">
         <v>0.59</v>
       </c>
-      <c r="D33" s="204" t="s">
+      <c r="D33" s="211" t="s">
         <v>290</v>
       </c>
-      <c r="E33" s="205"/>
-      <c r="F33" s="205"/>
-      <c r="G33" s="206"/>
+      <c r="E33" s="212"/>
+      <c r="F33" s="212"/>
+      <c r="G33" s="213"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="52" t="s">
@@ -13724,25 +13810,25 @@
       <c r="C34" s="72">
         <v>0.54</v>
       </c>
-      <c r="D34" s="204" t="s">
+      <c r="D34" s="211" t="s">
         <v>291</v>
       </c>
-      <c r="E34" s="205"/>
-      <c r="F34" s="205"/>
-      <c r="G34" s="206"/>
+      <c r="E34" s="212"/>
+      <c r="F34" s="212"/>
+      <c r="G34" s="213"/>
     </row>
     <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="202" t="s">
+      <c r="A36" s="207" t="s">
         <v>315</v>
       </c>
-      <c r="B36" s="202"/>
-      <c r="C36" s="202"/>
-      <c r="D36" s="202"/>
-      <c r="E36" s="202"/>
-      <c r="F36" s="202"/>
-      <c r="G36" s="202"/>
-      <c r="H36" s="202"/>
-      <c r="I36" s="202"/>
+      <c r="B36" s="207"/>
+      <c r="C36" s="207"/>
+      <c r="D36" s="207"/>
+      <c r="E36" s="207"/>
+      <c r="F36" s="207"/>
+      <c r="G36" s="207"/>
+      <c r="H36" s="207"/>
+      <c r="I36" s="207"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="87" t="s">
@@ -13809,12 +13895,12 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="208" t="s">
+      <c r="A46" s="199" t="s">
         <v>318</v>
       </c>
-      <c r="B46" s="208"/>
-      <c r="C46" s="208"/>
-      <c r="D46" s="208"/>
+      <c r="B46" s="199"/>
+      <c r="C46" s="199"/>
+      <c r="D46" s="199"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="88" t="s">
@@ -13965,11 +14051,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="D28:G28"/>
-    <mergeCell ref="D6:D13"/>
-    <mergeCell ref="A2:I2"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="A25:I25"/>
@@ -13985,6 +14066,11 @@
     <mergeCell ref="D30:G30"/>
     <mergeCell ref="D31:G31"/>
     <mergeCell ref="D32:G32"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="D6:D13"/>
+    <mergeCell ref="A2:I2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -15692,8 +15778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16553,12 +16639,29 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="235" t="s">
+        <v>525</v>
+      </c>
+      <c r="B1" s="235"/>
+      <c r="C1" s="235"/>
+      <c r="D1" s="235"/>
+      <c r="E1" s="235"/>
+      <c r="F1" s="235"/>
+      <c r="G1" s="235"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
FSB do 29 ao 51 menos 5
</commit_message>
<xml_diff>
--- a/Experiment01_Resumo/Resumo_Exp01.xlsx
+++ b/Experiment01_Resumo/Resumo_Exp01.xlsx
@@ -9,22 +9,23 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="1" r:id="rId1"/>
     <sheet name="Resumo DatabaseSnowballing" sheetId="8" r:id="rId2"/>
     <sheet name="SearchResults" sheetId="9" r:id="rId3"/>
     <sheet name="Seed Set" sheetId="5" r:id="rId4"/>
-    <sheet name="ResearchQuestions" sheetId="11" r:id="rId5"/>
-    <sheet name="Scopus" sheetId="10" r:id="rId6"/>
-    <sheet name="BSB-FSB" sheetId="16" r:id="rId7"/>
-    <sheet name="NewSetOfPapers" sheetId="17" r:id="rId8"/>
-    <sheet name="SeedSet_DL" sheetId="18" r:id="rId9"/>
-    <sheet name="Não encontrados na Busca" sheetId="15" r:id="rId10"/>
-    <sheet name="BuscaGoogleScholar" sheetId="13" r:id="rId11"/>
-    <sheet name="BuscaPorTítulo" sheetId="14" r:id="rId12"/>
-    <sheet name="Threats" sheetId="12" r:id="rId13"/>
+    <sheet name="Plan1" sheetId="19" r:id="rId5"/>
+    <sheet name="ResearchQuestions" sheetId="11" r:id="rId6"/>
+    <sheet name="Scopus" sheetId="10" r:id="rId7"/>
+    <sheet name="BSB-FSB" sheetId="16" r:id="rId8"/>
+    <sheet name="NewSetOfPapers" sheetId="17" r:id="rId9"/>
+    <sheet name="SeedSet_DL" sheetId="18" r:id="rId10"/>
+    <sheet name="Não encontrados na Busca" sheetId="15" r:id="rId11"/>
+    <sheet name="BuscaGoogleScholar" sheetId="13" r:id="rId12"/>
+    <sheet name="BuscaPorTítulo" sheetId="14" r:id="rId13"/>
+    <sheet name="Threats" sheetId="12" r:id="rId14"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1474" uniqueCount="551">
   <si>
     <t>Database search</t>
   </si>
@@ -1716,6 +1717,81 @@
   </si>
   <si>
     <t>Análise da quantidade de seed set por biblioteca digital</t>
+  </si>
+  <si>
+    <t>Excluído</t>
+  </si>
+  <si>
+    <t>Comprou</t>
+  </si>
+  <si>
+    <t>Recebeu cópia ao comprar o 39</t>
+  </si>
+  <si>
+    <t>Não acessível</t>
+  </si>
+  <si>
+    <t>Selecionados</t>
+  </si>
+  <si>
+    <t>Não fez BSB pq estava indisponível</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Citado por 8, mas 2 são de 2016 e 1 de 2017. Então foram incluídos somente 5. </t>
+  </si>
+  <si>
+    <t>Citado por 1, mas este é de 2016. Logo, a JF Tool não pegou.</t>
+  </si>
+  <si>
+    <t>Citado por 4, mas view 1.</t>
+  </si>
+  <si>
+    <t>Citado por 0.</t>
+  </si>
+  <si>
+    <t>Citado por 1.</t>
+  </si>
+  <si>
+    <t>Citado por 19</t>
+  </si>
+  <si>
+    <t>Citado por 4.</t>
+  </si>
+  <si>
+    <t>Citado por 3, mas são de 2016.</t>
+  </si>
+  <si>
+    <t>Citado por 5, mas 1 é de 2016</t>
+  </si>
+  <si>
+    <t>Citado por 1 de 2018.</t>
+  </si>
+  <si>
+    <t>Citado por 15 na JF Tool, mas no Scholar está com 17 pq 2 já existiam, e resultado final com 10 (tirando os anos de 2016, 2017)</t>
+  </si>
+  <si>
+    <t>Citado por 5, mas 3 de 2016 e 2 de 2017.</t>
+  </si>
+  <si>
+    <t>Dos 15 retornados, 2 eram em jap e rus</t>
+  </si>
+  <si>
+    <t>Citado por 4, mas 1 é de 2017.</t>
+  </si>
+  <si>
+    <t>Inclui 19 pela JF Tool, mas já existiam 2, total 21.</t>
+  </si>
+  <si>
+    <t>JF encontra 12, mas 4 estao em japones. Inclusao de 8, mas já existiam 3, total = 11.</t>
+  </si>
+  <si>
+    <t>erro na JF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Citado por 31, mas JF inclui 29 </t>
+  </si>
+  <si>
+    <t>Citado por 50, mas 4 não foram pegos.</t>
   </si>
 </sst>
 </file>
@@ -1814,7 +1890,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1950,6 +2026,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2402,7 +2484,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="236">
+  <cellXfs count="246">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2868,6 +2950,27 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3006,6 +3109,9 @@
     <xf numFmtId="0" fontId="1" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3024,8 +3130,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3037,8 +3149,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFCCCC"/>
       <color rgb="FFFF99FF"/>
-      <color rgb="FFFFCCCC"/>
       <color rgb="FFFF6699"/>
       <color rgb="FFFF3399"/>
       <color rgb="FFFF66FF"/>
@@ -3350,12 +3462,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="206411768"/>
-        <c:axId val="206408240"/>
+        <c:axId val="214768240"/>
+        <c:axId val="214762360"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="206411768"/>
+        <c:axId val="214768240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3447,7 +3559,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206408240"/>
+        <c:crossAx val="214762360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3455,7 +3567,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="206408240"/>
+        <c:axId val="214762360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3506,7 +3618,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206411768"/>
+        <c:crossAx val="214768240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3815,12 +3927,12 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:shape val="box"/>
-        <c:axId val="206409808"/>
-        <c:axId val="206410984"/>
+        <c:axId val="214762752"/>
+        <c:axId val="214766280"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="206409808"/>
+        <c:axId val="214762752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3909,7 +4021,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206410984"/>
+        <c:crossAx val="214766280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3917,7 +4029,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="206410984"/>
+        <c:axId val="214766280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4000,7 +4112,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206409808"/>
+        <c:crossAx val="214762752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4285,12 +4397,12 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:shape val="box"/>
-        <c:axId val="206409024"/>
-        <c:axId val="209227736"/>
+        <c:axId val="214765104"/>
+        <c:axId val="214765496"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="206409024"/>
+        <c:axId val="214765104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4379,7 +4491,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209227736"/>
+        <c:crossAx val="214765496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4387,7 +4499,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209227736"/>
+        <c:axId val="214765496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4470,7 +4582,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206409024"/>
+        <c:crossAx val="214765104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5257,12 +5369,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="209229304"/>
-        <c:axId val="209225776"/>
+        <c:axId val="214763928"/>
+        <c:axId val="214763144"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="209229304"/>
+        <c:axId val="214763928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5302,7 +5414,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209225776"/>
+        <c:crossAx val="214763144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5310,7 +5422,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209225776"/>
+        <c:axId val="214763144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5358,7 +5470,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209229304"/>
+        <c:crossAx val="214763928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5666,8 +5778,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="209226168"/>
-        <c:axId val="209226952"/>
+        <c:axId val="214764320"/>
+        <c:axId val="214768632"/>
         <c:axId val="0"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -5837,7 +5949,7 @@
         </c:extLst>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="209226168"/>
+        <c:axId val="214764320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5935,7 +6047,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209226952"/>
+        <c:crossAx val="214768632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5943,7 +6055,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209226952"/>
+        <c:axId val="214768632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6022,7 +6134,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="209226168"/>
+        <c:crossAx val="214764320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6336,8 +6448,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="209223424"/>
-        <c:axId val="209229696"/>
+        <c:axId val="214765888"/>
+        <c:axId val="216473200"/>
         <c:axId val="0"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -6507,7 +6619,7 @@
         </c:extLst>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="209223424"/>
+        <c:axId val="214765888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6605,7 +6717,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209229696"/>
+        <c:crossAx val="216473200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6613,7 +6725,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209229696"/>
+        <c:axId val="216473200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6692,7 +6804,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="209223424"/>
+        <c:crossAx val="214765888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10379,7 +10491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -10390,22 +10502,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="183" t="s">
+      <c r="A1" s="190" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="184"/>
+      <c r="B1" s="191"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="185" t="s">
+      <c r="A2" s="192" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="186"/>
+      <c r="B2" s="193"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="185" t="s">
+      <c r="A3" s="192" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="186"/>
+      <c r="B3" s="193"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -10440,10 +10552,10 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="187" t="s">
+      <c r="A8" s="194" t="s">
         <v>103</v>
       </c>
-      <c r="B8" s="188"/>
+      <c r="B8" s="195"/>
     </row>
     <row r="9" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
@@ -10509,6 +10621,35 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="236" t="s">
+        <v>525</v>
+      </c>
+      <c r="B1" s="236"/>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
+      <c r="G1" s="236"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K31"/>
   <sheetViews>
@@ -10533,19 +10674,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="205" t="s">
         <v>326</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
-      <c r="E1" s="198"/>
-      <c r="F1" s="198"/>
-      <c r="G1" s="198"/>
-      <c r="H1" s="198"/>
-      <c r="I1" s="198"/>
-      <c r="J1" s="198"/>
-      <c r="K1" s="198"/>
+      <c r="B1" s="205"/>
+      <c r="C1" s="205"/>
+      <c r="D1" s="205"/>
+      <c r="E1" s="205"/>
+      <c r="F1" s="205"/>
+      <c r="G1" s="205"/>
+      <c r="H1" s="205"/>
+      <c r="I1" s="205"/>
+      <c r="J1" s="205"/>
+      <c r="K1" s="205"/>
     </row>
     <row r="2" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
@@ -11252,7 +11393,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -11267,10 +11408,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="229" t="s">
+      <c r="A1" s="237" t="s">
         <v>333</v>
       </c>
-      <c r="B1" s="230"/>
+      <c r="B1" s="238"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="79" t="s">
@@ -11316,7 +11457,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L28"/>
   <sheetViews>
@@ -11338,20 +11479,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="231" t="s">
+      <c r="A1" s="239" t="s">
         <v>327</v>
       </c>
-      <c r="B1" s="231"/>
-      <c r="C1" s="231"/>
-      <c r="D1" s="231"/>
-      <c r="E1" s="231"/>
-      <c r="F1" s="231"/>
-      <c r="G1" s="231"/>
-      <c r="H1" s="231"/>
-      <c r="I1" s="231"/>
-      <c r="J1" s="231"/>
-      <c r="K1" s="231"/>
-      <c r="L1" s="231"/>
+      <c r="B1" s="239"/>
+      <c r="C1" s="239"/>
+      <c r="D1" s="239"/>
+      <c r="E1" s="239"/>
+      <c r="F1" s="239"/>
+      <c r="G1" s="239"/>
+      <c r="H1" s="239"/>
+      <c r="I1" s="239"/>
+      <c r="J1" s="239"/>
+      <c r="K1" s="239"/>
+      <c r="L1" s="239"/>
     </row>
     <row r="2" spans="1:12" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="142" t="s">
@@ -12070,15 +12211,15 @@
     </row>
     <row r="26" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="134"/>
-      <c r="B26" s="232" t="s">
+      <c r="B26" s="240" t="s">
         <v>334</v>
       </c>
-      <c r="C26" s="233"/>
-      <c r="D26" s="233"/>
-      <c r="E26" s="233"/>
-      <c r="F26" s="233"/>
-      <c r="G26" s="233"/>
-      <c r="H26" s="234"/>
+      <c r="C26" s="241"/>
+      <c r="D26" s="241"/>
+      <c r="E26" s="241"/>
+      <c r="F26" s="241"/>
+      <c r="G26" s="241"/>
+      <c r="H26" s="242"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="66"/>
@@ -12099,7 +12240,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
@@ -12244,10 +12385,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="193" t="s">
+      <c r="A1" s="200" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="194"/>
+      <c r="B1" s="201"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
@@ -12280,16 +12421,16 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="189" t="s">
+      <c r="A6" s="196" t="s">
         <v>147</v>
       </c>
-      <c r="B6" s="190"/>
+      <c r="B6" s="197"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="191" t="s">
+      <c r="A7" s="198" t="s">
         <v>150</v>
       </c>
-      <c r="B7" s="192"/>
+      <c r="B7" s="199"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -12371,16 +12512,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="195" t="s">
+      <c r="A1" s="202" t="s">
         <v>336</v>
       </c>
-      <c r="B1" s="196"/>
-      <c r="C1" s="196"/>
-      <c r="D1" s="196"/>
-      <c r="E1" s="196"/>
-      <c r="F1" s="196"/>
-      <c r="G1" s="196"/>
-      <c r="H1" s="197"/>
+      <c r="B1" s="203"/>
+      <c r="C1" s="203"/>
+      <c r="D1" s="203"/>
+      <c r="E1" s="203"/>
+      <c r="F1" s="203"/>
+      <c r="G1" s="203"/>
+      <c r="H1" s="204"/>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
     </row>
@@ -12735,8 +12876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12750,14 +12891,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="205" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
-      <c r="E1" s="198"/>
-      <c r="F1" s="198"/>
+      <c r="B1" s="205"/>
+      <c r="C1" s="205"/>
+      <c r="D1" s="205"/>
+      <c r="E1" s="205"/>
+      <c r="F1" s="205"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
@@ -13239,6 +13380,1555 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:L53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="62.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="7" width="18.85546875" style="81" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="81" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="3"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>474</v>
+      </c>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21" t="s">
+        <v>530</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>526</v>
+      </c>
+      <c r="J2" s="82" t="s">
+        <v>529</v>
+      </c>
+      <c r="K2" s="91"/>
+      <c r="L2" s="91"/>
+    </row>
+    <row r="3" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="188" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="131" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="132" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="48" t="s">
+        <v>502</v>
+      </c>
+      <c r="G3" s="48"/>
+      <c r="H3" s="184" t="s">
+        <v>346</v>
+      </c>
+      <c r="I3" s="94"/>
+      <c r="J3" s="94"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+    </row>
+    <row r="4" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="188" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="131" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="132">
+        <v>2007</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="F4" s="48" t="s">
+        <v>209</v>
+      </c>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J4" s="94"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="91"/>
+    </row>
+    <row r="5" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="188" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="132">
+        <v>2008</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="F5" s="48" t="s">
+        <v>210</v>
+      </c>
+      <c r="G5" s="48"/>
+      <c r="H5" s="184" t="s">
+        <v>346</v>
+      </c>
+      <c r="I5" s="94"/>
+      <c r="J5" s="187" t="s">
+        <v>346</v>
+      </c>
+      <c r="K5" s="183" t="s">
+        <v>528</v>
+      </c>
+      <c r="L5" s="91"/>
+    </row>
+    <row r="6" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="189" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="132">
+        <v>2015</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="F6" s="48" t="s">
+        <v>511</v>
+      </c>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J6" s="94"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="91"/>
+    </row>
+    <row r="7" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="188" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="131" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="132">
+        <v>2011</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="F7" s="48" t="s">
+        <v>211</v>
+      </c>
+      <c r="G7" s="48"/>
+      <c r="H7" s="184" t="s">
+        <v>346</v>
+      </c>
+      <c r="I7" s="94"/>
+      <c r="J7" s="94"/>
+      <c r="K7" s="91"/>
+      <c r="L7" s="91"/>
+    </row>
+    <row r="8" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="188" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="132">
+        <v>2010</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="F8" s="48" t="s">
+        <v>512</v>
+      </c>
+      <c r="G8" s="48"/>
+      <c r="H8" s="184" t="s">
+        <v>346</v>
+      </c>
+      <c r="I8" s="94"/>
+      <c r="J8" s="94"/>
+      <c r="K8" s="91"/>
+      <c r="L8" s="91"/>
+    </row>
+    <row r="9" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="188" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="D9" s="132">
+        <v>2009</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="F9" s="48" t="s">
+        <v>513</v>
+      </c>
+      <c r="G9" s="48"/>
+      <c r="H9" s="184" t="s">
+        <v>346</v>
+      </c>
+      <c r="I9" s="94"/>
+      <c r="J9" s="94"/>
+      <c r="K9" s="91"/>
+      <c r="L9" s="91"/>
+    </row>
+    <row r="10" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="189" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="131" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="132">
+        <v>2010</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="F10" s="48" t="s">
+        <v>212</v>
+      </c>
+      <c r="G10" s="48"/>
+      <c r="H10" s="184" t="s">
+        <v>346</v>
+      </c>
+      <c r="I10" s="94"/>
+      <c r="J10" s="94"/>
+      <c r="K10" s="91"/>
+      <c r="L10" s="91"/>
+    </row>
+    <row r="11" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="188" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="131" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="132">
+        <v>2010</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="F11" s="48" t="s">
+        <v>514</v>
+      </c>
+      <c r="G11" s="48"/>
+      <c r="H11" s="184" t="s">
+        <v>346</v>
+      </c>
+      <c r="I11" s="94"/>
+      <c r="J11" s="94"/>
+      <c r="K11" s="91"/>
+      <c r="L11" s="91"/>
+    </row>
+    <row r="12" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="188" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="131" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="132">
+        <v>1999</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="48" t="s">
+        <v>515</v>
+      </c>
+      <c r="G12" s="48"/>
+      <c r="H12" s="184" t="s">
+        <v>346</v>
+      </c>
+      <c r="I12" s="94"/>
+      <c r="J12" s="94"/>
+      <c r="K12" s="91"/>
+      <c r="L12" s="91"/>
+    </row>
+    <row r="13" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="188" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="132">
+        <v>2005</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="F13" s="48" t="s">
+        <v>516</v>
+      </c>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J13" s="94"/>
+      <c r="K13" s="91"/>
+      <c r="L13" s="91"/>
+    </row>
+    <row r="14" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="188" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="131" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="132">
+        <v>2008</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="F14" s="48" t="s">
+        <v>213</v>
+      </c>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J14" s="94"/>
+      <c r="K14" s="91"/>
+      <c r="L14" s="91"/>
+    </row>
+    <row r="15" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="188" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="132">
+        <v>2011</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="F15" s="48" t="s">
+        <v>517</v>
+      </c>
+      <c r="G15" s="48"/>
+      <c r="H15" s="184" t="s">
+        <v>346</v>
+      </c>
+      <c r="I15" s="94"/>
+      <c r="J15" s="94"/>
+      <c r="K15" s="91"/>
+      <c r="L15" s="91"/>
+    </row>
+    <row r="16" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="188" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="132">
+        <v>2009</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="F16" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="G16" s="48"/>
+      <c r="H16" s="184" t="s">
+        <v>346</v>
+      </c>
+      <c r="I16" s="94"/>
+      <c r="J16" s="94"/>
+      <c r="K16" s="91"/>
+      <c r="L16" s="91"/>
+    </row>
+    <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="188" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="131" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="132">
+        <v>1997</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="F17" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="G17" s="48"/>
+      <c r="H17" s="184" t="s">
+        <v>346</v>
+      </c>
+      <c r="I17" s="94"/>
+      <c r="J17" s="94"/>
+      <c r="K17" s="91"/>
+      <c r="L17" s="91"/>
+    </row>
+    <row r="18" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="188" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="132">
+        <v>2010</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="F18" s="48" t="s">
+        <v>518</v>
+      </c>
+      <c r="G18" s="48"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J18" s="94"/>
+      <c r="K18" s="91"/>
+      <c r="L18" s="91"/>
+    </row>
+    <row r="19" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="189" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="131" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="132">
+        <v>2005</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="F19" s="48" t="s">
+        <v>519</v>
+      </c>
+      <c r="G19" s="48"/>
+      <c r="H19" s="184" t="s">
+        <v>346</v>
+      </c>
+      <c r="I19" s="94"/>
+      <c r="J19" s="94"/>
+      <c r="K19" s="91"/>
+      <c r="L19" s="91"/>
+    </row>
+    <row r="20" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="189" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="132">
+        <v>2011</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F20" s="48" t="s">
+        <v>520</v>
+      </c>
+      <c r="G20" s="48"/>
+      <c r="H20" s="184" t="s">
+        <v>346</v>
+      </c>
+      <c r="I20" s="94"/>
+      <c r="J20" s="94"/>
+      <c r="K20" s="91"/>
+      <c r="L20" s="91"/>
+    </row>
+    <row r="21" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="189" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" s="132">
+        <v>2008</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="F21" s="48" t="s">
+        <v>521</v>
+      </c>
+      <c r="G21" s="48"/>
+      <c r="H21" s="184" t="s">
+        <v>346</v>
+      </c>
+      <c r="I21" s="94"/>
+      <c r="J21" s="94"/>
+      <c r="K21" s="91"/>
+      <c r="L21" s="91"/>
+    </row>
+    <row r="22" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="189" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" s="132">
+        <v>2015</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="F22" s="48" t="s">
+        <v>522</v>
+      </c>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J22" s="94"/>
+      <c r="K22" s="91"/>
+      <c r="L22" s="91"/>
+    </row>
+    <row r="23" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="189" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="132">
+        <v>2000</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="F23" s="48" t="s">
+        <v>523</v>
+      </c>
+      <c r="G23" s="48"/>
+      <c r="H23" s="184" t="s">
+        <v>346</v>
+      </c>
+      <c r="I23" s="94"/>
+      <c r="J23" s="94"/>
+      <c r="K23" s="91"/>
+      <c r="L23" s="91"/>
+    </row>
+    <row r="24" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="189" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="132">
+        <v>2010</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="F24" s="48" t="s">
+        <v>524</v>
+      </c>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J24" s="94"/>
+      <c r="K24" s="91"/>
+      <c r="L24" s="91"/>
+    </row>
+    <row r="25" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="53" t="s">
+        <v>359</v>
+      </c>
+      <c r="B25" s="176" t="s">
+        <v>399</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>358</v>
+      </c>
+      <c r="D25" s="18">
+        <v>1999</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="F25" s="244" t="s">
+        <v>501</v>
+      </c>
+      <c r="G25" s="29"/>
+      <c r="H25" s="85"/>
+      <c r="I25" s="85"/>
+      <c r="J25" s="74" t="s">
+        <v>346</v>
+      </c>
+      <c r="K25" s="91" t="s">
+        <v>531</v>
+      </c>
+      <c r="L25" s="91"/>
+    </row>
+    <row r="26" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="53" t="s">
+        <v>360</v>
+      </c>
+      <c r="B26" s="176" t="s">
+        <v>363</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>362</v>
+      </c>
+      <c r="D26" s="18">
+        <v>2010</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>361</v>
+      </c>
+      <c r="F26" s="243" t="s">
+        <v>470</v>
+      </c>
+      <c r="G26" s="53" t="s">
+        <v>532</v>
+      </c>
+      <c r="H26" s="53"/>
+      <c r="I26" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J26" s="94"/>
+      <c r="K26" s="91"/>
+      <c r="L26" s="91"/>
+    </row>
+    <row r="27" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="53" t="s">
+        <v>364</v>
+      </c>
+      <c r="B27" s="176" t="s">
+        <v>367</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="D27" s="18">
+        <v>2014</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>365</v>
+      </c>
+      <c r="F27" s="244" t="s">
+        <v>471</v>
+      </c>
+      <c r="G27" s="89" t="s">
+        <v>533</v>
+      </c>
+      <c r="H27" s="85"/>
+      <c r="I27" s="85"/>
+      <c r="J27" s="74" t="s">
+        <v>346</v>
+      </c>
+      <c r="K27" s="91" t="s">
+        <v>531</v>
+      </c>
+      <c r="L27" s="91"/>
+    </row>
+    <row r="28" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="53" t="s">
+        <v>368</v>
+      </c>
+      <c r="B28" s="176" t="s">
+        <v>370</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>371</v>
+      </c>
+      <c r="D28" s="18">
+        <v>2014</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>369</v>
+      </c>
+      <c r="F28" s="243" t="s">
+        <v>472</v>
+      </c>
+      <c r="G28" s="53" t="s">
+        <v>534</v>
+      </c>
+      <c r="H28" s="53"/>
+      <c r="I28" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J28" s="94"/>
+      <c r="K28" s="91"/>
+      <c r="L28" s="91"/>
+    </row>
+    <row r="29" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="53" t="s">
+        <v>372</v>
+      </c>
+      <c r="B29" s="176" t="s">
+        <v>374</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>375</v>
+      </c>
+      <c r="D29" s="18">
+        <v>2002</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>373</v>
+      </c>
+      <c r="F29" s="244" t="s">
+        <v>476</v>
+      </c>
+      <c r="G29" s="29" t="s">
+        <v>549</v>
+      </c>
+      <c r="H29" s="185" t="s">
+        <v>346</v>
+      </c>
+      <c r="I29" s="94"/>
+      <c r="J29" s="94"/>
+      <c r="K29" s="91"/>
+      <c r="L29" s="91"/>
+    </row>
+    <row r="30" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="53" t="s">
+        <v>378</v>
+      </c>
+      <c r="B30" s="176" t="s">
+        <v>478</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>377</v>
+      </c>
+      <c r="D30" s="18">
+        <v>2013</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>376</v>
+      </c>
+      <c r="F30" s="244" t="s">
+        <v>477</v>
+      </c>
+      <c r="G30" s="94" t="s">
+        <v>535</v>
+      </c>
+      <c r="H30" s="94"/>
+      <c r="I30" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J30" s="94"/>
+      <c r="K30" s="91"/>
+      <c r="L30" s="91"/>
+    </row>
+    <row r="31" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="53" t="s">
+        <v>379</v>
+      </c>
+      <c r="B31" s="176" t="s">
+        <v>382</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>381</v>
+      </c>
+      <c r="D31" s="18">
+        <v>1995</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>380</v>
+      </c>
+      <c r="F31" s="244" t="s">
+        <v>500</v>
+      </c>
+      <c r="G31" s="29" t="s">
+        <v>536</v>
+      </c>
+      <c r="H31" s="29"/>
+      <c r="I31" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J31" s="94"/>
+      <c r="K31" s="91"/>
+      <c r="L31" s="91"/>
+    </row>
+    <row r="32" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="53" t="s">
+        <v>383</v>
+      </c>
+      <c r="B32" s="176" t="s">
+        <v>385</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>386</v>
+      </c>
+      <c r="D32" s="18">
+        <v>2010</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>384</v>
+      </c>
+      <c r="F32" s="244" t="s">
+        <v>479</v>
+      </c>
+      <c r="G32" s="29" t="s">
+        <v>550</v>
+      </c>
+      <c r="H32" s="185" t="s">
+        <v>346</v>
+      </c>
+      <c r="I32" s="94"/>
+      <c r="J32" s="94"/>
+      <c r="K32" s="91"/>
+      <c r="L32" s="91"/>
+    </row>
+    <row r="33" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="53" t="s">
+        <v>387</v>
+      </c>
+      <c r="B33" s="176" t="s">
+        <v>390</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>389</v>
+      </c>
+      <c r="D33" s="18">
+        <v>2010</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>388</v>
+      </c>
+      <c r="F33" s="244" t="s">
+        <v>480</v>
+      </c>
+      <c r="G33" s="29" t="s">
+        <v>538</v>
+      </c>
+      <c r="H33" s="185" t="s">
+        <v>346</v>
+      </c>
+      <c r="I33" s="94"/>
+      <c r="J33" s="94"/>
+      <c r="K33" s="91"/>
+      <c r="L33" s="91"/>
+    </row>
+    <row r="34" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="53" t="s">
+        <v>391</v>
+      </c>
+      <c r="B34" s="176" t="s">
+        <v>393</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>394</v>
+      </c>
+      <c r="D34" s="18">
+        <v>2000</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>392</v>
+      </c>
+      <c r="F34" s="244" t="s">
+        <v>499</v>
+      </c>
+      <c r="G34" s="29" t="s">
+        <v>537</v>
+      </c>
+      <c r="H34" s="185" t="s">
+        <v>346</v>
+      </c>
+      <c r="I34" s="94"/>
+      <c r="J34" s="186" t="s">
+        <v>346</v>
+      </c>
+      <c r="K34" s="183" t="s">
+        <v>528</v>
+      </c>
+      <c r="L34" s="91"/>
+    </row>
+    <row r="35" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="53" t="s">
+        <v>395</v>
+      </c>
+      <c r="B35" s="176" t="s">
+        <v>398</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>397</v>
+      </c>
+      <c r="D35" s="18">
+        <v>2014</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>396</v>
+      </c>
+      <c r="F35" s="244" t="s">
+        <v>481</v>
+      </c>
+      <c r="G35" s="94" t="s">
+        <v>539</v>
+      </c>
+      <c r="H35" s="94"/>
+      <c r="I35" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J35" s="94"/>
+      <c r="K35" s="91"/>
+      <c r="L35" s="91"/>
+    </row>
+    <row r="36" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="53" t="s">
+        <v>400</v>
+      </c>
+      <c r="B36" s="176" t="s">
+        <v>402</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>403</v>
+      </c>
+      <c r="D36" s="18">
+        <v>2010</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>401</v>
+      </c>
+      <c r="F36" s="244" t="s">
+        <v>482</v>
+      </c>
+      <c r="G36" s="94" t="s">
+        <v>540</v>
+      </c>
+      <c r="H36" s="185" t="s">
+        <v>346</v>
+      </c>
+      <c r="I36" s="94"/>
+      <c r="J36" s="94"/>
+      <c r="K36" s="91"/>
+      <c r="L36" s="91"/>
+    </row>
+    <row r="37" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="53" t="s">
+        <v>404</v>
+      </c>
+      <c r="B37" s="176" t="s">
+        <v>406</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>405</v>
+      </c>
+      <c r="D37" s="18">
+        <v>2010</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>401</v>
+      </c>
+      <c r="F37" s="85" t="s">
+        <v>483</v>
+      </c>
+      <c r="G37" s="94" t="s">
+        <v>548</v>
+      </c>
+      <c r="H37" s="185" t="s">
+        <v>346</v>
+      </c>
+      <c r="I37" s="94"/>
+      <c r="J37" s="94"/>
+      <c r="K37" s="91"/>
+      <c r="L37" s="91"/>
+    </row>
+    <row r="38" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="53" t="s">
+        <v>407</v>
+      </c>
+      <c r="B38" s="176" t="s">
+        <v>409</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>410</v>
+      </c>
+      <c r="D38" s="18">
+        <v>2005</v>
+      </c>
+      <c r="E38" s="18" t="s">
+        <v>408</v>
+      </c>
+      <c r="F38" s="244" t="s">
+        <v>484</v>
+      </c>
+      <c r="G38" s="94" t="s">
+        <v>547</v>
+      </c>
+      <c r="H38" s="185" t="s">
+        <v>346</v>
+      </c>
+      <c r="I38" s="94"/>
+      <c r="J38" s="94"/>
+      <c r="K38" s="91"/>
+      <c r="L38" s="91"/>
+    </row>
+    <row r="39" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="53" t="s">
+        <v>411</v>
+      </c>
+      <c r="B39" s="176" t="s">
+        <v>413</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>414</v>
+      </c>
+      <c r="D39" s="18">
+        <v>1998</v>
+      </c>
+      <c r="E39" s="18" t="s">
+        <v>412</v>
+      </c>
+      <c r="F39" s="29" t="s">
+        <v>498</v>
+      </c>
+      <c r="G39" s="29"/>
+      <c r="H39" s="185" t="s">
+        <v>346</v>
+      </c>
+      <c r="I39" s="94"/>
+      <c r="J39" s="94"/>
+      <c r="K39" s="91"/>
+      <c r="L39" s="91"/>
+    </row>
+    <row r="40" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="53" t="s">
+        <v>415</v>
+      </c>
+      <c r="B40" s="176" t="s">
+        <v>419</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>416</v>
+      </c>
+      <c r="D40" s="18">
+        <v>2007</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>420</v>
+      </c>
+      <c r="F40" s="94" t="s">
+        <v>485</v>
+      </c>
+      <c r="G40" s="94"/>
+      <c r="H40" s="185" t="s">
+        <v>346</v>
+      </c>
+      <c r="I40" s="94"/>
+      <c r="J40" s="94"/>
+      <c r="K40" s="91"/>
+      <c r="L40" s="91"/>
+    </row>
+    <row r="41" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="53" t="s">
+        <v>417</v>
+      </c>
+      <c r="B41" s="176" t="s">
+        <v>421</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>422</v>
+      </c>
+      <c r="D41" s="18">
+        <v>2014</v>
+      </c>
+      <c r="E41" s="18" t="s">
+        <v>418</v>
+      </c>
+      <c r="F41" s="244" t="s">
+        <v>497</v>
+      </c>
+      <c r="G41" s="29" t="s">
+        <v>541</v>
+      </c>
+      <c r="H41" s="185" t="s">
+        <v>346</v>
+      </c>
+      <c r="I41" s="94"/>
+      <c r="J41" s="186" t="s">
+        <v>346</v>
+      </c>
+      <c r="K41" s="183" t="s">
+        <v>527</v>
+      </c>
+      <c r="L41" s="91"/>
+    </row>
+    <row r="42" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="53" t="s">
+        <v>423</v>
+      </c>
+      <c r="B42" s="176" t="s">
+        <v>466</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>425</v>
+      </c>
+      <c r="D42" s="18">
+        <v>2013</v>
+      </c>
+      <c r="E42" s="18" t="s">
+        <v>424</v>
+      </c>
+      <c r="F42" s="244" t="s">
+        <v>506</v>
+      </c>
+      <c r="G42" s="94" t="s">
+        <v>542</v>
+      </c>
+      <c r="H42" s="185" t="s">
+        <v>346</v>
+      </c>
+      <c r="I42" s="94"/>
+      <c r="J42" s="94"/>
+      <c r="K42" s="91"/>
+      <c r="L42" s="91"/>
+    </row>
+    <row r="43" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="53" t="s">
+        <v>426</v>
+      </c>
+      <c r="B43" s="176" t="s">
+        <v>428</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>427</v>
+      </c>
+      <c r="D43" s="18">
+        <v>2013</v>
+      </c>
+      <c r="E43" s="18" t="s">
+        <v>424</v>
+      </c>
+      <c r="F43" s="245" t="s">
+        <v>496</v>
+      </c>
+      <c r="G43" s="98" t="s">
+        <v>543</v>
+      </c>
+      <c r="H43" s="98"/>
+      <c r="I43" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J43" s="94"/>
+      <c r="K43" s="91"/>
+      <c r="L43" s="91"/>
+    </row>
+    <row r="44" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="53" t="s">
+        <v>429</v>
+      </c>
+      <c r="B44" s="176" t="s">
+        <v>431</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>432</v>
+      </c>
+      <c r="D44" s="18">
+        <v>2007</v>
+      </c>
+      <c r="E44" s="18" t="s">
+        <v>430</v>
+      </c>
+      <c r="F44" s="94" t="s">
+        <v>486</v>
+      </c>
+      <c r="G44" s="94"/>
+      <c r="H44" s="185" t="s">
+        <v>346</v>
+      </c>
+      <c r="I44" s="94"/>
+      <c r="J44" s="94"/>
+      <c r="K44" s="91"/>
+      <c r="L44" s="91"/>
+    </row>
+    <row r="45" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="53" t="s">
+        <v>433</v>
+      </c>
+      <c r="B45" s="176" t="s">
+        <v>436</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>435</v>
+      </c>
+      <c r="D45" s="18">
+        <v>2011</v>
+      </c>
+      <c r="E45" s="18" t="s">
+        <v>434</v>
+      </c>
+      <c r="F45" s="244" t="s">
+        <v>487</v>
+      </c>
+      <c r="G45" s="94" t="s">
+        <v>544</v>
+      </c>
+      <c r="H45" s="94"/>
+      <c r="I45" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J45" s="94"/>
+      <c r="K45" s="91"/>
+      <c r="L45" s="91"/>
+    </row>
+    <row r="46" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="53" t="s">
+        <v>437</v>
+      </c>
+      <c r="B46" s="176" t="s">
+        <v>439</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>468</v>
+      </c>
+      <c r="D46" s="18">
+        <v>2007</v>
+      </c>
+      <c r="E46" s="18" t="s">
+        <v>438</v>
+      </c>
+      <c r="F46" s="29" t="s">
+        <v>495</v>
+      </c>
+      <c r="G46" s="29"/>
+      <c r="H46" s="29"/>
+      <c r="I46" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J46" s="94"/>
+      <c r="K46" s="91"/>
+      <c r="L46" s="91"/>
+    </row>
+    <row r="47" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="53" t="s">
+        <v>440</v>
+      </c>
+      <c r="B47" s="176" t="s">
+        <v>442</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>443</v>
+      </c>
+      <c r="D47" s="18">
+        <v>2010</v>
+      </c>
+      <c r="E47" s="18" t="s">
+        <v>441</v>
+      </c>
+      <c r="F47" s="244" t="s">
+        <v>494</v>
+      </c>
+      <c r="G47" s="29" t="s">
+        <v>535</v>
+      </c>
+      <c r="H47" s="29"/>
+      <c r="I47" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J47" s="94"/>
+      <c r="K47" s="91"/>
+      <c r="L47" s="91"/>
+    </row>
+    <row r="48" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="53" t="s">
+        <v>444</v>
+      </c>
+      <c r="B48" s="176" t="s">
+        <v>445</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>446</v>
+      </c>
+      <c r="D48" s="18">
+        <v>2006</v>
+      </c>
+      <c r="E48" s="18" t="s">
+        <v>408</v>
+      </c>
+      <c r="F48" s="85" t="s">
+        <v>488</v>
+      </c>
+      <c r="G48" s="94" t="s">
+        <v>548</v>
+      </c>
+      <c r="H48" s="85"/>
+      <c r="I48" s="85"/>
+      <c r="J48" s="53" t="s">
+        <v>346</v>
+      </c>
+      <c r="K48" s="91" t="s">
+        <v>531</v>
+      </c>
+      <c r="L48" s="91"/>
+    </row>
+    <row r="49" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="53" t="s">
+        <v>447</v>
+      </c>
+      <c r="B49" s="176" t="s">
+        <v>450</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>449</v>
+      </c>
+      <c r="D49" s="18">
+        <v>2011</v>
+      </c>
+      <c r="E49" s="18" t="s">
+        <v>448</v>
+      </c>
+      <c r="F49" s="244" t="s">
+        <v>489</v>
+      </c>
+      <c r="G49" s="29" t="s">
+        <v>545</v>
+      </c>
+      <c r="H49" s="29"/>
+      <c r="I49" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J49" s="94"/>
+      <c r="K49" s="91"/>
+      <c r="L49" s="91"/>
+    </row>
+    <row r="50" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="53" t="s">
+        <v>451</v>
+      </c>
+      <c r="B50" s="176" t="s">
+        <v>467</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>456</v>
+      </c>
+      <c r="D50" s="18">
+        <v>2004</v>
+      </c>
+      <c r="E50" s="18" t="s">
+        <v>455</v>
+      </c>
+      <c r="F50" s="244" t="s">
+        <v>490</v>
+      </c>
+      <c r="G50" s="29" t="s">
+        <v>536</v>
+      </c>
+      <c r="H50" s="185" t="s">
+        <v>346</v>
+      </c>
+      <c r="I50" s="94"/>
+      <c r="J50" s="94"/>
+      <c r="K50" s="91"/>
+      <c r="L50" s="91"/>
+    </row>
+    <row r="51" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="53" t="s">
+        <v>452</v>
+      </c>
+      <c r="B51" s="176" t="s">
+        <v>458</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>459</v>
+      </c>
+      <c r="D51" s="18">
+        <v>2010</v>
+      </c>
+      <c r="E51" s="18" t="s">
+        <v>457</v>
+      </c>
+      <c r="F51" s="244" t="s">
+        <v>493</v>
+      </c>
+      <c r="G51" s="29"/>
+      <c r="H51" s="185" t="s">
+        <v>346</v>
+      </c>
+      <c r="I51" s="94"/>
+      <c r="J51" s="94"/>
+      <c r="K51" s="91"/>
+      <c r="L51" s="91"/>
+    </row>
+    <row r="52" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="53" t="s">
+        <v>453</v>
+      </c>
+      <c r="B52" s="176" t="s">
+        <v>462</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>461</v>
+      </c>
+      <c r="D52" s="18">
+        <v>2003</v>
+      </c>
+      <c r="E52" s="18" t="s">
+        <v>460</v>
+      </c>
+      <c r="F52" s="244" t="s">
+        <v>491</v>
+      </c>
+      <c r="G52" s="29" t="s">
+        <v>546</v>
+      </c>
+      <c r="H52" s="29"/>
+      <c r="I52" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J52" s="94"/>
+      <c r="K52" s="91"/>
+      <c r="L52" s="91"/>
+    </row>
+    <row r="53" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="53" t="s">
+        <v>454</v>
+      </c>
+      <c r="B53" s="176" t="s">
+        <v>463</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>469</v>
+      </c>
+      <c r="D53" s="18">
+        <v>2007</v>
+      </c>
+      <c r="E53" s="18" t="s">
+        <v>420</v>
+      </c>
+      <c r="F53" s="29" t="s">
+        <v>492</v>
+      </c>
+      <c r="G53" s="29"/>
+      <c r="H53" s="185" t="s">
+        <v>346</v>
+      </c>
+      <c r="I53" s="94"/>
+      <c r="J53" s="94"/>
+      <c r="K53" s="91"/>
+      <c r="L53" s="91"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S54"/>
   <sheetViews>
@@ -13258,43 +14948,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="208" t="s">
+      <c r="A1" s="215" t="s">
         <v>230</v>
       </c>
-      <c r="B1" s="209"/>
-      <c r="C1" s="209"/>
-      <c r="D1" s="209"/>
-      <c r="E1" s="209"/>
-      <c r="F1" s="209"/>
-      <c r="G1" s="209"/>
-      <c r="H1" s="209"/>
-      <c r="I1" s="209"/>
+      <c r="B1" s="216"/>
+      <c r="C1" s="216"/>
+      <c r="D1" s="216"/>
+      <c r="E1" s="216"/>
+      <c r="F1" s="216"/>
+      <c r="G1" s="216"/>
+      <c r="H1" s="216"/>
+      <c r="I1" s="216"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="207" t="s">
+      <c r="A2" s="214" t="s">
         <v>229</v>
       </c>
-      <c r="B2" s="207"/>
-      <c r="C2" s="207"/>
-      <c r="D2" s="207"/>
-      <c r="E2" s="207"/>
-      <c r="F2" s="207"/>
-      <c r="G2" s="207"/>
-      <c r="H2" s="207"/>
-      <c r="I2" s="207"/>
+      <c r="B2" s="214"/>
+      <c r="C2" s="214"/>
+      <c r="D2" s="214"/>
+      <c r="E2" s="214"/>
+      <c r="F2" s="214"/>
+      <c r="G2" s="214"/>
+      <c r="H2" s="214"/>
+      <c r="I2" s="214"/>
     </row>
     <row r="3" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="200" t="s">
+      <c r="A3" s="207" t="s">
         <v>337</v>
       </c>
-      <c r="B3" s="200"/>
-      <c r="C3" s="200"/>
-      <c r="D3" s="200"/>
-      <c r="E3" s="200"/>
-      <c r="F3" s="200"/>
-      <c r="G3" s="200"/>
-      <c r="H3" s="200"/>
-      <c r="I3" s="200"/>
+      <c r="B3" s="207"/>
+      <c r="C3" s="207"/>
+      <c r="D3" s="207"/>
+      <c r="E3" s="207"/>
+      <c r="F3" s="207"/>
+      <c r="G3" s="207"/>
+      <c r="H3" s="207"/>
+      <c r="I3" s="207"/>
       <c r="J3" s="71"/>
       <c r="K3" s="71"/>
       <c r="L3" s="71"/>
@@ -13307,12 +14997,12 @@
       <c r="S3" s="71"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="210" t="s">
+      <c r="A4" s="217" t="s">
         <v>253</v>
       </c>
-      <c r="B4" s="210"/>
-      <c r="C4" s="210"/>
-      <c r="D4" s="210"/>
+      <c r="B4" s="217"/>
+      <c r="C4" s="217"/>
+      <c r="D4" s="217"/>
     </row>
     <row r="5" spans="1:19" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="69" t="s">
@@ -13338,7 +15028,7 @@
       <c r="C6" s="49" t="s">
         <v>196</v>
       </c>
-      <c r="D6" s="204" t="s">
+      <c r="D6" s="211" t="s">
         <v>339</v>
       </c>
       <c r="E6" t="e">
@@ -13357,7 +15047,7 @@
       <c r="C7" s="49" t="s">
         <v>228</v>
       </c>
-      <c r="D7" s="205"/>
+      <c r="D7" s="212"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="78" t="s">
@@ -13369,7 +15059,7 @@
       <c r="C8" s="49" t="s">
         <v>235</v>
       </c>
-      <c r="D8" s="205"/>
+      <c r="D8" s="212"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="78" t="s">
@@ -13381,7 +15071,7 @@
       <c r="C9" s="49" t="s">
         <v>236</v>
       </c>
-      <c r="D9" s="205"/>
+      <c r="D9" s="212"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="78" t="s">
@@ -13393,7 +15083,7 @@
       <c r="C10" s="49" t="s">
         <v>237</v>
       </c>
-      <c r="D10" s="205"/>
+      <c r="D10" s="212"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="78" t="s">
@@ -13405,7 +15095,7 @@
       <c r="C11" s="49" t="s">
         <v>237</v>
       </c>
-      <c r="D11" s="205"/>
+      <c r="D11" s="212"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="78" t="s">
@@ -13417,7 +15107,7 @@
       <c r="C12" s="49" t="s">
         <v>266</v>
       </c>
-      <c r="D12" s="205"/>
+      <c r="D12" s="212"/>
     </row>
     <row r="13" spans="1:19" s="77" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="145" t="s">
@@ -13429,7 +15119,7 @@
       <c r="C13" s="136" t="s">
         <v>273</v>
       </c>
-      <c r="D13" s="206"/>
+      <c r="D13" s="213"/>
     </row>
     <row r="14" spans="1:19" s="77" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="146" t="s">
@@ -13446,30 +15136,30 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="207" t="s">
+      <c r="A15" s="214" t="s">
         <v>261</v>
       </c>
-      <c r="B15" s="207"/>
-      <c r="C15" s="207"/>
-      <c r="D15" s="207"/>
-      <c r="E15" s="207"/>
-      <c r="F15" s="207"/>
-      <c r="G15" s="207"/>
-      <c r="H15" s="207"/>
-      <c r="I15" s="207"/>
+      <c r="B15" s="214"/>
+      <c r="C15" s="214"/>
+      <c r="D15" s="214"/>
+      <c r="E15" s="214"/>
+      <c r="F15" s="214"/>
+      <c r="G15" s="214"/>
+      <c r="H15" s="214"/>
+      <c r="I15" s="214"/>
     </row>
     <row r="16" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="200" t="s">
+      <c r="A16" s="207" t="s">
         <v>238</v>
       </c>
-      <c r="B16" s="200"/>
-      <c r="C16" s="200"/>
-      <c r="D16" s="200"/>
-      <c r="E16" s="200"/>
-      <c r="F16" s="200"/>
-      <c r="G16" s="200"/>
-      <c r="H16" s="200"/>
-      <c r="I16" s="200"/>
+      <c r="B16" s="207"/>
+      <c r="C16" s="207"/>
+      <c r="D16" s="207"/>
+      <c r="E16" s="207"/>
+      <c r="F16" s="207"/>
+      <c r="G16" s="207"/>
+      <c r="H16" s="207"/>
+      <c r="I16" s="207"/>
       <c r="J16" s="71"/>
       <c r="K16" s="71"/>
       <c r="L16" s="71"/>
@@ -13482,14 +15172,14 @@
       <c r="S16" s="71"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="210" t="s">
+      <c r="A17" s="217" t="s">
         <v>259</v>
       </c>
-      <c r="B17" s="210"/>
-      <c r="C17" s="210"/>
-      <c r="D17" s="210"/>
-      <c r="E17" s="210"/>
-      <c r="F17" s="210"/>
+      <c r="B17" s="217"/>
+      <c r="C17" s="217"/>
+      <c r="D17" s="217"/>
+      <c r="E17" s="217"/>
+      <c r="F17" s="217"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="69" t="s">
@@ -13656,30 +15346,30 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="207" t="s">
+      <c r="A25" s="214" t="s">
         <v>260</v>
       </c>
-      <c r="B25" s="207"/>
-      <c r="C25" s="207"/>
-      <c r="D25" s="207"/>
-      <c r="E25" s="207"/>
-      <c r="F25" s="207"/>
-      <c r="G25" s="207"/>
-      <c r="H25" s="207"/>
-      <c r="I25" s="207"/>
+      <c r="B25" s="214"/>
+      <c r="C25" s="214"/>
+      <c r="D25" s="214"/>
+      <c r="E25" s="214"/>
+      <c r="F25" s="214"/>
+      <c r="G25" s="214"/>
+      <c r="H25" s="214"/>
+      <c r="I25" s="214"/>
     </row>
     <row r="26" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="200" t="s">
+      <c r="A26" s="207" t="s">
         <v>338</v>
       </c>
-      <c r="B26" s="200"/>
-      <c r="C26" s="200"/>
-      <c r="D26" s="200"/>
-      <c r="E26" s="200"/>
-      <c r="F26" s="200"/>
-      <c r="G26" s="200"/>
-      <c r="H26" s="200"/>
-      <c r="I26" s="200"/>
+      <c r="B26" s="207"/>
+      <c r="C26" s="207"/>
+      <c r="D26" s="207"/>
+      <c r="E26" s="207"/>
+      <c r="F26" s="207"/>
+      <c r="G26" s="207"/>
+      <c r="H26" s="207"/>
+      <c r="I26" s="207"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="69" t="s">
@@ -13691,12 +15381,12 @@
       <c r="C27" s="69" t="s">
         <v>201</v>
       </c>
-      <c r="D27" s="214" t="s">
+      <c r="D27" s="221" t="s">
         <v>292</v>
       </c>
-      <c r="E27" s="214"/>
-      <c r="F27" s="214"/>
-      <c r="G27" s="214"/>
+      <c r="E27" s="221"/>
+      <c r="F27" s="221"/>
+      <c r="G27" s="221"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="52" t="s">
@@ -13708,12 +15398,12 @@
       <c r="C28" s="72">
         <v>0.59</v>
       </c>
-      <c r="D28" s="201" t="s">
+      <c r="D28" s="208" t="s">
         <v>285</v>
       </c>
-      <c r="E28" s="202"/>
-      <c r="F28" s="202"/>
-      <c r="G28" s="203"/>
+      <c r="E28" s="209"/>
+      <c r="F28" s="209"/>
+      <c r="G28" s="210"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="52" t="s">
@@ -13725,12 +15415,12 @@
       <c r="C29" s="72">
         <v>0.77</v>
       </c>
-      <c r="D29" s="211" t="s">
+      <c r="D29" s="218" t="s">
         <v>286</v>
       </c>
-      <c r="E29" s="212"/>
-      <c r="F29" s="212"/>
-      <c r="G29" s="213"/>
+      <c r="E29" s="219"/>
+      <c r="F29" s="219"/>
+      <c r="G29" s="220"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="52" t="s">
@@ -13742,12 +15432,12 @@
       <c r="C30" s="72">
         <v>0.41</v>
       </c>
-      <c r="D30" s="211" t="s">
+      <c r="D30" s="218" t="s">
         <v>287</v>
       </c>
-      <c r="E30" s="212"/>
-      <c r="F30" s="212"/>
-      <c r="G30" s="213"/>
+      <c r="E30" s="219"/>
+      <c r="F30" s="219"/>
+      <c r="G30" s="220"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="52" t="s">
@@ -13759,12 +15449,12 @@
       <c r="C31" s="72">
         <v>0.59</v>
       </c>
-      <c r="D31" s="211" t="s">
+      <c r="D31" s="218" t="s">
         <v>289</v>
       </c>
-      <c r="E31" s="212"/>
-      <c r="F31" s="212"/>
-      <c r="G31" s="213"/>
+      <c r="E31" s="219"/>
+      <c r="F31" s="219"/>
+      <c r="G31" s="220"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="52" t="s">
@@ -13776,12 +15466,12 @@
       <c r="C32" s="72">
         <v>0.5</v>
       </c>
-      <c r="D32" s="211" t="s">
+      <c r="D32" s="218" t="s">
         <v>288</v>
       </c>
-      <c r="E32" s="212"/>
-      <c r="F32" s="212"/>
-      <c r="G32" s="213"/>
+      <c r="E32" s="219"/>
+      <c r="F32" s="219"/>
+      <c r="G32" s="220"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="52" t="s">
@@ -13793,12 +15483,12 @@
       <c r="C33" s="72">
         <v>0.59</v>
       </c>
-      <c r="D33" s="211" t="s">
+      <c r="D33" s="218" t="s">
         <v>290</v>
       </c>
-      <c r="E33" s="212"/>
-      <c r="F33" s="212"/>
-      <c r="G33" s="213"/>
+      <c r="E33" s="219"/>
+      <c r="F33" s="219"/>
+      <c r="G33" s="220"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="52" t="s">
@@ -13810,25 +15500,25 @@
       <c r="C34" s="72">
         <v>0.54</v>
       </c>
-      <c r="D34" s="211" t="s">
+      <c r="D34" s="218" t="s">
         <v>291</v>
       </c>
-      <c r="E34" s="212"/>
-      <c r="F34" s="212"/>
-      <c r="G34" s="213"/>
+      <c r="E34" s="219"/>
+      <c r="F34" s="219"/>
+      <c r="G34" s="220"/>
     </row>
     <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="207" t="s">
+      <c r="A36" s="214" t="s">
         <v>315</v>
       </c>
-      <c r="B36" s="207"/>
-      <c r="C36" s="207"/>
-      <c r="D36" s="207"/>
-      <c r="E36" s="207"/>
-      <c r="F36" s="207"/>
-      <c r="G36" s="207"/>
-      <c r="H36" s="207"/>
-      <c r="I36" s="207"/>
+      <c r="B36" s="214"/>
+      <c r="C36" s="214"/>
+      <c r="D36" s="214"/>
+      <c r="E36" s="214"/>
+      <c r="F36" s="214"/>
+      <c r="G36" s="214"/>
+      <c r="H36" s="214"/>
+      <c r="I36" s="214"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="87" t="s">
@@ -13895,12 +15585,12 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="199" t="s">
+      <c r="A46" s="206" t="s">
         <v>318</v>
       </c>
-      <c r="B46" s="199"/>
-      <c r="C46" s="199"/>
-      <c r="D46" s="199"/>
+      <c r="B46" s="206"/>
+      <c r="C46" s="206"/>
+      <c r="D46" s="206"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="88" t="s">
@@ -14078,7 +15768,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V48"/>
   <sheetViews>
@@ -14102,15 +15792,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="220" t="s">
+      <c r="A1" s="227" t="s">
         <v>347</v>
       </c>
-      <c r="B1" s="220"/>
-      <c r="C1" s="220"/>
-      <c r="D1" s="220"/>
-      <c r="E1" s="220"/>
-      <c r="F1" s="220"/>
-      <c r="G1" s="220"/>
+      <c r="B1" s="227"/>
+      <c r="C1" s="227"/>
+      <c r="D1" s="227"/>
+      <c r="E1" s="227"/>
+      <c r="F1" s="227"/>
+      <c r="G1" s="227"/>
     </row>
     <row r="2" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="158" t="s">
@@ -14134,11 +15824,11 @@
       <c r="G2" s="158" t="s">
         <v>344</v>
       </c>
-      <c r="I2" s="219" t="s">
+      <c r="I2" s="226" t="s">
         <v>197</v>
       </c>
-      <c r="J2" s="219"/>
-      <c r="K2" s="219"/>
+      <c r="J2" s="226"/>
+      <c r="K2" s="226"/>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
@@ -14591,20 +16281,20 @@
       <c r="J22" s="115" t="s">
         <v>217</v>
       </c>
-      <c r="K22" s="221" t="s">
+      <c r="K22" s="228" t="s">
         <v>307</v>
       </c>
-      <c r="L22" s="221"/>
-      <c r="M22" s="221"/>
-      <c r="N22" s="221"/>
-      <c r="O22" s="221"/>
-      <c r="P22" s="221"/>
-      <c r="Q22" s="221"/>
-      <c r="R22" s="221"/>
-      <c r="S22" s="221"/>
-      <c r="T22" s="221"/>
-      <c r="U22" s="221"/>
-      <c r="V22" s="221"/>
+      <c r="L22" s="228"/>
+      <c r="M22" s="228"/>
+      <c r="N22" s="228"/>
+      <c r="O22" s="228"/>
+      <c r="P22" s="228"/>
+      <c r="Q22" s="228"/>
+      <c r="R22" s="228"/>
+      <c r="S22" s="228"/>
+      <c r="T22" s="228"/>
+      <c r="U22" s="228"/>
+      <c r="V22" s="228"/>
     </row>
     <row r="23" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="36" t="s">
@@ -14710,10 +16400,10 @@
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="223"/>
-      <c r="B29" s="224"/>
-      <c r="C29" s="224"/>
-      <c r="D29" s="225"/>
+      <c r="A29" s="230"/>
+      <c r="B29" s="231"/>
+      <c r="C29" s="231"/>
+      <c r="D29" s="232"/>
       <c r="I29" s="43" t="s">
         <v>187</v>
       </c>
@@ -14730,10 +16420,10 @@
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" s="226" t="s">
+      <c r="A31" s="233" t="s">
         <v>181</v>
       </c>
-      <c r="B31" s="227"/>
+      <c r="B31" s="234"/>
       <c r="C31" s="68"/>
       <c r="I31" s="43" t="s">
         <v>189</v>
@@ -14755,20 +16445,20 @@
       <c r="J32" s="116" t="s">
         <v>308</v>
       </c>
-      <c r="K32" s="222" t="s">
+      <c r="K32" s="229" t="s">
         <v>306</v>
       </c>
-      <c r="L32" s="222"/>
-      <c r="M32" s="222"/>
-      <c r="N32" s="222"/>
-      <c r="O32" s="222"/>
-      <c r="P32" s="222"/>
-      <c r="Q32" s="222"/>
-      <c r="R32" s="222"/>
-      <c r="S32" s="222"/>
-      <c r="T32" s="222"/>
-      <c r="U32" s="222"/>
-      <c r="V32" s="222"/>
+      <c r="L32" s="229"/>
+      <c r="M32" s="229"/>
+      <c r="N32" s="229"/>
+      <c r="O32" s="229"/>
+      <c r="P32" s="229"/>
+      <c r="Q32" s="229"/>
+      <c r="R32" s="229"/>
+      <c r="S32" s="229"/>
+      <c r="T32" s="229"/>
+      <c r="U32" s="229"/>
+      <c r="V32" s="229"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="84" t="s">
@@ -14801,10 +16491,10 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="215" t="s">
+      <c r="A35" s="222" t="s">
         <v>184</v>
       </c>
-      <c r="B35" s="217" t="s">
+      <c r="B35" s="224" t="s">
         <v>219</v>
       </c>
       <c r="D35" s="90"/>
@@ -14814,8 +16504,8 @@
       <c r="J35" s="41"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="216"/>
-      <c r="B36" s="218"/>
+      <c r="A36" s="223"/>
+      <c r="B36" s="225"/>
       <c r="D36" s="90"/>
       <c r="I36" s="105" t="s">
         <v>296</v>
@@ -14904,7 +16594,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V48"/>
   <sheetViews>
@@ -14934,15 +16624,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="220" t="s">
+      <c r="A1" s="227" t="s">
         <v>347</v>
       </c>
-      <c r="B1" s="220"/>
-      <c r="C1" s="220"/>
-      <c r="D1" s="220"/>
-      <c r="E1" s="220"/>
-      <c r="F1" s="220"/>
-      <c r="G1" s="220"/>
+      <c r="B1" s="227"/>
+      <c r="C1" s="227"/>
+      <c r="D1" s="227"/>
+      <c r="E1" s="227"/>
+      <c r="F1" s="227"/>
+      <c r="G1" s="227"/>
     </row>
     <row r="2" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="158" t="s">
@@ -14966,11 +16656,11 @@
       <c r="G2" s="158" t="s">
         <v>344</v>
       </c>
-      <c r="I2" s="219" t="s">
+      <c r="I2" s="226" t="s">
         <v>197</v>
       </c>
-      <c r="J2" s="219"/>
-      <c r="K2" s="219"/>
+      <c r="J2" s="226"/>
+      <c r="K2" s="226"/>
       <c r="O2" s="170" t="s">
         <v>351</v>
       </c>
@@ -15471,20 +17161,20 @@
       <c r="J22" s="115" t="s">
         <v>217</v>
       </c>
-      <c r="K22" s="221" t="s">
+      <c r="K22" s="228" t="s">
         <v>307</v>
       </c>
-      <c r="L22" s="221"/>
-      <c r="M22" s="221"/>
-      <c r="N22" s="221"/>
-      <c r="O22" s="221"/>
-      <c r="P22" s="221"/>
-      <c r="Q22" s="221"/>
-      <c r="R22" s="221"/>
-      <c r="S22" s="221"/>
-      <c r="T22" s="221"/>
-      <c r="U22" s="221"/>
-      <c r="V22" s="221"/>
+      <c r="L22" s="228"/>
+      <c r="M22" s="228"/>
+      <c r="N22" s="228"/>
+      <c r="O22" s="228"/>
+      <c r="P22" s="228"/>
+      <c r="Q22" s="228"/>
+      <c r="R22" s="228"/>
+      <c r="S22" s="228"/>
+      <c r="T22" s="228"/>
+      <c r="U22" s="228"/>
+      <c r="V22" s="228"/>
     </row>
     <row r="23" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="36" t="s">
@@ -15590,10 +17280,10 @@
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="223"/>
-      <c r="B29" s="224"/>
-      <c r="C29" s="224"/>
-      <c r="D29" s="225"/>
+      <c r="A29" s="230"/>
+      <c r="B29" s="231"/>
+      <c r="C29" s="231"/>
+      <c r="D29" s="232"/>
       <c r="I29" s="43" t="s">
         <v>187</v>
       </c>
@@ -15610,10 +17300,10 @@
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" s="226" t="s">
+      <c r="A31" s="233" t="s">
         <v>181</v>
       </c>
-      <c r="B31" s="227"/>
+      <c r="B31" s="234"/>
       <c r="C31" s="68"/>
       <c r="I31" s="43" t="s">
         <v>189</v>
@@ -15635,20 +17325,20 @@
       <c r="J32" s="116" t="s">
         <v>308</v>
       </c>
-      <c r="K32" s="222" t="s">
+      <c r="K32" s="229" t="s">
         <v>306</v>
       </c>
-      <c r="L32" s="222"/>
-      <c r="M32" s="222"/>
-      <c r="N32" s="222"/>
-      <c r="O32" s="222"/>
-      <c r="P32" s="222"/>
-      <c r="Q32" s="222"/>
-      <c r="R32" s="222"/>
-      <c r="S32" s="222"/>
-      <c r="T32" s="222"/>
-      <c r="U32" s="222"/>
-      <c r="V32" s="222"/>
+      <c r="L32" s="229"/>
+      <c r="M32" s="229"/>
+      <c r="N32" s="229"/>
+      <c r="O32" s="229"/>
+      <c r="P32" s="229"/>
+      <c r="Q32" s="229"/>
+      <c r="R32" s="229"/>
+      <c r="S32" s="229"/>
+      <c r="T32" s="229"/>
+      <c r="U32" s="229"/>
+      <c r="V32" s="229"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="84" t="s">
@@ -15679,10 +17369,10 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="215" t="s">
+      <c r="A35" s="222" t="s">
         <v>184</v>
       </c>
-      <c r="B35" s="217" t="s">
+      <c r="B35" s="224" t="s">
         <v>219</v>
       </c>
       <c r="I35" s="43" t="s">
@@ -15691,8 +17381,8 @@
       <c r="J35" s="41"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="216"/>
-      <c r="B36" s="218"/>
+      <c r="A36" s="223"/>
+      <c r="B36" s="225"/>
       <c r="I36" s="105" t="s">
         <v>296</v>
       </c>
@@ -15774,12 +17464,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="A24" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15794,18 +17484,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="228" t="s">
+      <c r="A1" s="235" t="s">
         <v>464</v>
       </c>
-      <c r="B1" s="228"/>
-      <c r="C1" s="228"/>
-      <c r="D1" s="228"/>
-      <c r="E1" s="228"/>
-      <c r="F1" s="228"/>
-      <c r="G1" s="228"/>
-      <c r="H1" s="228"/>
-      <c r="I1" s="228"/>
-      <c r="J1" s="228"/>
+      <c r="B1" s="235"/>
+      <c r="C1" s="235"/>
+      <c r="D1" s="235"/>
+      <c r="E1" s="235"/>
+      <c r="F1" s="235"/>
+      <c r="G1" s="235"/>
+      <c r="H1" s="235"/>
+      <c r="I1" s="235"/>
+      <c r="J1" s="235"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="173" t="s">
@@ -16635,33 +18325,4 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:G1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="235" t="s">
-        <v>525</v>
-      </c>
-      <c r="B1" s="235"/>
-      <c r="C1" s="235"/>
-      <c r="D1" s="235"/>
-      <c r="E1" s="235"/>
-      <c r="F1" s="235"/>
-      <c r="G1" s="235"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
-  </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
ajustes no FSB e inclusao da tag final selected
</commit_message>
<xml_diff>
--- a/Experiment01_Resumo/Resumo_Exp01.xlsx
+++ b/Experiment01_Resumo/Resumo_Exp01.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1492" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1494" uniqueCount="570">
   <si>
     <t>Database search</t>
   </si>
@@ -1731,12 +1731,6 @@
     <t>Não acessível</t>
   </si>
   <si>
-    <t>Selecionados</t>
-  </si>
-  <si>
-    <t>Não fez BSB pq estava indisponível</t>
-  </si>
-  <si>
     <t xml:space="preserve">Citado por 8, mas 2 são de 2016 e 1 de 2017. Então foram incluídos somente 5. </t>
   </si>
   <si>
@@ -1809,12 +1803,6 @@
     <t>Google scholar em 16/3</t>
   </si>
   <si>
-    <t>Forward JF Tool</t>
-  </si>
-  <si>
-    <t>Related JF Tool</t>
-  </si>
-  <si>
     <t>Obs. FSB</t>
   </si>
   <si>
@@ -1843,6 +1831,24 @@
   </si>
   <si>
     <t>15 menos 3 =12 incluidos</t>
+  </si>
+  <si>
+    <t>Forward JF Tool em 13 e 14/04</t>
+  </si>
+  <si>
+    <t>Related JF Tool em 13 e 14/04</t>
+  </si>
+  <si>
+    <t>Solicitou a compra/cópia / Não fez BSB</t>
+  </si>
+  <si>
+    <t>Selecionados Final</t>
+  </si>
+  <si>
+    <t>Não fez BSB pq estava indisponível, mas fez FSB.</t>
+  </si>
+  <si>
+    <t>Resumo dos 51 estudos - JF Tool, Selecionados no Final, Excluídos, BSB, FSB</t>
   </si>
 </sst>
 </file>
@@ -1941,7 +1947,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="25">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2077,12 +2083,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF99FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2535,7 +2535,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="257">
+  <cellXfs count="255">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3019,15 +3019,6 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3112,6 +3103,33 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3121,12 +3139,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3139,27 +3151,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3222,6 +3213,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3546,12 +3540,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="187213064"/>
-        <c:axId val="187216592"/>
+        <c:axId val="191324120"/>
+        <c:axId val="191324512"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="187213064"/>
+        <c:axId val="191324120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3643,7 +3637,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="187216592"/>
+        <c:crossAx val="191324512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3651,7 +3645,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="187216592"/>
+        <c:axId val="191324512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3702,7 +3696,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="187213064"/>
+        <c:crossAx val="191324120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4011,12 +4005,12 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:shape val="box"/>
-        <c:axId val="189324152"/>
-        <c:axId val="189325720"/>
+        <c:axId val="221061384"/>
+        <c:axId val="221061776"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="189324152"/>
+        <c:axId val="221061384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4105,7 +4099,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189325720"/>
+        <c:crossAx val="221061776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4113,7 +4107,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189325720"/>
+        <c:axId val="221061776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4196,7 +4190,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189324152"/>
+        <c:crossAx val="221061384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4481,12 +4475,12 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:shape val="box"/>
-        <c:axId val="189328464"/>
-        <c:axId val="189323760"/>
+        <c:axId val="221062560"/>
+        <c:axId val="221056288"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="189328464"/>
+        <c:axId val="221062560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4575,7 +4569,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189323760"/>
+        <c:crossAx val="221056288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4583,7 +4577,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189323760"/>
+        <c:axId val="221056288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4666,7 +4660,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189328464"/>
+        <c:crossAx val="221062560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5453,12 +5447,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="189329640"/>
-        <c:axId val="189325328"/>
+        <c:axId val="221057072"/>
+        <c:axId val="221055504"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="189329640"/>
+        <c:axId val="221057072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5498,7 +5492,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189325328"/>
+        <c:crossAx val="221055504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5506,7 +5500,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189325328"/>
+        <c:axId val="221055504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5554,7 +5548,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189329640"/>
+        <c:crossAx val="221057072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5862,8 +5856,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="189328856"/>
-        <c:axId val="189329248"/>
+        <c:axId val="221055112"/>
+        <c:axId val="221055896"/>
         <c:axId val="0"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -6033,7 +6027,7 @@
         </c:extLst>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="189328856"/>
+        <c:axId val="221055112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6131,7 +6125,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189329248"/>
+        <c:crossAx val="221055896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6139,7 +6133,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189329248"/>
+        <c:axId val="221055896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6218,7 +6212,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="189328856"/>
+        <c:crossAx val="221055112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6532,8 +6526,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="189326112"/>
-        <c:axId val="189326504"/>
+        <c:axId val="221059816"/>
+        <c:axId val="221060600"/>
         <c:axId val="0"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -6703,7 +6697,7 @@
         </c:extLst>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="189326112"/>
+        <c:axId val="221059816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6801,7 +6795,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189326504"/>
+        <c:crossAx val="221060600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6809,7 +6803,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189326504"/>
+        <c:axId val="221060600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6888,7 +6882,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="189326112"/>
+        <c:crossAx val="221059816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10586,22 +10580,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="204" t="s">
+      <c r="A1" s="201" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="205"/>
+      <c r="B1" s="202"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="206" t="s">
+      <c r="A2" s="203" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="207"/>
+      <c r="B2" s="204"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="206" t="s">
+      <c r="A3" s="203" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="207"/>
+      <c r="B3" s="204"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -10636,10 +10630,10 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="208" t="s">
+      <c r="A8" s="205" t="s">
         <v>103</v>
       </c>
-      <c r="B8" s="209"/>
+      <c r="B8" s="206"/>
     </row>
     <row r="9" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
@@ -10715,15 +10709,15 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="250" t="s">
+      <c r="A1" s="247" t="s">
         <v>525</v>
       </c>
-      <c r="B1" s="250"/>
-      <c r="C1" s="250"/>
-      <c r="D1" s="250"/>
-      <c r="E1" s="250"/>
-      <c r="F1" s="250"/>
-      <c r="G1" s="250"/>
+      <c r="B1" s="247"/>
+      <c r="C1" s="247"/>
+      <c r="D1" s="247"/>
+      <c r="E1" s="247"/>
+      <c r="F1" s="247"/>
+      <c r="G1" s="247"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -10758,19 +10752,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="219" t="s">
+      <c r="A1" s="216" t="s">
         <v>326</v>
       </c>
-      <c r="B1" s="219"/>
-      <c r="C1" s="219"/>
-      <c r="D1" s="219"/>
-      <c r="E1" s="219"/>
-      <c r="F1" s="219"/>
-      <c r="G1" s="219"/>
-      <c r="H1" s="219"/>
-      <c r="I1" s="219"/>
-      <c r="J1" s="219"/>
-      <c r="K1" s="219"/>
+      <c r="B1" s="216"/>
+      <c r="C1" s="216"/>
+      <c r="D1" s="216"/>
+      <c r="E1" s="216"/>
+      <c r="F1" s="216"/>
+      <c r="G1" s="216"/>
+      <c r="H1" s="216"/>
+      <c r="I1" s="216"/>
+      <c r="J1" s="216"/>
+      <c r="K1" s="216"/>
     </row>
     <row r="2" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
@@ -11492,10 +11486,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="251" t="s">
+      <c r="A1" s="248" t="s">
         <v>333</v>
       </c>
-      <c r="B1" s="252"/>
+      <c r="B1" s="249"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="79" t="s">
@@ -11563,20 +11557,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="253" t="s">
+      <c r="A1" s="250" t="s">
         <v>327</v>
       </c>
-      <c r="B1" s="253"/>
-      <c r="C1" s="253"/>
-      <c r="D1" s="253"/>
-      <c r="E1" s="253"/>
-      <c r="F1" s="253"/>
-      <c r="G1" s="253"/>
-      <c r="H1" s="253"/>
-      <c r="I1" s="253"/>
-      <c r="J1" s="253"/>
-      <c r="K1" s="253"/>
-      <c r="L1" s="253"/>
+      <c r="B1" s="250"/>
+      <c r="C1" s="250"/>
+      <c r="D1" s="250"/>
+      <c r="E1" s="250"/>
+      <c r="F1" s="250"/>
+      <c r="G1" s="250"/>
+      <c r="H1" s="250"/>
+      <c r="I1" s="250"/>
+      <c r="J1" s="250"/>
+      <c r="K1" s="250"/>
+      <c r="L1" s="250"/>
     </row>
     <row r="2" spans="1:12" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="142" t="s">
@@ -12295,15 +12289,15 @@
     </row>
     <row r="26" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="134"/>
-      <c r="B26" s="254" t="s">
+      <c r="B26" s="251" t="s">
         <v>334</v>
       </c>
-      <c r="C26" s="255"/>
-      <c r="D26" s="255"/>
-      <c r="E26" s="255"/>
-      <c r="F26" s="255"/>
-      <c r="G26" s="255"/>
-      <c r="H26" s="256"/>
+      <c r="C26" s="252"/>
+      <c r="D26" s="252"/>
+      <c r="E26" s="252"/>
+      <c r="F26" s="252"/>
+      <c r="G26" s="252"/>
+      <c r="H26" s="253"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="66"/>
@@ -12471,10 +12465,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="214" t="s">
+      <c r="A1" s="211" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="215"/>
+      <c r="B1" s="212"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
@@ -12507,16 +12501,16 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="210" t="s">
+      <c r="A6" s="207" t="s">
         <v>147</v>
       </c>
-      <c r="B6" s="211"/>
+      <c r="B6" s="208"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="212" t="s">
+      <c r="A7" s="209" t="s">
         <v>150</v>
       </c>
-      <c r="B7" s="213"/>
+      <c r="B7" s="210"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -12598,16 +12592,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="216" t="s">
+      <c r="A1" s="213" t="s">
         <v>336</v>
       </c>
-      <c r="B1" s="217"/>
-      <c r="C1" s="217"/>
-      <c r="D1" s="217"/>
-      <c r="E1" s="217"/>
-      <c r="F1" s="217"/>
-      <c r="G1" s="217"/>
-      <c r="H1" s="218"/>
+      <c r="B1" s="214"/>
+      <c r="C1" s="214"/>
+      <c r="D1" s="214"/>
+      <c r="E1" s="214"/>
+      <c r="F1" s="214"/>
+      <c r="G1" s="214"/>
+      <c r="H1" s="215"/>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
     </row>
@@ -12977,14 +12971,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="219" t="s">
+      <c r="A1" s="216" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="219"/>
-      <c r="C1" s="219"/>
-      <c r="D1" s="219"/>
-      <c r="E1" s="219"/>
-      <c r="F1" s="219"/>
+      <c r="B1" s="216"/>
+      <c r="C1" s="216"/>
+      <c r="D1" s="216"/>
+      <c r="E1" s="216"/>
+      <c r="F1" s="216"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
@@ -13467,31 +13461,55 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:T53"/>
+  <dimension ref="A1:T53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="62.42578125" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" customWidth="1"/>
     <col min="3" max="3" width="25.5703125" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" style="81" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="81" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="81" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" style="81" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" style="81" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" style="81" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" style="3" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="3"/>
-    <col min="14" max="14" width="14.5703125" style="71" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" style="81" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" style="81" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="3"/>
+    <col min="11" max="11" width="14.5703125" style="71" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" style="81" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" style="81" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="81" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" customWidth="1"/>
+    <col min="17" max="17" width="12" customWidth="1"/>
+    <col min="18" max="20" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="254" t="s">
+        <v>569</v>
+      </c>
+      <c r="B1" s="254"/>
+      <c r="C1" s="254"/>
+      <c r="D1" s="254"/>
+      <c r="E1" s="254"/>
+      <c r="F1" s="254"/>
+      <c r="G1" s="254"/>
+      <c r="H1" s="254"/>
+      <c r="I1" s="254"/>
+      <c r="J1" s="254"/>
+      <c r="K1" s="254"/>
+      <c r="L1" s="254"/>
+      <c r="M1" s="254"/>
+      <c r="N1" s="254"/>
+      <c r="O1" s="254"/>
+      <c r="P1" s="254"/>
+      <c r="Q1" s="254"/>
+    </row>
     <row r="2" spans="1:20" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>123</v>
@@ -13511,41 +13529,43 @@
       <c r="F2" s="21" t="s">
         <v>474</v>
       </c>
-      <c r="G2" s="82" t="s">
+      <c r="G2" s="21"/>
+      <c r="H2" s="82" t="s">
+        <v>567</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>526</v>
+      </c>
+      <c r="J2" s="82" t="s">
+        <v>529</v>
+      </c>
+      <c r="K2" s="82" t="s">
+        <v>566</v>
+      </c>
+      <c r="L2" s="82" t="s">
+        <v>549</v>
+      </c>
+      <c r="M2" s="82" t="s">
+        <v>564</v>
+      </c>
+      <c r="N2" s="82" t="s">
+        <v>565</v>
+      </c>
+      <c r="O2" s="91"/>
+      <c r="P2" s="196" t="s">
+        <v>550</v>
+      </c>
+      <c r="Q2" s="196" t="s">
         <v>551</v>
       </c>
-      <c r="H2" s="82" t="s">
-        <v>556</v>
-      </c>
-      <c r="I2" s="82" t="s">
-        <v>557</v>
-      </c>
-      <c r="J2" s="21"/>
-      <c r="K2" s="199" t="s">
-        <v>530</v>
-      </c>
-      <c r="L2" s="21" t="s">
-        <v>526</v>
-      </c>
-      <c r="M2" s="82" t="s">
-        <v>529</v>
-      </c>
-      <c r="N2" s="19"/>
-      <c r="O2" s="91"/>
-      <c r="P2" s="199" t="s">
+      <c r="R2" s="198" t="s">
         <v>552</v>
       </c>
-      <c r="Q2" s="199" t="s">
+      <c r="S2" s="198" t="s">
         <v>553</v>
       </c>
-      <c r="R2" s="201" t="s">
+      <c r="T2" s="199" t="s">
         <v>554</v>
-      </c>
-      <c r="S2" s="201" t="s">
-        <v>555</v>
-      </c>
-      <c r="T2" s="202" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -13564,25 +13584,25 @@
       <c r="E3" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="48" t="s">
+      <c r="F3" s="183" t="s">
         <v>502</v>
       </c>
-      <c r="G3" s="48">
+      <c r="G3" s="48"/>
+      <c r="H3" s="183" t="s">
+        <v>346</v>
+      </c>
+      <c r="I3" s="94"/>
+      <c r="J3" s="94"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="48">
         <v>2</v>
       </c>
-      <c r="H3" s="48">
+      <c r="M3" s="48">
         <v>2</v>
       </c>
-      <c r="I3" s="48">
+      <c r="N3" s="48">
         <v>0</v>
       </c>
-      <c r="J3" s="48"/>
-      <c r="K3" s="183" t="s">
-        <v>346</v>
-      </c>
-      <c r="L3" s="94"/>
-      <c r="M3" s="94"/>
-      <c r="N3" s="19"/>
       <c r="O3" s="91"/>
       <c r="P3" s="67">
         <v>25</v>
@@ -13614,25 +13634,25 @@
       <c r="E4" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="F4" s="48" t="s">
+      <c r="F4" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="G4" s="48">
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J4" s="94"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="48">
         <v>10</v>
       </c>
-      <c r="H4" s="48">
+      <c r="M4" s="48">
         <v>9</v>
       </c>
-      <c r="I4" s="48">
+      <c r="N4" s="48">
         <v>0</v>
       </c>
-      <c r="J4" s="48"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="34" t="s">
-        <v>346</v>
-      </c>
-      <c r="M4" s="94"/>
-      <c r="N4" s="19"/>
       <c r="O4" s="91"/>
       <c r="P4" s="67">
         <v>20</v>
@@ -13664,28 +13684,28 @@
       <c r="E5" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="183" t="s">
         <v>210</v>
       </c>
-      <c r="G5" s="48">
+      <c r="G5" s="48"/>
+      <c r="H5" s="183" t="s">
+        <v>346</v>
+      </c>
+      <c r="I5" s="94"/>
+      <c r="J5" s="186" t="s">
+        <v>346</v>
+      </c>
+      <c r="K5" s="189" t="s">
+        <v>528</v>
+      </c>
+      <c r="L5" s="48">
         <v>1</v>
       </c>
-      <c r="H5" s="48">
+      <c r="M5" s="48">
         <v>0</v>
       </c>
-      <c r="I5" s="48">
+      <c r="N5" s="48">
         <v>0</v>
-      </c>
-      <c r="J5" s="48"/>
-      <c r="K5" s="183" t="s">
-        <v>346</v>
-      </c>
-      <c r="L5" s="94"/>
-      <c r="M5" s="186" t="s">
-        <v>346</v>
-      </c>
-      <c r="N5" s="192" t="s">
-        <v>528</v>
       </c>
       <c r="O5" s="91"/>
       <c r="P5" s="67">
@@ -13718,25 +13738,25 @@
       <c r="E6" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="F6" s="48" t="s">
+      <c r="F6" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="G6" s="48">
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J6" s="94"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="48">
         <v>11</v>
       </c>
-      <c r="H6" s="48">
+      <c r="M6" s="48">
         <v>2</v>
       </c>
-      <c r="I6" s="48">
+      <c r="N6" s="48">
         <v>0</v>
       </c>
-      <c r="J6" s="48"/>
-      <c r="K6" s="48"/>
-      <c r="L6" s="34" t="s">
-        <v>346</v>
-      </c>
-      <c r="M6" s="94"/>
-      <c r="N6" s="19"/>
       <c r="O6" s="91"/>
       <c r="P6" s="67">
         <v>57</v>
@@ -13768,25 +13788,25 @@
       <c r="E7" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="F7" s="48" t="s">
+      <c r="F7" s="183" t="s">
         <v>211</v>
       </c>
-      <c r="G7" s="48">
+      <c r="G7" s="48"/>
+      <c r="H7" s="183" t="s">
+        <v>346</v>
+      </c>
+      <c r="I7" s="94"/>
+      <c r="J7" s="94"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="48">
         <v>15</v>
       </c>
-      <c r="H7" s="48">
+      <c r="M7" s="48">
         <v>8</v>
       </c>
-      <c r="I7" s="48">
+      <c r="N7" s="48">
         <v>1</v>
       </c>
-      <c r="J7" s="48"/>
-      <c r="K7" s="183" t="s">
-        <v>346</v>
-      </c>
-      <c r="L7" s="94"/>
-      <c r="M7" s="94"/>
-      <c r="N7" s="19"/>
       <c r="O7" s="91"/>
       <c r="P7" s="48">
         <v>11</v>
@@ -13818,25 +13838,25 @@
       <c r="E8" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="F8" s="48" t="s">
+      <c r="F8" s="183" t="s">
         <v>512</v>
       </c>
-      <c r="G8" s="48">
+      <c r="G8" s="48"/>
+      <c r="H8" s="183" t="s">
+        <v>346</v>
+      </c>
+      <c r="I8" s="94"/>
+      <c r="J8" s="94"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="48">
         <v>11</v>
       </c>
-      <c r="H8" s="48">
+      <c r="M8" s="48">
         <v>8</v>
       </c>
-      <c r="I8" s="48">
+      <c r="N8" s="48">
         <v>0</v>
       </c>
-      <c r="J8" s="48"/>
-      <c r="K8" s="183" t="s">
-        <v>346</v>
-      </c>
-      <c r="L8" s="94"/>
-      <c r="M8" s="94"/>
-      <c r="N8" s="19"/>
       <c r="O8" s="91"/>
       <c r="P8" s="48">
         <v>22</v>
@@ -13868,25 +13888,25 @@
       <c r="E9" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="F9" s="48" t="s">
+      <c r="F9" s="183" t="s">
         <v>513</v>
       </c>
-      <c r="G9" s="48">
+      <c r="G9" s="48"/>
+      <c r="H9" s="183" t="s">
+        <v>346</v>
+      </c>
+      <c r="I9" s="94"/>
+      <c r="J9" s="94"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="48">
         <v>22</v>
       </c>
-      <c r="H9" s="48">
-        <v>19</v>
-      </c>
-      <c r="I9" s="48">
+      <c r="M9" s="48">
+        <v>20</v>
+      </c>
+      <c r="N9" s="48">
         <v>1</v>
       </c>
-      <c r="J9" s="48"/>
-      <c r="K9" s="183" t="s">
-        <v>346</v>
-      </c>
-      <c r="L9" s="94"/>
-      <c r="M9" s="94"/>
-      <c r="N9" s="19"/>
       <c r="O9" s="91"/>
       <c r="P9" s="48">
         <v>13</v>
@@ -13918,25 +13938,25 @@
       <c r="E10" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="F10" s="48" t="s">
+      <c r="F10" s="183" t="s">
         <v>212</v>
       </c>
-      <c r="G10" s="48">
+      <c r="G10" s="48"/>
+      <c r="H10" s="183" t="s">
+        <v>346</v>
+      </c>
+      <c r="I10" s="94"/>
+      <c r="J10" s="94"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="48">
         <v>19</v>
       </c>
-      <c r="H10" s="48">
+      <c r="M10" s="48">
         <v>15</v>
       </c>
-      <c r="I10" s="48">
+      <c r="N10" s="48">
         <v>0</v>
       </c>
-      <c r="J10" s="48"/>
-      <c r="K10" s="183" t="s">
-        <v>346</v>
-      </c>
-      <c r="L10" s="94"/>
-      <c r="M10" s="94"/>
-      <c r="N10" s="19"/>
       <c r="O10" s="91"/>
       <c r="P10" s="48">
         <v>43</v>
@@ -13968,25 +13988,25 @@
       <c r="E11" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="F11" s="48" t="s">
+      <c r="F11" s="183" t="s">
         <v>514</v>
       </c>
-      <c r="G11" s="48">
+      <c r="G11" s="48"/>
+      <c r="H11" s="183" t="s">
+        <v>346</v>
+      </c>
+      <c r="I11" s="94"/>
+      <c r="J11" s="94"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="2">
         <v>147</v>
       </c>
-      <c r="H11" s="48">
-        <v>103</v>
-      </c>
-      <c r="I11" s="48">
+      <c r="M11" s="48">
+        <v>105</v>
+      </c>
+      <c r="N11" s="48">
         <v>11</v>
       </c>
-      <c r="J11" s="48"/>
-      <c r="K11" s="183" t="s">
-        <v>346</v>
-      </c>
-      <c r="L11" s="94"/>
-      <c r="M11" s="94"/>
-      <c r="N11" s="19"/>
       <c r="O11" s="91"/>
       <c r="P11" s="48">
         <v>11</v>
@@ -14000,8 +14020,8 @@
       <c r="S11" s="183">
         <v>146</v>
       </c>
-      <c r="T11" s="203" t="s">
-        <v>559</v>
+      <c r="T11" s="200" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -14020,25 +14040,25 @@
       <c r="E12" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="F12" s="48" t="s">
+      <c r="F12" s="183" t="s">
         <v>515</v>
       </c>
-      <c r="G12" s="48">
+      <c r="G12" s="48"/>
+      <c r="H12" s="183" t="s">
+        <v>346</v>
+      </c>
+      <c r="I12" s="94"/>
+      <c r="J12" s="94"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="2">
         <v>56</v>
       </c>
-      <c r="H12" s="48">
-        <v>50</v>
-      </c>
-      <c r="I12" s="48">
+      <c r="M12" s="48">
+        <v>51</v>
+      </c>
+      <c r="N12" s="48">
         <v>1</v>
       </c>
-      <c r="J12" s="48"/>
-      <c r="K12" s="183" t="s">
-        <v>346</v>
-      </c>
-      <c r="L12" s="94"/>
-      <c r="M12" s="94"/>
-      <c r="N12" s="19"/>
       <c r="O12" s="91"/>
       <c r="P12" s="2">
         <v>37</v>
@@ -14070,25 +14090,25 @@
       <c r="E13" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="F13" s="48" t="s">
+      <c r="F13" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="G13" s="48">
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J13" s="94"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="2">
         <v>42</v>
       </c>
-      <c r="H13" s="48">
-        <v>34</v>
-      </c>
-      <c r="I13" s="48">
+      <c r="M13" s="48">
+        <v>39</v>
+      </c>
+      <c r="N13" s="48">
         <v>0</v>
       </c>
-      <c r="J13" s="48"/>
-      <c r="K13" s="48"/>
-      <c r="L13" s="34" t="s">
-        <v>346</v>
-      </c>
-      <c r="M13" s="94"/>
-      <c r="N13" s="19"/>
       <c r="O13" s="91"/>
       <c r="P13" s="48">
         <v>16</v>
@@ -14103,7 +14123,7 @@
         <v>41</v>
       </c>
       <c r="T13" s="66" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -14122,25 +14142,25 @@
       <c r="E14" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="F14" s="48" t="s">
+      <c r="F14" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="G14" s="48">
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J14" s="94"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="48">
         <v>5</v>
       </c>
-      <c r="H14" s="48">
+      <c r="M14" s="48">
         <v>4</v>
       </c>
-      <c r="I14" s="48">
+      <c r="N14" s="48">
         <v>0</v>
       </c>
-      <c r="J14" s="48"/>
-      <c r="K14" s="48"/>
-      <c r="L14" s="34" t="s">
-        <v>346</v>
-      </c>
-      <c r="M14" s="94"/>
-      <c r="N14" s="19"/>
       <c r="O14" s="91"/>
       <c r="P14" s="48">
         <v>14</v>
@@ -14172,25 +14192,25 @@
       <c r="E15" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="F15" s="48" t="s">
+      <c r="F15" s="183" t="s">
         <v>517</v>
       </c>
-      <c r="G15" s="48">
+      <c r="G15" s="48"/>
+      <c r="H15" s="183" t="s">
+        <v>346</v>
+      </c>
+      <c r="I15" s="94"/>
+      <c r="J15" s="94"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="48">
         <v>7</v>
       </c>
-      <c r="H15" s="48">
+      <c r="M15" s="48">
         <v>2</v>
       </c>
-      <c r="I15" s="48">
+      <c r="N15" s="48">
         <v>1</v>
       </c>
-      <c r="J15" s="48"/>
-      <c r="K15" s="183" t="s">
-        <v>346</v>
-      </c>
-      <c r="L15" s="94"/>
-      <c r="M15" s="94"/>
-      <c r="N15" s="19"/>
       <c r="O15" s="91"/>
       <c r="P15" s="48">
         <v>8</v>
@@ -14222,25 +14242,25 @@
       <c r="E16" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="F16" s="48" t="s">
+      <c r="F16" s="183" t="s">
         <v>215</v>
       </c>
-      <c r="G16" s="48">
+      <c r="G16" s="48"/>
+      <c r="H16" s="183" t="s">
+        <v>346</v>
+      </c>
+      <c r="I16" s="94"/>
+      <c r="J16" s="94"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="48">
         <v>5</v>
       </c>
-      <c r="H16" s="48">
+      <c r="M16" s="48">
         <v>3</v>
       </c>
-      <c r="I16" s="48">
+      <c r="N16" s="48">
         <v>0</v>
       </c>
-      <c r="J16" s="48"/>
-      <c r="K16" s="183" t="s">
-        <v>346</v>
-      </c>
-      <c r="L16" s="94"/>
-      <c r="M16" s="94"/>
-      <c r="N16" s="19"/>
       <c r="O16" s="91"/>
       <c r="P16" s="48">
         <v>27</v>
@@ -14272,25 +14292,25 @@
       <c r="E17" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="F17" s="48" t="s">
+      <c r="F17" s="183" t="s">
         <v>216</v>
       </c>
-      <c r="G17" s="48">
+      <c r="G17" s="48"/>
+      <c r="H17" s="183" t="s">
+        <v>346</v>
+      </c>
+      <c r="I17" s="94"/>
+      <c r="J17" s="94"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="48">
         <v>10</v>
       </c>
-      <c r="H17" s="48">
+      <c r="M17" s="48">
         <v>10</v>
       </c>
-      <c r="I17" s="48">
+      <c r="N17" s="48">
         <v>0</v>
       </c>
-      <c r="J17" s="48"/>
-      <c r="K17" s="183" t="s">
-        <v>346</v>
-      </c>
-      <c r="L17" s="94"/>
-      <c r="M17" s="94"/>
-      <c r="N17" s="19"/>
       <c r="O17" s="91"/>
       <c r="P17" s="48">
         <v>14</v>
@@ -14322,25 +14342,25 @@
       <c r="E18" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="F18" s="48" t="s">
+      <c r="F18" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="G18" s="48">
+      <c r="G18" s="48"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J18" s="94"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="48">
         <v>8</v>
       </c>
-      <c r="H18" s="48">
-        <v>6</v>
-      </c>
-      <c r="I18" s="48">
+      <c r="M18" s="48">
+        <v>7</v>
+      </c>
+      <c r="N18" s="48">
         <v>1</v>
       </c>
-      <c r="J18" s="48"/>
-      <c r="K18" s="48"/>
-      <c r="L18" s="34" t="s">
-        <v>346</v>
-      </c>
-      <c r="M18" s="94"/>
-      <c r="N18" s="19"/>
       <c r="O18" s="91"/>
       <c r="P18" s="48">
         <v>8</v>
@@ -14372,25 +14392,25 @@
       <c r="E19" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="F19" s="48" t="s">
+      <c r="F19" s="183" t="s">
         <v>519</v>
       </c>
-      <c r="G19" s="48">
+      <c r="G19" s="48"/>
+      <c r="H19" s="183" t="s">
+        <v>346</v>
+      </c>
+      <c r="I19" s="94"/>
+      <c r="J19" s="94"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="48">
         <v>17</v>
       </c>
-      <c r="H19" s="48">
-        <v>12</v>
-      </c>
-      <c r="I19" s="48">
+      <c r="M19" s="48">
+        <v>14</v>
+      </c>
+      <c r="N19" s="48">
         <v>0</v>
       </c>
-      <c r="J19" s="48"/>
-      <c r="K19" s="183" t="s">
-        <v>346</v>
-      </c>
-      <c r="L19" s="94"/>
-      <c r="M19" s="94"/>
-      <c r="N19" s="19"/>
       <c r="O19" s="91"/>
       <c r="P19" s="48">
         <v>15</v>
@@ -14405,7 +14425,7 @@
         <v>17</v>
       </c>
       <c r="T19" s="66" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
     </row>
     <row r="20" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -14424,25 +14444,25 @@
       <c r="E20" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="F20" s="48" t="s">
+      <c r="F20" s="183" t="s">
         <v>520</v>
       </c>
-      <c r="G20" s="48">
+      <c r="G20" s="48"/>
+      <c r="H20" s="183" t="s">
+        <v>346</v>
+      </c>
+      <c r="I20" s="94"/>
+      <c r="J20" s="94"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="48">
         <v>8</v>
       </c>
-      <c r="H20" s="48">
+      <c r="M20" s="48">
         <v>8</v>
       </c>
-      <c r="I20" s="48">
+      <c r="N20" s="48">
         <v>0</v>
       </c>
-      <c r="J20" s="48"/>
-      <c r="K20" s="183" t="s">
-        <v>346</v>
-      </c>
-      <c r="L20" s="94"/>
-      <c r="M20" s="94"/>
-      <c r="N20" s="19"/>
       <c r="O20" s="91"/>
       <c r="P20" s="48">
         <v>18</v>
@@ -14474,25 +14494,25 @@
       <c r="E21" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="F21" s="48" t="s">
+      <c r="F21" s="183" t="s">
         <v>521</v>
       </c>
-      <c r="G21" s="48">
+      <c r="G21" s="48"/>
+      <c r="H21" s="183" t="s">
+        <v>346</v>
+      </c>
+      <c r="I21" s="94"/>
+      <c r="J21" s="94"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="48">
         <v>21</v>
       </c>
-      <c r="H21" s="48">
-        <v>15</v>
-      </c>
-      <c r="I21" s="48">
+      <c r="M21" s="48">
+        <v>17</v>
+      </c>
+      <c r="N21" s="48">
         <v>4</v>
       </c>
-      <c r="J21" s="48"/>
-      <c r="K21" s="183" t="s">
-        <v>346</v>
-      </c>
-      <c r="L21" s="94"/>
-      <c r="M21" s="94"/>
-      <c r="N21" s="19"/>
       <c r="O21" s="91"/>
       <c r="P21" s="48">
         <v>22</v>
@@ -14507,7 +14527,7 @@
         <v>21</v>
       </c>
       <c r="T21" s="66" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
     </row>
     <row r="22" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -14526,25 +14546,25 @@
       <c r="E22" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="F22" s="48" t="s">
+      <c r="F22" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="G22" s="48">
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J22" s="94"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="48">
         <v>4</v>
       </c>
-      <c r="H22" s="48">
+      <c r="M22" s="48">
         <v>0</v>
       </c>
-      <c r="I22" s="48">
+      <c r="N22" s="48">
         <v>0</v>
       </c>
-      <c r="J22" s="48"/>
-      <c r="K22" s="48"/>
-      <c r="L22" s="34" t="s">
-        <v>346</v>
-      </c>
-      <c r="M22" s="94"/>
-      <c r="N22" s="19"/>
       <c r="O22" s="91"/>
       <c r="P22" s="48">
         <v>15</v>
@@ -14576,25 +14596,25 @@
       <c r="E23" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="F23" s="48" t="s">
+      <c r="F23" s="183" t="s">
         <v>523</v>
       </c>
-      <c r="G23" s="48">
+      <c r="G23" s="48"/>
+      <c r="H23" s="183" t="s">
+        <v>346</v>
+      </c>
+      <c r="I23" s="94"/>
+      <c r="J23" s="94"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="2">
         <v>95</v>
       </c>
-      <c r="H23" s="48">
+      <c r="M23" s="48">
         <v>80</v>
       </c>
-      <c r="I23" s="48">
+      <c r="N23" s="48">
         <v>0</v>
       </c>
-      <c r="J23" s="48"/>
-      <c r="K23" s="183" t="s">
-        <v>346</v>
-      </c>
-      <c r="L23" s="94"/>
-      <c r="M23" s="94"/>
-      <c r="N23" s="19"/>
       <c r="O23" s="91"/>
       <c r="P23" s="48">
         <v>11</v>
@@ -14609,7 +14629,7 @@
         <v>95</v>
       </c>
       <c r="T23" s="66" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="24" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -14628,25 +14648,25 @@
       <c r="E24" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="F24" s="48" t="s">
+      <c r="F24" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="G24" s="48">
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J24" s="94"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="48">
         <v>29</v>
       </c>
-      <c r="H24" s="48">
+      <c r="M24" s="48">
         <v>21</v>
       </c>
-      <c r="I24" s="48">
+      <c r="N24" s="48">
         <v>5</v>
       </c>
-      <c r="J24" s="48"/>
-      <c r="K24" s="48"/>
-      <c r="L24" s="34" t="s">
-        <v>346</v>
-      </c>
-      <c r="M24" s="94"/>
-      <c r="N24" s="19"/>
       <c r="O24" s="91"/>
       <c r="P24" s="48">
         <v>33</v>
@@ -14661,7 +14681,7 @@
         <v>29</v>
       </c>
       <c r="T24" s="66" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="25" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -14680,34 +14700,34 @@
       <c r="E25" s="18" t="s">
         <v>357</v>
       </c>
-      <c r="F25" s="190" t="s">
+      <c r="F25" s="29" t="s">
         <v>501</v>
       </c>
-      <c r="G25" s="29">
+      <c r="G25" s="191" t="s">
+        <v>545</v>
+      </c>
+      <c r="H25" s="85"/>
+      <c r="I25" s="85"/>
+      <c r="J25" s="74" t="s">
+        <v>346</v>
+      </c>
+      <c r="K25" s="19" t="s">
+        <v>568</v>
+      </c>
+      <c r="L25" s="29">
         <v>40</v>
       </c>
-      <c r="H25" s="29">
+      <c r="M25" s="29">
         <v>33</v>
       </c>
-      <c r="I25" s="29">
+      <c r="N25" s="29">
         <v>1</v>
       </c>
-      <c r="J25" s="194" t="s">
-        <v>547</v>
-      </c>
-      <c r="K25" s="85"/>
-      <c r="L25" s="85"/>
-      <c r="M25" s="74" t="s">
-        <v>346</v>
-      </c>
-      <c r="N25" s="19" t="s">
-        <v>531</v>
-      </c>
       <c r="O25" s="91"/>
-      <c r="P25" s="94" t="s">
+      <c r="P25" s="85" t="s">
         <v>510</v>
       </c>
-      <c r="Q25" s="200">
+      <c r="Q25" s="197">
         <v>0</v>
       </c>
     </row>
@@ -14727,27 +14747,27 @@
       <c r="E26" s="18" t="s">
         <v>361</v>
       </c>
-      <c r="F26" s="189" t="s">
+      <c r="F26" s="53" t="s">
         <v>470</v>
       </c>
-      <c r="G26" s="53">
+      <c r="G26" s="192" t="s">
+        <v>530</v>
+      </c>
+      <c r="H26" s="53"/>
+      <c r="I26" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J26" s="94"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="53">
         <v>8</v>
       </c>
-      <c r="H26" s="53">
+      <c r="M26" s="53">
         <v>5</v>
       </c>
-      <c r="I26" s="53">
+      <c r="N26" s="53">
         <v>1</v>
       </c>
-      <c r="J26" s="195" t="s">
-        <v>532</v>
-      </c>
-      <c r="K26" s="53"/>
-      <c r="L26" s="34" t="s">
-        <v>346</v>
-      </c>
-      <c r="M26" s="94"/>
-      <c r="N26" s="19"/>
       <c r="O26" s="91"/>
       <c r="P26" s="94">
         <v>12</v>
@@ -14772,28 +14792,28 @@
       <c r="E27" s="18" t="s">
         <v>365</v>
       </c>
-      <c r="F27" s="190" t="s">
+      <c r="F27" s="29" t="s">
         <v>471</v>
       </c>
-      <c r="G27" s="29">
+      <c r="G27" s="89" t="s">
+        <v>531</v>
+      </c>
+      <c r="H27" s="85"/>
+      <c r="I27" s="85"/>
+      <c r="J27" s="74" t="s">
+        <v>346</v>
+      </c>
+      <c r="K27" s="19" t="s">
+        <v>568</v>
+      </c>
+      <c r="L27" s="29">
         <v>1</v>
       </c>
-      <c r="H27" s="29">
+      <c r="M27" s="29">
         <v>0</v>
       </c>
-      <c r="I27" s="29">
+      <c r="N27" s="29">
         <v>0</v>
-      </c>
-      <c r="J27" s="89" t="s">
-        <v>533</v>
-      </c>
-      <c r="K27" s="85"/>
-      <c r="L27" s="85"/>
-      <c r="M27" s="74" t="s">
-        <v>346</v>
-      </c>
-      <c r="N27" s="19" t="s">
-        <v>531</v>
       </c>
       <c r="O27" s="91"/>
       <c r="P27" s="94">
@@ -14819,27 +14839,27 @@
       <c r="E28" s="18" t="s">
         <v>369</v>
       </c>
-      <c r="F28" s="189" t="s">
+      <c r="F28" s="53" t="s">
         <v>472</v>
       </c>
-      <c r="G28" s="53">
+      <c r="G28" s="192" t="s">
+        <v>532</v>
+      </c>
+      <c r="H28" s="53"/>
+      <c r="I28" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J28" s="94"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="53">
         <v>4</v>
       </c>
-      <c r="H28" s="53">
+      <c r="M28" s="53">
         <v>1</v>
       </c>
-      <c r="I28" s="53">
+      <c r="N28" s="53">
         <v>0</v>
       </c>
-      <c r="J28" s="195" t="s">
-        <v>534</v>
-      </c>
-      <c r="K28" s="53"/>
-      <c r="L28" s="34" t="s">
-        <v>346</v>
-      </c>
-      <c r="M28" s="94"/>
-      <c r="N28" s="19"/>
       <c r="O28" s="91"/>
       <c r="P28" s="94">
         <v>94</v>
@@ -14864,27 +14884,27 @@
       <c r="E29" s="18" t="s">
         <v>373</v>
       </c>
-      <c r="F29" s="190" t="s">
+      <c r="F29" s="184" t="s">
         <v>476</v>
       </c>
-      <c r="G29" s="29">
+      <c r="G29" s="191" t="s">
+        <v>561</v>
+      </c>
+      <c r="H29" s="184" t="s">
+        <v>346</v>
+      </c>
+      <c r="I29" s="94"/>
+      <c r="J29" s="94"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="29">
         <v>31</v>
       </c>
-      <c r="H29" s="29">
+      <c r="M29" s="29">
         <v>30</v>
       </c>
-      <c r="I29" s="29">
+      <c r="N29" s="29">
         <v>0</v>
       </c>
-      <c r="J29" s="194" t="s">
-        <v>565</v>
-      </c>
-      <c r="K29" s="184" t="s">
-        <v>346</v>
-      </c>
-      <c r="L29" s="94"/>
-      <c r="M29" s="94"/>
-      <c r="N29" s="19"/>
       <c r="O29" s="91"/>
       <c r="P29" s="94">
         <v>19</v>
@@ -14909,27 +14929,27 @@
       <c r="E30" s="18" t="s">
         <v>376</v>
       </c>
-      <c r="F30" s="190" t="s">
+      <c r="F30" s="29" t="s">
         <v>477</v>
       </c>
-      <c r="G30" s="29">
+      <c r="G30" s="193" t="s">
+        <v>533</v>
+      </c>
+      <c r="H30" s="94"/>
+      <c r="I30" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J30" s="94"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="29">
         <v>0</v>
       </c>
-      <c r="H30" s="29">
+      <c r="M30" s="29">
         <v>0</v>
       </c>
-      <c r="I30" s="29">
+      <c r="N30" s="29">
         <v>0</v>
       </c>
-      <c r="J30" s="196" t="s">
-        <v>535</v>
-      </c>
-      <c r="K30" s="94"/>
-      <c r="L30" s="34" t="s">
-        <v>346</v>
-      </c>
-      <c r="M30" s="94"/>
-      <c r="N30" s="19"/>
       <c r="O30" s="91"/>
       <c r="P30" s="94">
         <v>13</v>
@@ -14954,27 +14974,27 @@
       <c r="E31" s="18" t="s">
         <v>380</v>
       </c>
-      <c r="F31" s="190" t="s">
+      <c r="F31" s="29" t="s">
         <v>500</v>
       </c>
-      <c r="G31" s="29">
+      <c r="G31" s="191" t="s">
+        <v>534</v>
+      </c>
+      <c r="H31" s="29"/>
+      <c r="I31" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J31" s="94"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="29">
         <v>1</v>
       </c>
-      <c r="H31" s="29">
+      <c r="M31" s="29">
         <v>1</v>
       </c>
-      <c r="I31" s="29">
+      <c r="N31" s="29">
         <v>1</v>
       </c>
-      <c r="J31" s="194" t="s">
-        <v>536</v>
-      </c>
-      <c r="K31" s="29"/>
-      <c r="L31" s="34" t="s">
-        <v>346</v>
-      </c>
-      <c r="M31" s="94"/>
-      <c r="N31" s="19"/>
       <c r="O31" s="91"/>
       <c r="P31" s="94">
         <v>16</v>
@@ -14999,25 +15019,25 @@
       <c r="E32" s="18" t="s">
         <v>384</v>
       </c>
-      <c r="F32" s="190" t="s">
+      <c r="F32" s="184" t="s">
         <v>479</v>
       </c>
-      <c r="G32" s="29">
+      <c r="G32" s="191"/>
+      <c r="H32" s="184" t="s">
+        <v>346</v>
+      </c>
+      <c r="I32" s="94"/>
+      <c r="J32" s="94"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="29">
         <v>50</v>
       </c>
-      <c r="H32" s="29">
+      <c r="M32" s="29">
         <v>32</v>
       </c>
-      <c r="I32" s="29">
+      <c r="N32" s="29">
         <v>0</v>
       </c>
-      <c r="J32" s="194"/>
-      <c r="K32" s="184" t="s">
-        <v>346</v>
-      </c>
-      <c r="L32" s="94"/>
-      <c r="M32" s="94"/>
-      <c r="N32" s="19"/>
       <c r="O32" s="91"/>
       <c r="P32" s="94">
         <v>26</v>
@@ -15042,27 +15062,27 @@
       <c r="E33" s="18" t="s">
         <v>388</v>
       </c>
-      <c r="F33" s="190" t="s">
+      <c r="F33" s="184" t="s">
         <v>480</v>
       </c>
-      <c r="G33" s="29">
+      <c r="G33" s="191" t="s">
+        <v>562</v>
+      </c>
+      <c r="H33" s="184" t="s">
+        <v>346</v>
+      </c>
+      <c r="I33" s="94"/>
+      <c r="J33" s="94"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="29">
         <v>5</v>
       </c>
-      <c r="H33" s="29">
+      <c r="M33" s="29">
         <v>4</v>
       </c>
-      <c r="I33" s="29">
+      <c r="N33" s="29">
         <v>1</v>
       </c>
-      <c r="J33" s="194" t="s">
-        <v>566</v>
-      </c>
-      <c r="K33" s="184" t="s">
-        <v>346</v>
-      </c>
-      <c r="L33" s="94"/>
-      <c r="M33" s="94"/>
-      <c r="N33" s="19"/>
       <c r="O33" s="91"/>
       <c r="P33" s="94">
         <v>21</v>
@@ -15087,30 +15107,30 @@
       <c r="E34" s="18" t="s">
         <v>392</v>
       </c>
-      <c r="F34" s="190" t="s">
+      <c r="F34" s="184" t="s">
         <v>499</v>
       </c>
-      <c r="G34" s="29">
+      <c r="G34" s="191" t="s">
+        <v>535</v>
+      </c>
+      <c r="H34" s="184" t="s">
+        <v>346</v>
+      </c>
+      <c r="I34" s="94"/>
+      <c r="J34" s="185" t="s">
+        <v>346</v>
+      </c>
+      <c r="K34" s="189" t="s">
+        <v>528</v>
+      </c>
+      <c r="L34" s="29">
         <v>55</v>
       </c>
-      <c r="H34" s="29">
+      <c r="M34" s="29">
         <v>51</v>
       </c>
-      <c r="I34" s="29">
+      <c r="N34" s="29">
         <v>4</v>
-      </c>
-      <c r="J34" s="194" t="s">
-        <v>537</v>
-      </c>
-      <c r="K34" s="184" t="s">
-        <v>346</v>
-      </c>
-      <c r="L34" s="94"/>
-      <c r="M34" s="185" t="s">
-        <v>346</v>
-      </c>
-      <c r="N34" s="192" t="s">
-        <v>528</v>
       </c>
       <c r="O34" s="91"/>
       <c r="P34" s="94">
@@ -15136,27 +15156,27 @@
       <c r="E35" s="18" t="s">
         <v>396</v>
       </c>
-      <c r="F35" s="190" t="s">
+      <c r="F35" s="29" t="s">
         <v>481</v>
       </c>
-      <c r="G35" s="29">
+      <c r="G35" s="193" t="s">
+        <v>536</v>
+      </c>
+      <c r="H35" s="94"/>
+      <c r="I35" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J35" s="94"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="29">
         <v>4</v>
       </c>
-      <c r="H35" s="29">
+      <c r="M35" s="29">
         <v>1</v>
       </c>
-      <c r="I35" s="29">
+      <c r="N35" s="29">
         <v>1</v>
       </c>
-      <c r="J35" s="196" t="s">
-        <v>538</v>
-      </c>
-      <c r="K35" s="94"/>
-      <c r="L35" s="34" t="s">
-        <v>346</v>
-      </c>
-      <c r="M35" s="94"/>
-      <c r="N35" s="19"/>
       <c r="O35" s="91"/>
       <c r="P35" s="94">
         <v>18</v>
@@ -15181,27 +15201,27 @@
       <c r="E36" s="18" t="s">
         <v>401</v>
       </c>
-      <c r="F36" s="190" t="s">
+      <c r="F36" s="184" t="s">
         <v>482</v>
       </c>
-      <c r="G36" s="29">
+      <c r="G36" s="193" t="s">
+        <v>537</v>
+      </c>
+      <c r="H36" s="184" t="s">
+        <v>346</v>
+      </c>
+      <c r="I36" s="94"/>
+      <c r="J36" s="94"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="29">
         <v>5</v>
       </c>
-      <c r="H36" s="29">
+      <c r="M36" s="29">
         <v>4</v>
       </c>
-      <c r="I36" s="29">
+      <c r="N36" s="29">
         <v>1</v>
       </c>
-      <c r="J36" s="196" t="s">
-        <v>539</v>
-      </c>
-      <c r="K36" s="184" t="s">
-        <v>346</v>
-      </c>
-      <c r="L36" s="94"/>
-      <c r="M36" s="94"/>
-      <c r="N36" s="19"/>
       <c r="O36" s="91"/>
       <c r="P36" s="94">
         <v>45</v>
@@ -15226,27 +15246,27 @@
       <c r="E37" s="18" t="s">
         <v>401</v>
       </c>
-      <c r="F37" s="190" t="s">
+      <c r="F37" s="184" t="s">
         <v>483</v>
       </c>
-      <c r="G37" s="29">
+      <c r="G37" s="193" t="s">
+        <v>544</v>
+      </c>
+      <c r="H37" s="184" t="s">
+        <v>346</v>
+      </c>
+      <c r="I37" s="94"/>
+      <c r="J37" s="94"/>
+      <c r="K37" s="19"/>
+      <c r="L37" s="29">
         <v>3</v>
       </c>
-      <c r="H37" s="29">
+      <c r="M37" s="29">
         <v>2</v>
       </c>
-      <c r="I37" s="29">
+      <c r="N37" s="29">
         <v>0</v>
       </c>
-      <c r="J37" s="196" t="s">
-        <v>546</v>
-      </c>
-      <c r="K37" s="184" t="s">
-        <v>346</v>
-      </c>
-      <c r="L37" s="94"/>
-      <c r="M37" s="94"/>
-      <c r="N37" s="19"/>
       <c r="O37" s="91"/>
       <c r="P37" s="94">
         <v>28</v>
@@ -15271,27 +15291,27 @@
       <c r="E38" s="18" t="s">
         <v>408</v>
       </c>
-      <c r="F38" s="190" t="s">
+      <c r="F38" s="184" t="s">
         <v>484</v>
       </c>
-      <c r="G38" s="29">
+      <c r="G38" s="193" t="s">
+        <v>563</v>
+      </c>
+      <c r="H38" s="184" t="s">
+        <v>346</v>
+      </c>
+      <c r="I38" s="94"/>
+      <c r="J38" s="94"/>
+      <c r="K38" s="19"/>
+      <c r="L38" s="29">
         <v>14</v>
       </c>
-      <c r="H38" s="29">
+      <c r="M38" s="29">
         <v>15</v>
       </c>
-      <c r="I38" s="29">
+      <c r="N38" s="29">
         <v>3</v>
       </c>
-      <c r="J38" s="196" t="s">
-        <v>567</v>
-      </c>
-      <c r="K38" s="184" t="s">
-        <v>346</v>
-      </c>
-      <c r="L38" s="94"/>
-      <c r="M38" s="94"/>
-      <c r="N38" s="19"/>
       <c r="O38" s="91"/>
       <c r="P38" s="94">
         <v>14</v>
@@ -15316,25 +15336,25 @@
       <c r="E39" s="18" t="s">
         <v>412</v>
       </c>
-      <c r="F39" s="190" t="s">
+      <c r="F39" s="184" t="s">
         <v>498</v>
       </c>
-      <c r="G39" s="29">
+      <c r="G39" s="191"/>
+      <c r="H39" s="184" t="s">
+        <v>346</v>
+      </c>
+      <c r="I39" s="94"/>
+      <c r="J39" s="94"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="29">
         <v>1</v>
       </c>
-      <c r="H39" s="29">
+      <c r="M39" s="29">
         <v>2</v>
       </c>
-      <c r="I39" s="29">
+      <c r="N39" s="29">
         <v>2</v>
       </c>
-      <c r="J39" s="194"/>
-      <c r="K39" s="184" t="s">
-        <v>346</v>
-      </c>
-      <c r="L39" s="94"/>
-      <c r="M39" s="94"/>
-      <c r="N39" s="19"/>
       <c r="O39" s="91"/>
       <c r="P39" s="94">
         <v>5</v>
@@ -15359,27 +15379,27 @@
       <c r="E40" s="18" t="s">
         <v>420</v>
       </c>
-      <c r="F40" s="190" t="s">
+      <c r="F40" s="184" t="s">
         <v>485</v>
       </c>
-      <c r="G40" s="29">
+      <c r="G40" s="193" t="s">
+        <v>546</v>
+      </c>
+      <c r="H40" s="184" t="s">
+        <v>346</v>
+      </c>
+      <c r="I40" s="94"/>
+      <c r="J40" s="94"/>
+      <c r="K40" s="19"/>
+      <c r="L40" s="29">
         <v>58</v>
       </c>
-      <c r="H40" s="29">
+      <c r="M40" s="29">
         <v>39</v>
       </c>
-      <c r="I40" s="29">
+      <c r="N40" s="29">
         <v>5</v>
       </c>
-      <c r="J40" s="196" t="s">
-        <v>548</v>
-      </c>
-      <c r="K40" s="184" t="s">
-        <v>346</v>
-      </c>
-      <c r="L40" s="94"/>
-      <c r="M40" s="94"/>
-      <c r="N40" s="19"/>
       <c r="O40" s="91"/>
       <c r="P40" s="94">
         <v>15</v>
@@ -15404,30 +15424,30 @@
       <c r="E41" s="18" t="s">
         <v>418</v>
       </c>
-      <c r="F41" s="190" t="s">
+      <c r="F41" s="184" t="s">
         <v>497</v>
       </c>
-      <c r="G41" s="29">
+      <c r="G41" s="191" t="s">
+        <v>538</v>
+      </c>
+      <c r="H41" s="184" t="s">
+        <v>346</v>
+      </c>
+      <c r="I41" s="94"/>
+      <c r="J41" s="185" t="s">
+        <v>346</v>
+      </c>
+      <c r="K41" s="189" t="s">
+        <v>527</v>
+      </c>
+      <c r="L41" s="29">
         <v>1</v>
       </c>
-      <c r="H41" s="29">
+      <c r="M41" s="29">
         <v>0</v>
       </c>
-      <c r="I41" s="29">
+      <c r="N41" s="29">
         <v>0</v>
-      </c>
-      <c r="J41" s="194" t="s">
-        <v>540</v>
-      </c>
-      <c r="K41" s="184" t="s">
-        <v>346</v>
-      </c>
-      <c r="L41" s="94"/>
-      <c r="M41" s="185" t="s">
-        <v>346</v>
-      </c>
-      <c r="N41" s="192" t="s">
-        <v>527</v>
       </c>
       <c r="O41" s="91"/>
       <c r="P41" s="94">
@@ -15453,27 +15473,27 @@
       <c r="E42" s="18" t="s">
         <v>424</v>
       </c>
-      <c r="F42" s="190" t="s">
+      <c r="F42" s="184" t="s">
         <v>506</v>
       </c>
-      <c r="G42" s="29">
+      <c r="G42" s="193" t="s">
+        <v>539</v>
+      </c>
+      <c r="H42" s="184" t="s">
+        <v>346</v>
+      </c>
+      <c r="I42" s="94"/>
+      <c r="J42" s="94"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="29">
         <v>17</v>
       </c>
-      <c r="H42" s="29">
+      <c r="M42" s="29">
         <v>10</v>
       </c>
-      <c r="I42" s="29">
+      <c r="N42" s="29">
         <v>2</v>
       </c>
-      <c r="J42" s="196" t="s">
-        <v>541</v>
-      </c>
-      <c r="K42" s="184" t="s">
-        <v>346</v>
-      </c>
-      <c r="L42" s="94"/>
-      <c r="M42" s="94"/>
-      <c r="N42" s="19"/>
       <c r="O42" s="91"/>
       <c r="P42" s="94">
         <v>31</v>
@@ -15498,27 +15518,27 @@
       <c r="E43" s="18" t="s">
         <v>424</v>
       </c>
-      <c r="F43" s="191" t="s">
+      <c r="F43" s="98" t="s">
         <v>496</v>
       </c>
-      <c r="G43" s="198">
+      <c r="G43" s="194" t="s">
+        <v>540</v>
+      </c>
+      <c r="H43" s="98"/>
+      <c r="I43" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J43" s="94"/>
+      <c r="K43" s="19"/>
+      <c r="L43" s="195">
         <v>6</v>
       </c>
-      <c r="H43" s="98">
+      <c r="M43" s="98">
         <v>1</v>
       </c>
-      <c r="I43" s="98">
+      <c r="N43" s="98">
         <v>1</v>
       </c>
-      <c r="J43" s="197" t="s">
-        <v>542</v>
-      </c>
-      <c r="K43" s="98"/>
-      <c r="L43" s="34" t="s">
-        <v>346</v>
-      </c>
-      <c r="M43" s="94"/>
-      <c r="N43" s="19"/>
       <c r="O43" s="91"/>
       <c r="P43" s="94">
         <v>15</v>
@@ -15543,25 +15563,25 @@
       <c r="E44" s="18" t="s">
         <v>430</v>
       </c>
-      <c r="F44" s="190" t="s">
+      <c r="F44" s="184" t="s">
         <v>486</v>
       </c>
-      <c r="G44" s="193">
+      <c r="G44" s="6"/>
+      <c r="H44" s="184" t="s">
+        <v>346</v>
+      </c>
+      <c r="I44" s="94"/>
+      <c r="J44" s="94"/>
+      <c r="K44" s="19"/>
+      <c r="L44" s="190">
         <v>69</v>
       </c>
-      <c r="H44" s="29">
+      <c r="M44" s="29">
         <v>51</v>
       </c>
-      <c r="I44" s="29">
+      <c r="N44" s="29">
         <v>5</v>
       </c>
-      <c r="J44" s="6"/>
-      <c r="K44" s="184" t="s">
-        <v>346</v>
-      </c>
-      <c r="L44" s="94"/>
-      <c r="M44" s="94"/>
-      <c r="N44" s="19"/>
       <c r="O44" s="91"/>
       <c r="P44" s="94">
         <v>7</v>
@@ -15586,27 +15606,27 @@
       <c r="E45" s="18" t="s">
         <v>434</v>
       </c>
-      <c r="F45" s="190" t="s">
+      <c r="F45" s="29" t="s">
         <v>487</v>
       </c>
-      <c r="G45" s="29">
+      <c r="G45" s="193" t="s">
+        <v>541</v>
+      </c>
+      <c r="H45" s="94"/>
+      <c r="I45" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J45" s="94"/>
+      <c r="K45" s="19"/>
+      <c r="L45" s="29">
         <v>17</v>
       </c>
-      <c r="H45" s="29">
+      <c r="M45" s="29">
         <v>10</v>
       </c>
-      <c r="I45" s="29">
+      <c r="N45" s="29">
         <v>2</v>
       </c>
-      <c r="J45" s="196" t="s">
-        <v>543</v>
-      </c>
-      <c r="K45" s="94"/>
-      <c r="L45" s="34" t="s">
-        <v>346</v>
-      </c>
-      <c r="M45" s="94"/>
-      <c r="N45" s="19"/>
       <c r="O45" s="91"/>
       <c r="P45" s="94">
         <v>7</v>
@@ -15631,27 +15651,27 @@
       <c r="E46" s="18" t="s">
         <v>438</v>
       </c>
-      <c r="F46" s="190" t="s">
+      <c r="F46" s="29" t="s">
         <v>495</v>
       </c>
-      <c r="G46" s="29">
+      <c r="G46" s="191" t="s">
+        <v>548</v>
+      </c>
+      <c r="H46" s="29"/>
+      <c r="I46" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J46" s="94"/>
+      <c r="K46" s="19"/>
+      <c r="L46" s="29">
         <v>15</v>
       </c>
-      <c r="H46" s="29">
+      <c r="M46" s="29">
         <v>14</v>
       </c>
-      <c r="I46" s="29">
+      <c r="N46" s="29">
         <v>2</v>
       </c>
-      <c r="J46" s="194" t="s">
-        <v>550</v>
-      </c>
-      <c r="K46" s="29"/>
-      <c r="L46" s="34" t="s">
-        <v>346</v>
-      </c>
-      <c r="M46" s="94"/>
-      <c r="N46" s="19"/>
       <c r="O46" s="91"/>
       <c r="P46" s="94">
         <v>14</v>
@@ -15676,27 +15696,27 @@
       <c r="E47" s="18" t="s">
         <v>441</v>
       </c>
-      <c r="F47" s="190" t="s">
+      <c r="F47" s="29" t="s">
         <v>494</v>
       </c>
-      <c r="G47" s="29">
+      <c r="G47" s="191" t="s">
+        <v>533</v>
+      </c>
+      <c r="H47" s="29"/>
+      <c r="I47" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J47" s="94"/>
+      <c r="K47" s="19"/>
+      <c r="L47" s="29">
         <v>0</v>
       </c>
-      <c r="H47" s="29">
+      <c r="M47" s="29">
         <v>0</v>
       </c>
-      <c r="I47" s="29">
+      <c r="N47" s="29">
         <v>0</v>
       </c>
-      <c r="J47" s="194" t="s">
-        <v>535</v>
-      </c>
-      <c r="K47" s="29"/>
-      <c r="L47" s="34" t="s">
-        <v>346</v>
-      </c>
-      <c r="M47" s="94"/>
-      <c r="N47" s="19"/>
       <c r="O47" s="91"/>
       <c r="P47" s="94">
         <v>27</v>
@@ -15721,28 +15741,28 @@
       <c r="E48" s="18" t="s">
         <v>408</v>
       </c>
-      <c r="F48" s="190" t="s">
+      <c r="F48" s="29" t="s">
         <v>488</v>
       </c>
-      <c r="G48" s="29">
+      <c r="G48" s="193" t="s">
+        <v>544</v>
+      </c>
+      <c r="H48" s="85"/>
+      <c r="I48" s="85"/>
+      <c r="J48" s="85" t="s">
+        <v>346</v>
+      </c>
+      <c r="K48" s="19" t="s">
+        <v>568</v>
+      </c>
+      <c r="L48" s="29">
         <v>11</v>
       </c>
-      <c r="H48" s="29">
+      <c r="M48" s="29">
         <v>10</v>
       </c>
-      <c r="I48" s="29">
+      <c r="N48" s="29">
         <v>2</v>
-      </c>
-      <c r="J48" s="196" t="s">
-        <v>546</v>
-      </c>
-      <c r="K48" s="85"/>
-      <c r="L48" s="85"/>
-      <c r="M48" s="53" t="s">
-        <v>346</v>
-      </c>
-      <c r="N48" s="19" t="s">
-        <v>531</v>
       </c>
       <c r="O48" s="91"/>
       <c r="P48" s="94">
@@ -15768,27 +15788,27 @@
       <c r="E49" s="18" t="s">
         <v>448</v>
       </c>
-      <c r="F49" s="190" t="s">
+      <c r="F49" s="29" t="s">
         <v>489</v>
       </c>
-      <c r="G49" s="29">
+      <c r="G49" s="191" t="s">
+        <v>542</v>
+      </c>
+      <c r="H49" s="29"/>
+      <c r="I49" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J49" s="94"/>
+      <c r="K49" s="19"/>
+      <c r="L49" s="29">
         <v>4</v>
       </c>
-      <c r="H49" s="29">
+      <c r="M49" s="29">
         <v>3</v>
       </c>
-      <c r="I49" s="29">
+      <c r="N49" s="29">
         <v>0</v>
       </c>
-      <c r="J49" s="194" t="s">
-        <v>544</v>
-      </c>
-      <c r="K49" s="29"/>
-      <c r="L49" s="34" t="s">
-        <v>346</v>
-      </c>
-      <c r="M49" s="94"/>
-      <c r="N49" s="19"/>
       <c r="O49" s="91"/>
       <c r="P49" s="94">
         <v>19</v>
@@ -15813,27 +15833,27 @@
       <c r="E50" s="18" t="s">
         <v>455</v>
       </c>
-      <c r="F50" s="190" t="s">
+      <c r="F50" s="184" t="s">
         <v>490</v>
       </c>
-      <c r="G50" s="29">
+      <c r="G50" s="191" t="s">
+        <v>534</v>
+      </c>
+      <c r="H50" s="184" t="s">
+        <v>346</v>
+      </c>
+      <c r="I50" s="94"/>
+      <c r="J50" s="94"/>
+      <c r="K50" s="19"/>
+      <c r="L50" s="29">
         <v>1</v>
       </c>
-      <c r="H50" s="29">
+      <c r="M50" s="29">
         <v>1</v>
       </c>
-      <c r="I50" s="29">
+      <c r="N50" s="29">
         <v>0</v>
       </c>
-      <c r="J50" s="194" t="s">
-        <v>536</v>
-      </c>
-      <c r="K50" s="184" t="s">
-        <v>346</v>
-      </c>
-      <c r="L50" s="94"/>
-      <c r="M50" s="94"/>
-      <c r="N50" s="19"/>
       <c r="O50" s="91"/>
       <c r="P50" s="94">
         <v>13</v>
@@ -15858,25 +15878,25 @@
       <c r="E51" s="18" t="s">
         <v>457</v>
       </c>
-      <c r="F51" s="190" t="s">
+      <c r="F51" s="184" t="s">
         <v>493</v>
       </c>
-      <c r="G51" s="29">
+      <c r="G51" s="191"/>
+      <c r="H51" s="184" t="s">
+        <v>346</v>
+      </c>
+      <c r="I51" s="94"/>
+      <c r="J51" s="94"/>
+      <c r="K51" s="19"/>
+      <c r="L51" s="29">
         <v>5</v>
       </c>
-      <c r="H51" s="29">
+      <c r="M51" s="29">
         <v>4</v>
       </c>
-      <c r="I51" s="29">
+      <c r="N51" s="29">
         <v>2</v>
       </c>
-      <c r="J51" s="194"/>
-      <c r="K51" s="184" t="s">
-        <v>346</v>
-      </c>
-      <c r="L51" s="94"/>
-      <c r="M51" s="94"/>
-      <c r="N51" s="19"/>
       <c r="O51" s="91"/>
       <c r="P51" s="94">
         <v>8</v>
@@ -15901,23 +15921,27 @@
       <c r="E52" s="18" t="s">
         <v>460</v>
       </c>
-      <c r="F52" s="85" t="s">
+      <c r="F52" s="29" t="s">
         <v>491</v>
       </c>
-      <c r="G52" s="29">
+      <c r="G52" s="191" t="s">
+        <v>543</v>
+      </c>
+      <c r="H52" s="29"/>
+      <c r="I52" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J52" s="94"/>
+      <c r="K52" s="19"/>
+      <c r="L52" s="29">
         <v>84</v>
       </c>
-      <c r="H52" s="85"/>
-      <c r="I52" s="29"/>
-      <c r="J52" s="194" t="s">
-        <v>545</v>
-      </c>
-      <c r="K52" s="29"/>
-      <c r="L52" s="34" t="s">
-        <v>346</v>
-      </c>
-      <c r="M52" s="94"/>
-      <c r="N52" s="19"/>
+      <c r="M52" s="29">
+        <v>66</v>
+      </c>
+      <c r="N52" s="29">
+        <v>2</v>
+      </c>
       <c r="O52" s="91"/>
       <c r="P52" s="94">
         <v>13</v>
@@ -15942,27 +15966,27 @@
       <c r="E53" s="18" t="s">
         <v>420</v>
       </c>
-      <c r="F53" s="190" t="s">
+      <c r="F53" s="184" t="s">
         <v>492</v>
       </c>
-      <c r="G53" s="29">
+      <c r="G53" s="191" t="s">
+        <v>547</v>
+      </c>
+      <c r="H53" s="184" t="s">
+        <v>346</v>
+      </c>
+      <c r="I53" s="94"/>
+      <c r="J53" s="94"/>
+      <c r="K53" s="19"/>
+      <c r="L53" s="29">
         <v>37</v>
       </c>
-      <c r="H53" s="29">
+      <c r="M53" s="29">
         <v>28</v>
       </c>
-      <c r="I53" s="29">
+      <c r="N53" s="29">
         <v>4</v>
       </c>
-      <c r="J53" s="194" t="s">
-        <v>549</v>
-      </c>
-      <c r="K53" s="184" t="s">
-        <v>346</v>
-      </c>
-      <c r="L53" s="94"/>
-      <c r="M53" s="94"/>
-      <c r="N53" s="19"/>
       <c r="O53" s="91"/>
       <c r="P53" s="94">
         <v>10</v>
@@ -15972,7 +15996,11 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:Q1"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -15996,43 +16024,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="220" t="s">
+      <c r="A1" s="226" t="s">
         <v>230</v>
       </c>
-      <c r="B1" s="221"/>
-      <c r="C1" s="221"/>
-      <c r="D1" s="221"/>
-      <c r="E1" s="221"/>
-      <c r="F1" s="221"/>
-      <c r="G1" s="221"/>
-      <c r="H1" s="221"/>
-      <c r="I1" s="221"/>
+      <c r="B1" s="227"/>
+      <c r="C1" s="227"/>
+      <c r="D1" s="227"/>
+      <c r="E1" s="227"/>
+      <c r="F1" s="227"/>
+      <c r="G1" s="227"/>
+      <c r="H1" s="227"/>
+      <c r="I1" s="227"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="223" t="s">
+      <c r="A2" s="225" t="s">
         <v>229</v>
       </c>
-      <c r="B2" s="223"/>
-      <c r="C2" s="223"/>
-      <c r="D2" s="223"/>
-      <c r="E2" s="223"/>
-      <c r="F2" s="223"/>
-      <c r="G2" s="223"/>
-      <c r="H2" s="223"/>
-      <c r="I2" s="223"/>
+      <c r="B2" s="225"/>
+      <c r="C2" s="225"/>
+      <c r="D2" s="225"/>
+      <c r="E2" s="225"/>
+      <c r="F2" s="225"/>
+      <c r="G2" s="225"/>
+      <c r="H2" s="225"/>
+      <c r="I2" s="225"/>
     </row>
     <row r="3" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="224" t="s">
+      <c r="A3" s="218" t="s">
         <v>337</v>
       </c>
-      <c r="B3" s="224"/>
-      <c r="C3" s="224"/>
-      <c r="D3" s="224"/>
-      <c r="E3" s="224"/>
-      <c r="F3" s="224"/>
-      <c r="G3" s="224"/>
-      <c r="H3" s="224"/>
-      <c r="I3" s="224"/>
+      <c r="B3" s="218"/>
+      <c r="C3" s="218"/>
+      <c r="D3" s="218"/>
+      <c r="E3" s="218"/>
+      <c r="F3" s="218"/>
+      <c r="G3" s="218"/>
+      <c r="H3" s="218"/>
+      <c r="I3" s="218"/>
       <c r="J3" s="71"/>
       <c r="K3" s="71"/>
       <c r="L3" s="71"/>
@@ -16045,12 +16073,12 @@
       <c r="S3" s="71"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="222" t="s">
+      <c r="A4" s="228" t="s">
         <v>253</v>
       </c>
-      <c r="B4" s="222"/>
-      <c r="C4" s="222"/>
-      <c r="D4" s="222"/>
+      <c r="B4" s="228"/>
+      <c r="C4" s="228"/>
+      <c r="D4" s="228"/>
     </row>
     <row r="5" spans="1:19" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="69" t="s">
@@ -16076,7 +16104,7 @@
       <c r="C6" s="49" t="s">
         <v>196</v>
       </c>
-      <c r="D6" s="233" t="s">
+      <c r="D6" s="222" t="s">
         <v>339</v>
       </c>
       <c r="E6" t="e">
@@ -16095,7 +16123,7 @@
       <c r="C7" s="49" t="s">
         <v>228</v>
       </c>
-      <c r="D7" s="234"/>
+      <c r="D7" s="223"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="78" t="s">
@@ -16107,7 +16135,7 @@
       <c r="C8" s="49" t="s">
         <v>235</v>
       </c>
-      <c r="D8" s="234"/>
+      <c r="D8" s="223"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="78" t="s">
@@ -16119,7 +16147,7 @@
       <c r="C9" s="49" t="s">
         <v>236</v>
       </c>
-      <c r="D9" s="234"/>
+      <c r="D9" s="223"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="78" t="s">
@@ -16131,7 +16159,7 @@
       <c r="C10" s="49" t="s">
         <v>237</v>
       </c>
-      <c r="D10" s="234"/>
+      <c r="D10" s="223"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="78" t="s">
@@ -16143,7 +16171,7 @@
       <c r="C11" s="49" t="s">
         <v>237</v>
       </c>
-      <c r="D11" s="234"/>
+      <c r="D11" s="223"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="78" t="s">
@@ -16155,7 +16183,7 @@
       <c r="C12" s="49" t="s">
         <v>266</v>
       </c>
-      <c r="D12" s="234"/>
+      <c r="D12" s="223"/>
     </row>
     <row r="13" spans="1:19" s="77" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="145" t="s">
@@ -16167,7 +16195,7 @@
       <c r="C13" s="136" t="s">
         <v>273</v>
       </c>
-      <c r="D13" s="235"/>
+      <c r="D13" s="224"/>
     </row>
     <row r="14" spans="1:19" s="77" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="146" t="s">
@@ -16184,30 +16212,30 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="223" t="s">
+      <c r="A15" s="225" t="s">
         <v>261</v>
       </c>
-      <c r="B15" s="223"/>
-      <c r="C15" s="223"/>
-      <c r="D15" s="223"/>
-      <c r="E15" s="223"/>
-      <c r="F15" s="223"/>
-      <c r="G15" s="223"/>
-      <c r="H15" s="223"/>
-      <c r="I15" s="223"/>
+      <c r="B15" s="225"/>
+      <c r="C15" s="225"/>
+      <c r="D15" s="225"/>
+      <c r="E15" s="225"/>
+      <c r="F15" s="225"/>
+      <c r="G15" s="225"/>
+      <c r="H15" s="225"/>
+      <c r="I15" s="225"/>
     </row>
     <row r="16" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="224" t="s">
+      <c r="A16" s="218" t="s">
         <v>238</v>
       </c>
-      <c r="B16" s="224"/>
-      <c r="C16" s="224"/>
-      <c r="D16" s="224"/>
-      <c r="E16" s="224"/>
-      <c r="F16" s="224"/>
-      <c r="G16" s="224"/>
-      <c r="H16" s="224"/>
-      <c r="I16" s="224"/>
+      <c r="B16" s="218"/>
+      <c r="C16" s="218"/>
+      <c r="D16" s="218"/>
+      <c r="E16" s="218"/>
+      <c r="F16" s="218"/>
+      <c r="G16" s="218"/>
+      <c r="H16" s="218"/>
+      <c r="I16" s="218"/>
       <c r="J16" s="71"/>
       <c r="K16" s="71"/>
       <c r="L16" s="71"/>
@@ -16220,14 +16248,14 @@
       <c r="S16" s="71"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="222" t="s">
+      <c r="A17" s="228" t="s">
         <v>259</v>
       </c>
-      <c r="B17" s="222"/>
-      <c r="C17" s="222"/>
-      <c r="D17" s="222"/>
-      <c r="E17" s="222"/>
-      <c r="F17" s="222"/>
+      <c r="B17" s="228"/>
+      <c r="C17" s="228"/>
+      <c r="D17" s="228"/>
+      <c r="E17" s="228"/>
+      <c r="F17" s="228"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="69" t="s">
@@ -16394,30 +16422,30 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="223" t="s">
+      <c r="A25" s="225" t="s">
         <v>260</v>
       </c>
-      <c r="B25" s="223"/>
-      <c r="C25" s="223"/>
-      <c r="D25" s="223"/>
-      <c r="E25" s="223"/>
-      <c r="F25" s="223"/>
-      <c r="G25" s="223"/>
-      <c r="H25" s="223"/>
-      <c r="I25" s="223"/>
+      <c r="B25" s="225"/>
+      <c r="C25" s="225"/>
+      <c r="D25" s="225"/>
+      <c r="E25" s="225"/>
+      <c r="F25" s="225"/>
+      <c r="G25" s="225"/>
+      <c r="H25" s="225"/>
+      <c r="I25" s="225"/>
     </row>
     <row r="26" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="224" t="s">
+      <c r="A26" s="218" t="s">
         <v>338</v>
       </c>
-      <c r="B26" s="224"/>
-      <c r="C26" s="224"/>
-      <c r="D26" s="224"/>
-      <c r="E26" s="224"/>
-      <c r="F26" s="224"/>
-      <c r="G26" s="224"/>
-      <c r="H26" s="224"/>
-      <c r="I26" s="224"/>
+      <c r="B26" s="218"/>
+      <c r="C26" s="218"/>
+      <c r="D26" s="218"/>
+      <c r="E26" s="218"/>
+      <c r="F26" s="218"/>
+      <c r="G26" s="218"/>
+      <c r="H26" s="218"/>
+      <c r="I26" s="218"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="69" t="s">
@@ -16429,12 +16457,12 @@
       <c r="C27" s="69" t="s">
         <v>201</v>
       </c>
-      <c r="D27" s="228" t="s">
+      <c r="D27" s="232" t="s">
         <v>292</v>
       </c>
-      <c r="E27" s="228"/>
-      <c r="F27" s="228"/>
-      <c r="G27" s="228"/>
+      <c r="E27" s="232"/>
+      <c r="F27" s="232"/>
+      <c r="G27" s="232"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="52" t="s">
@@ -16446,12 +16474,12 @@
       <c r="C28" s="72">
         <v>0.59</v>
       </c>
-      <c r="D28" s="230" t="s">
+      <c r="D28" s="219" t="s">
         <v>285</v>
       </c>
-      <c r="E28" s="231"/>
-      <c r="F28" s="231"/>
-      <c r="G28" s="232"/>
+      <c r="E28" s="220"/>
+      <c r="F28" s="220"/>
+      <c r="G28" s="221"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="52" t="s">
@@ -16463,12 +16491,12 @@
       <c r="C29" s="72">
         <v>0.77</v>
       </c>
-      <c r="D29" s="225" t="s">
+      <c r="D29" s="229" t="s">
         <v>286</v>
       </c>
-      <c r="E29" s="226"/>
-      <c r="F29" s="226"/>
-      <c r="G29" s="227"/>
+      <c r="E29" s="230"/>
+      <c r="F29" s="230"/>
+      <c r="G29" s="231"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="52" t="s">
@@ -16480,12 +16508,12 @@
       <c r="C30" s="72">
         <v>0.41</v>
       </c>
-      <c r="D30" s="225" t="s">
+      <c r="D30" s="229" t="s">
         <v>287</v>
       </c>
-      <c r="E30" s="226"/>
-      <c r="F30" s="226"/>
-      <c r="G30" s="227"/>
+      <c r="E30" s="230"/>
+      <c r="F30" s="230"/>
+      <c r="G30" s="231"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="52" t="s">
@@ -16497,12 +16525,12 @@
       <c r="C31" s="72">
         <v>0.59</v>
       </c>
-      <c r="D31" s="225" t="s">
+      <c r="D31" s="229" t="s">
         <v>289</v>
       </c>
-      <c r="E31" s="226"/>
-      <c r="F31" s="226"/>
-      <c r="G31" s="227"/>
+      <c r="E31" s="230"/>
+      <c r="F31" s="230"/>
+      <c r="G31" s="231"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="52" t="s">
@@ -16514,12 +16542,12 @@
       <c r="C32" s="72">
         <v>0.5</v>
       </c>
-      <c r="D32" s="225" t="s">
+      <c r="D32" s="229" t="s">
         <v>288</v>
       </c>
-      <c r="E32" s="226"/>
-      <c r="F32" s="226"/>
-      <c r="G32" s="227"/>
+      <c r="E32" s="230"/>
+      <c r="F32" s="230"/>
+      <c r="G32" s="231"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="52" t="s">
@@ -16531,12 +16559,12 @@
       <c r="C33" s="72">
         <v>0.59</v>
       </c>
-      <c r="D33" s="225" t="s">
+      <c r="D33" s="229" t="s">
         <v>290</v>
       </c>
-      <c r="E33" s="226"/>
-      <c r="F33" s="226"/>
-      <c r="G33" s="227"/>
+      <c r="E33" s="230"/>
+      <c r="F33" s="230"/>
+      <c r="G33" s="231"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="52" t="s">
@@ -16548,25 +16576,25 @@
       <c r="C34" s="72">
         <v>0.54</v>
       </c>
-      <c r="D34" s="225" t="s">
+      <c r="D34" s="229" t="s">
         <v>291</v>
       </c>
-      <c r="E34" s="226"/>
-      <c r="F34" s="226"/>
-      <c r="G34" s="227"/>
+      <c r="E34" s="230"/>
+      <c r="F34" s="230"/>
+      <c r="G34" s="231"/>
     </row>
     <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="223" t="s">
+      <c r="A36" s="225" t="s">
         <v>315</v>
       </c>
-      <c r="B36" s="223"/>
-      <c r="C36" s="223"/>
-      <c r="D36" s="223"/>
-      <c r="E36" s="223"/>
-      <c r="F36" s="223"/>
-      <c r="G36" s="223"/>
-      <c r="H36" s="223"/>
-      <c r="I36" s="223"/>
+      <c r="B36" s="225"/>
+      <c r="C36" s="225"/>
+      <c r="D36" s="225"/>
+      <c r="E36" s="225"/>
+      <c r="F36" s="225"/>
+      <c r="G36" s="225"/>
+      <c r="H36" s="225"/>
+      <c r="I36" s="225"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="87" t="s">
@@ -16633,12 +16661,12 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="229" t="s">
+      <c r="A46" s="217" t="s">
         <v>318</v>
       </c>
-      <c r="B46" s="229"/>
-      <c r="C46" s="229"/>
-      <c r="D46" s="229"/>
+      <c r="B46" s="217"/>
+      <c r="C46" s="217"/>
+      <c r="D46" s="217"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="88" t="s">
@@ -16789,11 +16817,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="D28:G28"/>
-    <mergeCell ref="D6:D13"/>
-    <mergeCell ref="A2:I2"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="A25:I25"/>
@@ -16809,6 +16832,11 @@
     <mergeCell ref="D30:G30"/>
     <mergeCell ref="D31:G31"/>
     <mergeCell ref="D32:G32"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="D6:D13"/>
+    <mergeCell ref="A2:I2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -16840,15 +16868,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="241" t="s">
+      <c r="A1" s="238" t="s">
         <v>347</v>
       </c>
-      <c r="B1" s="241"/>
-      <c r="C1" s="241"/>
-      <c r="D1" s="241"/>
-      <c r="E1" s="241"/>
-      <c r="F1" s="241"/>
-      <c r="G1" s="241"/>
+      <c r="B1" s="238"/>
+      <c r="C1" s="238"/>
+      <c r="D1" s="238"/>
+      <c r="E1" s="238"/>
+      <c r="F1" s="238"/>
+      <c r="G1" s="238"/>
     </row>
     <row r="2" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="158" t="s">
@@ -16872,11 +16900,11 @@
       <c r="G2" s="158" t="s">
         <v>344</v>
       </c>
-      <c r="I2" s="240" t="s">
+      <c r="I2" s="237" t="s">
         <v>197</v>
       </c>
-      <c r="J2" s="240"/>
-      <c r="K2" s="240"/>
+      <c r="J2" s="237"/>
+      <c r="K2" s="237"/>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
@@ -17329,20 +17357,20 @@
       <c r="J22" s="115" t="s">
         <v>217</v>
       </c>
-      <c r="K22" s="242" t="s">
+      <c r="K22" s="239" t="s">
         <v>307</v>
       </c>
-      <c r="L22" s="242"/>
-      <c r="M22" s="242"/>
-      <c r="N22" s="242"/>
-      <c r="O22" s="242"/>
-      <c r="P22" s="242"/>
-      <c r="Q22" s="242"/>
-      <c r="R22" s="242"/>
-      <c r="S22" s="242"/>
-      <c r="T22" s="242"/>
-      <c r="U22" s="242"/>
-      <c r="V22" s="242"/>
+      <c r="L22" s="239"/>
+      <c r="M22" s="239"/>
+      <c r="N22" s="239"/>
+      <c r="O22" s="239"/>
+      <c r="P22" s="239"/>
+      <c r="Q22" s="239"/>
+      <c r="R22" s="239"/>
+      <c r="S22" s="239"/>
+      <c r="T22" s="239"/>
+      <c r="U22" s="239"/>
+      <c r="V22" s="239"/>
     </row>
     <row r="23" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="36" t="s">
@@ -17448,10 +17476,10 @@
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="244"/>
-      <c r="B29" s="245"/>
-      <c r="C29" s="245"/>
-      <c r="D29" s="246"/>
+      <c r="A29" s="241"/>
+      <c r="B29" s="242"/>
+      <c r="C29" s="242"/>
+      <c r="D29" s="243"/>
       <c r="I29" s="43" t="s">
         <v>187</v>
       </c>
@@ -17468,10 +17496,10 @@
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" s="247" t="s">
+      <c r="A31" s="244" t="s">
         <v>181</v>
       </c>
-      <c r="B31" s="248"/>
+      <c r="B31" s="245"/>
       <c r="C31" s="68"/>
       <c r="I31" s="43" t="s">
         <v>189</v>
@@ -17493,20 +17521,20 @@
       <c r="J32" s="116" t="s">
         <v>308</v>
       </c>
-      <c r="K32" s="243" t="s">
+      <c r="K32" s="240" t="s">
         <v>306</v>
       </c>
-      <c r="L32" s="243"/>
-      <c r="M32" s="243"/>
-      <c r="N32" s="243"/>
-      <c r="O32" s="243"/>
-      <c r="P32" s="243"/>
-      <c r="Q32" s="243"/>
-      <c r="R32" s="243"/>
-      <c r="S32" s="243"/>
-      <c r="T32" s="243"/>
-      <c r="U32" s="243"/>
-      <c r="V32" s="243"/>
+      <c r="L32" s="240"/>
+      <c r="M32" s="240"/>
+      <c r="N32" s="240"/>
+      <c r="O32" s="240"/>
+      <c r="P32" s="240"/>
+      <c r="Q32" s="240"/>
+      <c r="R32" s="240"/>
+      <c r="S32" s="240"/>
+      <c r="T32" s="240"/>
+      <c r="U32" s="240"/>
+      <c r="V32" s="240"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="84" t="s">
@@ -17539,10 +17567,10 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="236" t="s">
+      <c r="A35" s="233" t="s">
         <v>184</v>
       </c>
-      <c r="B35" s="238" t="s">
+      <c r="B35" s="235" t="s">
         <v>219</v>
       </c>
       <c r="D35" s="90"/>
@@ -17552,8 +17580,8 @@
       <c r="J35" s="41"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="237"/>
-      <c r="B36" s="239"/>
+      <c r="A36" s="234"/>
+      <c r="B36" s="236"/>
       <c r="D36" s="90"/>
       <c r="I36" s="105" t="s">
         <v>296</v>
@@ -17672,15 +17700,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="241" t="s">
+      <c r="A1" s="238" t="s">
         <v>347</v>
       </c>
-      <c r="B1" s="241"/>
-      <c r="C1" s="241"/>
-      <c r="D1" s="241"/>
-      <c r="E1" s="241"/>
-      <c r="F1" s="241"/>
-      <c r="G1" s="241"/>
+      <c r="B1" s="238"/>
+      <c r="C1" s="238"/>
+      <c r="D1" s="238"/>
+      <c r="E1" s="238"/>
+      <c r="F1" s="238"/>
+      <c r="G1" s="238"/>
     </row>
     <row r="2" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="158" t="s">
@@ -17704,11 +17732,11 @@
       <c r="G2" s="158" t="s">
         <v>344</v>
       </c>
-      <c r="I2" s="240" t="s">
+      <c r="I2" s="237" t="s">
         <v>197</v>
       </c>
-      <c r="J2" s="240"/>
-      <c r="K2" s="240"/>
+      <c r="J2" s="237"/>
+      <c r="K2" s="237"/>
       <c r="O2" s="170" t="s">
         <v>351</v>
       </c>
@@ -18209,20 +18237,20 @@
       <c r="J22" s="115" t="s">
         <v>217</v>
       </c>
-      <c r="K22" s="242" t="s">
+      <c r="K22" s="239" t="s">
         <v>307</v>
       </c>
-      <c r="L22" s="242"/>
-      <c r="M22" s="242"/>
-      <c r="N22" s="242"/>
-      <c r="O22" s="242"/>
-      <c r="P22" s="242"/>
-      <c r="Q22" s="242"/>
-      <c r="R22" s="242"/>
-      <c r="S22" s="242"/>
-      <c r="T22" s="242"/>
-      <c r="U22" s="242"/>
-      <c r="V22" s="242"/>
+      <c r="L22" s="239"/>
+      <c r="M22" s="239"/>
+      <c r="N22" s="239"/>
+      <c r="O22" s="239"/>
+      <c r="P22" s="239"/>
+      <c r="Q22" s="239"/>
+      <c r="R22" s="239"/>
+      <c r="S22" s="239"/>
+      <c r="T22" s="239"/>
+      <c r="U22" s="239"/>
+      <c r="V22" s="239"/>
     </row>
     <row r="23" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="36" t="s">
@@ -18328,10 +18356,10 @@
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="244"/>
-      <c r="B29" s="245"/>
-      <c r="C29" s="245"/>
-      <c r="D29" s="246"/>
+      <c r="A29" s="241"/>
+      <c r="B29" s="242"/>
+      <c r="C29" s="242"/>
+      <c r="D29" s="243"/>
       <c r="I29" s="43" t="s">
         <v>187</v>
       </c>
@@ -18348,10 +18376,10 @@
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" s="247" t="s">
+      <c r="A31" s="244" t="s">
         <v>181</v>
       </c>
-      <c r="B31" s="248"/>
+      <c r="B31" s="245"/>
       <c r="C31" s="68"/>
       <c r="I31" s="43" t="s">
         <v>189</v>
@@ -18373,20 +18401,20 @@
       <c r="J32" s="116" t="s">
         <v>308</v>
       </c>
-      <c r="K32" s="243" t="s">
+      <c r="K32" s="240" t="s">
         <v>306</v>
       </c>
-      <c r="L32" s="243"/>
-      <c r="M32" s="243"/>
-      <c r="N32" s="243"/>
-      <c r="O32" s="243"/>
-      <c r="P32" s="243"/>
-      <c r="Q32" s="243"/>
-      <c r="R32" s="243"/>
-      <c r="S32" s="243"/>
-      <c r="T32" s="243"/>
-      <c r="U32" s="243"/>
-      <c r="V32" s="243"/>
+      <c r="L32" s="240"/>
+      <c r="M32" s="240"/>
+      <c r="N32" s="240"/>
+      <c r="O32" s="240"/>
+      <c r="P32" s="240"/>
+      <c r="Q32" s="240"/>
+      <c r="R32" s="240"/>
+      <c r="S32" s="240"/>
+      <c r="T32" s="240"/>
+      <c r="U32" s="240"/>
+      <c r="V32" s="240"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="84" t="s">
@@ -18417,10 +18445,10 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="236" t="s">
+      <c r="A35" s="233" t="s">
         <v>184</v>
       </c>
-      <c r="B35" s="238" t="s">
+      <c r="B35" s="235" t="s">
         <v>219</v>
       </c>
       <c r="I35" s="43" t="s">
@@ -18429,8 +18457,8 @@
       <c r="J35" s="41"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="237"/>
-      <c r="B36" s="239"/>
+      <c r="A36" s="234"/>
+      <c r="B36" s="236"/>
       <c r="I36" s="105" t="s">
         <v>296</v>
       </c>
@@ -18532,18 +18560,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="249" t="s">
+      <c r="A1" s="246" t="s">
         <v>464</v>
       </c>
-      <c r="B1" s="249"/>
-      <c r="C1" s="249"/>
-      <c r="D1" s="249"/>
-      <c r="E1" s="249"/>
-      <c r="F1" s="249"/>
-      <c r="G1" s="249"/>
-      <c r="H1" s="249"/>
-      <c r="I1" s="249"/>
-      <c r="J1" s="249"/>
+      <c r="B1" s="246"/>
+      <c r="C1" s="246"/>
+      <c r="D1" s="246"/>
+      <c r="E1" s="246"/>
+      <c r="F1" s="246"/>
+      <c r="G1" s="246"/>
+      <c r="H1" s="246"/>
+      <c r="I1" s="246"/>
+      <c r="J1" s="246"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="173" t="s">

</xml_diff>

<commit_message>
inclusao de tags nos 30 selecionados
</commit_message>
<xml_diff>
--- a/Experiment01_Resumo/Resumo_Exp01.xlsx
+++ b/Experiment01_Resumo/Resumo_Exp01.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1494" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1525" uniqueCount="577">
   <si>
     <t>Database search</t>
   </si>
@@ -1849,6 +1849,27 @@
   </si>
   <si>
     <t>Resumo dos 51 estudos - JF Tool, Selecionados no Final, Excluídos, BSB, FSB</t>
+  </si>
+  <si>
+    <t>SPRINGER</t>
+  </si>
+  <si>
+    <t>WEB OF SCIENCE</t>
+  </si>
+  <si>
+    <t>SCOPUS</t>
+  </si>
+  <si>
+    <t>International Symposium on Empirical Software Engineering, ISESE 2005</t>
+  </si>
+  <si>
+    <t>ENG VILLAGE (EL COMPENDEX)</t>
+  </si>
+  <si>
+    <t>Coluna Fonte do review.xls Aba Análise (Francisco)</t>
+  </si>
+  <si>
+    <t>Existe na lista de resultado da Scopus do review.xls Aba Scopus (Francisco)</t>
   </si>
 </sst>
 </file>
@@ -1947,7 +1968,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="28">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2083,6 +2104,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3399"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2535,7 +2580,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="255">
+  <cellXfs count="264">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3055,6 +3100,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3103,12 +3175,39 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -3127,30 +3226,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3213,9 +3288,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3227,10 +3299,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF3399"/>
       <color rgb="FFFFCCCC"/>
       <color rgb="FFFF99FF"/>
       <color rgb="FFFF6699"/>
-      <color rgb="FFFF3399"/>
       <color rgb="FFFF66FF"/>
     </mruColors>
   </colors>
@@ -3540,12 +3612,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="191324120"/>
-        <c:axId val="191324512"/>
+        <c:axId val="191930280"/>
+        <c:axId val="191933416"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="191324120"/>
+        <c:axId val="191930280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3637,7 +3709,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="191324512"/>
+        <c:crossAx val="191933416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3645,7 +3717,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="191324512"/>
+        <c:axId val="191933416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3696,7 +3768,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="191324120"/>
+        <c:crossAx val="191930280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4005,12 +4077,12 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:shape val="box"/>
-        <c:axId val="221061384"/>
-        <c:axId val="221061776"/>
+        <c:axId val="191934200"/>
+        <c:axId val="191930672"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="221061384"/>
+        <c:axId val="191934200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4099,7 +4171,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="221061776"/>
+        <c:crossAx val="191930672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4107,7 +4179,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="221061776"/>
+        <c:axId val="191930672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4190,7 +4262,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="221061384"/>
+        <c:crossAx val="191934200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4475,12 +4547,12 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:shape val="box"/>
-        <c:axId val="221062560"/>
-        <c:axId val="221056288"/>
+        <c:axId val="191929496"/>
+        <c:axId val="191929888"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="221062560"/>
+        <c:axId val="191929496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4569,7 +4641,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="221056288"/>
+        <c:crossAx val="191929888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4577,7 +4649,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="221056288"/>
+        <c:axId val="191929888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4660,7 +4732,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="221062560"/>
+        <c:crossAx val="191929496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5447,12 +5519,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="221057072"/>
-        <c:axId val="221055504"/>
+        <c:axId val="191934984"/>
+        <c:axId val="191935376"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="221057072"/>
+        <c:axId val="191934984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5492,7 +5564,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="221055504"/>
+        <c:crossAx val="191935376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5500,7 +5572,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="221055504"/>
+        <c:axId val="191935376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5548,7 +5620,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="221057072"/>
+        <c:crossAx val="191934984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5856,8 +5928,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="221055112"/>
-        <c:axId val="221055896"/>
+        <c:axId val="192433040"/>
+        <c:axId val="192434608"/>
         <c:axId val="0"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -6027,7 +6099,7 @@
         </c:extLst>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="221055112"/>
+        <c:axId val="192433040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6125,7 +6197,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="221055896"/>
+        <c:crossAx val="192434608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6133,7 +6205,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="221055896"/>
+        <c:axId val="192434608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6212,7 +6284,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="221055112"/>
+        <c:crossAx val="192433040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6526,8 +6598,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="221059816"/>
-        <c:axId val="221060600"/>
+        <c:axId val="192439312"/>
+        <c:axId val="192431864"/>
         <c:axId val="0"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -6697,7 +6769,7 @@
         </c:extLst>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="221059816"/>
+        <c:axId val="192439312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6795,7 +6867,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="221060600"/>
+        <c:crossAx val="192431864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6803,7 +6875,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="221060600"/>
+        <c:axId val="192431864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6882,7 +6954,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="221059816"/>
+        <c:crossAx val="192439312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10580,22 +10652,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="201" t="s">
+      <c r="A1" s="210" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="202"/>
+      <c r="B1" s="211"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="203" t="s">
+      <c r="A2" s="212" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="204"/>
+      <c r="B2" s="213"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="203" t="s">
+      <c r="A3" s="212" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="204"/>
+      <c r="B3" s="213"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -10630,10 +10702,10 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="205" t="s">
+      <c r="A8" s="214" t="s">
         <v>103</v>
       </c>
-      <c r="B8" s="206"/>
+      <c r="B8" s="215"/>
     </row>
     <row r="9" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
@@ -10709,15 +10781,15 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="247" t="s">
+      <c r="A1" s="257" t="s">
         <v>525</v>
       </c>
-      <c r="B1" s="247"/>
-      <c r="C1" s="247"/>
-      <c r="D1" s="247"/>
-      <c r="E1" s="247"/>
-      <c r="F1" s="247"/>
-      <c r="G1" s="247"/>
+      <c r="B1" s="257"/>
+      <c r="C1" s="257"/>
+      <c r="D1" s="257"/>
+      <c r="E1" s="257"/>
+      <c r="F1" s="257"/>
+      <c r="G1" s="257"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -10752,19 +10824,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="216" t="s">
+      <c r="A1" s="225" t="s">
         <v>326</v>
       </c>
-      <c r="B1" s="216"/>
-      <c r="C1" s="216"/>
-      <c r="D1" s="216"/>
-      <c r="E1" s="216"/>
-      <c r="F1" s="216"/>
-      <c r="G1" s="216"/>
-      <c r="H1" s="216"/>
-      <c r="I1" s="216"/>
-      <c r="J1" s="216"/>
-      <c r="K1" s="216"/>
+      <c r="B1" s="225"/>
+      <c r="C1" s="225"/>
+      <c r="D1" s="225"/>
+      <c r="E1" s="225"/>
+      <c r="F1" s="225"/>
+      <c r="G1" s="225"/>
+      <c r="H1" s="225"/>
+      <c r="I1" s="225"/>
+      <c r="J1" s="225"/>
+      <c r="K1" s="225"/>
     </row>
     <row r="2" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
@@ -11486,10 +11558,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="248" t="s">
+      <c r="A1" s="258" t="s">
         <v>333</v>
       </c>
-      <c r="B1" s="249"/>
+      <c r="B1" s="259"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="79" t="s">
@@ -11540,7 +11612,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11557,20 +11629,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="250" t="s">
+      <c r="A1" s="260" t="s">
         <v>327</v>
       </c>
-      <c r="B1" s="250"/>
-      <c r="C1" s="250"/>
-      <c r="D1" s="250"/>
-      <c r="E1" s="250"/>
-      <c r="F1" s="250"/>
-      <c r="G1" s="250"/>
-      <c r="H1" s="250"/>
-      <c r="I1" s="250"/>
-      <c r="J1" s="250"/>
-      <c r="K1" s="250"/>
-      <c r="L1" s="250"/>
+      <c r="B1" s="260"/>
+      <c r="C1" s="260"/>
+      <c r="D1" s="260"/>
+      <c r="E1" s="260"/>
+      <c r="F1" s="260"/>
+      <c r="G1" s="260"/>
+      <c r="H1" s="260"/>
+      <c r="I1" s="260"/>
+      <c r="J1" s="260"/>
+      <c r="K1" s="260"/>
+      <c r="L1" s="260"/>
     </row>
     <row r="2" spans="1:12" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="142" t="s">
@@ -12289,15 +12361,15 @@
     </row>
     <row r="26" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="134"/>
-      <c r="B26" s="251" t="s">
+      <c r="B26" s="261" t="s">
         <v>334</v>
       </c>
-      <c r="C26" s="252"/>
-      <c r="D26" s="252"/>
-      <c r="E26" s="252"/>
-      <c r="F26" s="252"/>
-      <c r="G26" s="252"/>
-      <c r="H26" s="253"/>
+      <c r="C26" s="262"/>
+      <c r="D26" s="262"/>
+      <c r="E26" s="262"/>
+      <c r="F26" s="262"/>
+      <c r="G26" s="262"/>
+      <c r="H26" s="263"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="66"/>
@@ -12465,10 +12537,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="211" t="s">
+      <c r="A1" s="220" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="212"/>
+      <c r="B1" s="221"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
@@ -12501,16 +12573,16 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="207" t="s">
+      <c r="A6" s="216" t="s">
         <v>147</v>
       </c>
-      <c r="B6" s="208"/>
+      <c r="B6" s="217"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="209" t="s">
+      <c r="A7" s="218" t="s">
         <v>150</v>
       </c>
-      <c r="B7" s="210"/>
+      <c r="B7" s="219"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -12592,16 +12664,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="213" t="s">
+      <c r="A1" s="222" t="s">
         <v>336</v>
       </c>
-      <c r="B1" s="214"/>
-      <c r="C1" s="214"/>
-      <c r="D1" s="214"/>
-      <c r="E1" s="214"/>
-      <c r="F1" s="214"/>
-      <c r="G1" s="214"/>
-      <c r="H1" s="215"/>
+      <c r="B1" s="223"/>
+      <c r="C1" s="223"/>
+      <c r="D1" s="223"/>
+      <c r="E1" s="223"/>
+      <c r="F1" s="223"/>
+      <c r="G1" s="223"/>
+      <c r="H1" s="224"/>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
     </row>
@@ -12971,14 +13043,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="216" t="s">
+      <c r="A1" s="225" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="216"/>
-      <c r="C1" s="216"/>
-      <c r="D1" s="216"/>
-      <c r="E1" s="216"/>
-      <c r="F1" s="216"/>
+      <c r="B1" s="225"/>
+      <c r="C1" s="225"/>
+      <c r="D1" s="225"/>
+      <c r="E1" s="225"/>
+      <c r="F1" s="225"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
@@ -13461,56 +13533,60 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T53"/>
+  <dimension ref="A1:V53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:Q1"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="51.28515625" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="2" max="2" width="59.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" style="81" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" style="81" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="81" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="3"/>
-    <col min="11" max="11" width="14.5703125" style="71" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" style="81" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" style="81" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" style="81" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="11.42578125" customWidth="1"/>
-    <col min="17" max="17" width="12" customWidth="1"/>
-    <col min="18" max="20" width="0" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="90" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" style="81" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="81" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" style="81" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="81" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="3"/>
+    <col min="13" max="13" width="14.5703125" style="71" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" style="81" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="81" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" style="81" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" customWidth="1"/>
+    <col min="19" max="19" width="12" customWidth="1"/>
+    <col min="20" max="22" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="254" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="226" t="s">
         <v>569</v>
       </c>
-      <c r="B1" s="254"/>
-      <c r="C1" s="254"/>
-      <c r="D1" s="254"/>
-      <c r="E1" s="254"/>
-      <c r="F1" s="254"/>
-      <c r="G1" s="254"/>
-      <c r="H1" s="254"/>
-      <c r="I1" s="254"/>
-      <c r="J1" s="254"/>
-      <c r="K1" s="254"/>
-      <c r="L1" s="254"/>
-      <c r="M1" s="254"/>
-      <c r="N1" s="254"/>
-      <c r="O1" s="254"/>
-      <c r="P1" s="254"/>
-      <c r="Q1" s="254"/>
-    </row>
-    <row r="2" spans="1:20" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="226"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="226"/>
+      <c r="H1" s="226"/>
+      <c r="I1" s="226"/>
+      <c r="J1" s="226"/>
+      <c r="K1" s="226"/>
+      <c r="L1" s="226"/>
+      <c r="M1" s="226"/>
+      <c r="N1" s="226"/>
+      <c r="O1" s="226"/>
+      <c r="P1" s="226"/>
+      <c r="Q1" s="226"/>
+      <c r="R1" s="226"/>
+      <c r="S1" s="226"/>
+    </row>
+    <row r="2" spans="1:22" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>123</v>
       </c>
@@ -13523,52 +13599,58 @@
       <c r="D2" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="82" t="s">
+        <v>576</v>
+      </c>
+      <c r="F2" s="82" t="s">
+        <v>575</v>
+      </c>
+      <c r="G2" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="H2" s="21" t="s">
         <v>474</v>
       </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="82" t="s">
+      <c r="I2" s="21"/>
+      <c r="J2" s="82" t="s">
         <v>567</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="K2" s="21" t="s">
         <v>526</v>
       </c>
-      <c r="J2" s="82" t="s">
+      <c r="L2" s="82" t="s">
         <v>529</v>
       </c>
-      <c r="K2" s="82" t="s">
+      <c r="M2" s="82" t="s">
         <v>566</v>
       </c>
-      <c r="L2" s="82" t="s">
+      <c r="N2" s="82" t="s">
         <v>549</v>
       </c>
-      <c r="M2" s="82" t="s">
+      <c r="O2" s="82" t="s">
         <v>564</v>
       </c>
-      <c r="N2" s="82" t="s">
+      <c r="P2" s="82" t="s">
         <v>565</v>
       </c>
-      <c r="O2" s="91"/>
-      <c r="P2" s="196" t="s">
+      <c r="Q2" s="91"/>
+      <c r="R2" s="196" t="s">
         <v>550</v>
       </c>
-      <c r="Q2" s="196" t="s">
+      <c r="S2" s="196" t="s">
         <v>551</v>
       </c>
-      <c r="R2" s="198" t="s">
+      <c r="T2" s="198" t="s">
         <v>552</v>
       </c>
-      <c r="S2" s="198" t="s">
+      <c r="U2" s="198" t="s">
         <v>553</v>
       </c>
-      <c r="T2" s="199" t="s">
+      <c r="V2" s="199" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>22</v>
       </c>
@@ -13581,44 +13663,48 @@
       <c r="D3" s="132" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="132"/>
+      <c r="F3" s="206" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="183" t="s">
+      <c r="H3" s="183" t="s">
         <v>502</v>
       </c>
-      <c r="G3" s="48"/>
-      <c r="H3" s="183" t="s">
+      <c r="I3" s="48"/>
+      <c r="J3" s="183" t="s">
         <v>346</v>
       </c>
-      <c r="I3" s="94"/>
-      <c r="J3" s="94"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="48">
+      <c r="K3" s="94"/>
+      <c r="L3" s="94"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="48">
         <v>2</v>
       </c>
-      <c r="M3" s="48">
+      <c r="O3" s="48">
         <v>2</v>
       </c>
-      <c r="N3" s="48">
+      <c r="P3" s="48">
         <v>0</v>
       </c>
-      <c r="O3" s="91"/>
-      <c r="P3" s="67">
+      <c r="Q3" s="91"/>
+      <c r="R3" s="67">
         <v>25</v>
       </c>
-      <c r="Q3" s="67">
+      <c r="S3" s="67">
         <v>25</v>
       </c>
-      <c r="R3" s="183">
+      <c r="T3" s="183">
         <v>2</v>
       </c>
-      <c r="S3" s="48">
+      <c r="U3" s="48">
         <v>2</v>
       </c>
-      <c r="T3" s="66"/>
-    </row>
-    <row r="4" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V3" s="66"/>
+    </row>
+    <row r="4" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>27</v>
       </c>
@@ -13631,44 +13717,50 @@
       <c r="D4" s="132">
         <v>2007</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="203" t="s">
+        <v>572</v>
+      </c>
+      <c r="F4" s="203" t="s">
+        <v>572</v>
+      </c>
+      <c r="G4" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="34" t="s">
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="34" t="s">
         <v>346</v>
       </c>
-      <c r="J4" s="94"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="48">
+      <c r="L4" s="94"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="48">
         <v>10</v>
       </c>
-      <c r="M4" s="48">
+      <c r="O4" s="48">
         <v>9</v>
       </c>
-      <c r="N4" s="48">
+      <c r="P4" s="48">
         <v>0</v>
       </c>
-      <c r="O4" s="91"/>
-      <c r="P4" s="67">
+      <c r="Q4" s="91"/>
+      <c r="R4" s="67">
         <v>20</v>
       </c>
-      <c r="Q4" s="67">
+      <c r="S4" s="67">
         <v>20</v>
       </c>
-      <c r="R4" s="183">
+      <c r="T4" s="183">
         <v>10</v>
       </c>
-      <c r="S4" s="48">
+      <c r="U4" s="48">
         <v>10</v>
       </c>
-      <c r="T4" s="66"/>
-    </row>
-    <row r="5" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V4" s="66"/>
+    </row>
+    <row r="5" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>29</v>
       </c>
@@ -13681,48 +13773,54 @@
       <c r="D5" s="132">
         <v>2008</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="203" t="s">
+        <v>572</v>
+      </c>
+      <c r="F5" s="204" t="s">
+        <v>571</v>
+      </c>
+      <c r="G5" s="201" t="s">
         <v>129</v>
       </c>
-      <c r="F5" s="183" t="s">
+      <c r="H5" s="183" t="s">
         <v>210</v>
       </c>
-      <c r="G5" s="48"/>
-      <c r="H5" s="183" t="s">
+      <c r="I5" s="48"/>
+      <c r="J5" s="183" t="s">
         <v>346</v>
       </c>
-      <c r="I5" s="94"/>
-      <c r="J5" s="186" t="s">
+      <c r="K5" s="94"/>
+      <c r="L5" s="186" t="s">
         <v>346</v>
       </c>
-      <c r="K5" s="189" t="s">
+      <c r="M5" s="189" t="s">
         <v>528</v>
       </c>
-      <c r="L5" s="48">
+      <c r="N5" s="48">
         <v>1</v>
       </c>
-      <c r="M5" s="48">
+      <c r="O5" s="48">
         <v>0</v>
       </c>
-      <c r="N5" s="48">
+      <c r="P5" s="48">
         <v>0</v>
       </c>
-      <c r="O5" s="91"/>
-      <c r="P5" s="67">
+      <c r="Q5" s="91"/>
+      <c r="R5" s="67">
         <v>24</v>
       </c>
-      <c r="Q5" s="67">
+      <c r="S5" s="67">
         <v>24</v>
       </c>
-      <c r="R5" s="183">
+      <c r="T5" s="183">
         <v>1</v>
       </c>
-      <c r="S5" s="48">
+      <c r="U5" s="48">
         <v>1</v>
       </c>
-      <c r="T5" s="66"/>
-    </row>
-    <row r="6" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V5" s="66"/>
+    </row>
+    <row r="6" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>31</v>
       </c>
@@ -13735,44 +13833,48 @@
       <c r="D6" s="132">
         <v>2015</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="132"/>
+      <c r="F6" s="207" t="s">
+        <v>570</v>
+      </c>
+      <c r="G6" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="34" t="s">
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="34" t="s">
         <v>346</v>
       </c>
-      <c r="J6" s="94"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="48">
+      <c r="L6" s="94"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="48">
         <v>11</v>
       </c>
-      <c r="M6" s="48">
+      <c r="O6" s="48">
         <v>2</v>
       </c>
-      <c r="N6" s="48">
+      <c r="P6" s="48">
         <v>0</v>
       </c>
-      <c r="O6" s="91"/>
-      <c r="P6" s="67">
+      <c r="Q6" s="91"/>
+      <c r="R6" s="67">
         <v>57</v>
       </c>
-      <c r="Q6" s="67">
+      <c r="S6" s="67">
         <v>57</v>
       </c>
-      <c r="R6" s="183">
+      <c r="T6" s="183">
         <v>11</v>
       </c>
-      <c r="S6" s="2">
+      <c r="U6" s="2">
         <v>11</v>
       </c>
-      <c r="T6" s="66"/>
-    </row>
-    <row r="7" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V6" s="66"/>
+    </row>
+    <row r="7" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
         <v>38</v>
       </c>
@@ -13785,44 +13887,50 @@
       <c r="D7" s="132">
         <v>2011</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="203" t="s">
+        <v>572</v>
+      </c>
+      <c r="F7" s="203" t="s">
+        <v>572</v>
+      </c>
+      <c r="G7" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="F7" s="183" t="s">
+      <c r="H7" s="183" t="s">
         <v>211</v>
       </c>
-      <c r="G7" s="48"/>
-      <c r="H7" s="183" t="s">
+      <c r="I7" s="48"/>
+      <c r="J7" s="183" t="s">
         <v>346</v>
       </c>
-      <c r="I7" s="94"/>
-      <c r="J7" s="94"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="48">
+      <c r="K7" s="94"/>
+      <c r="L7" s="94"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="48">
         <v>15</v>
       </c>
-      <c r="M7" s="48">
+      <c r="O7" s="48">
         <v>8</v>
       </c>
-      <c r="N7" s="48">
+      <c r="P7" s="48">
         <v>1</v>
       </c>
-      <c r="O7" s="91"/>
-      <c r="P7" s="48">
+      <c r="Q7" s="91"/>
+      <c r="R7" s="48">
         <v>11</v>
       </c>
-      <c r="Q7" s="48">
+      <c r="S7" s="48">
         <v>11</v>
       </c>
-      <c r="R7" s="183">
+      <c r="T7" s="183">
         <v>15</v>
       </c>
-      <c r="S7" s="48">
+      <c r="U7" s="48">
         <v>15</v>
       </c>
-      <c r="T7" s="66"/>
-    </row>
-    <row r="8" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V7" s="66"/>
+    </row>
+    <row r="8" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
         <v>39</v>
       </c>
@@ -13835,44 +13943,48 @@
       <c r="D8" s="132">
         <v>2010</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="132"/>
+      <c r="F8" s="208" t="s">
+        <v>574</v>
+      </c>
+      <c r="G8" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="F8" s="183" t="s">
+      <c r="H8" s="183" t="s">
         <v>512</v>
       </c>
-      <c r="G8" s="48"/>
-      <c r="H8" s="183" t="s">
+      <c r="I8" s="48"/>
+      <c r="J8" s="183" t="s">
         <v>346</v>
       </c>
-      <c r="I8" s="94"/>
-      <c r="J8" s="94"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="48">
+      <c r="K8" s="94"/>
+      <c r="L8" s="94"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="48">
         <v>11</v>
       </c>
-      <c r="M8" s="48">
+      <c r="O8" s="48">
         <v>8</v>
       </c>
-      <c r="N8" s="48">
+      <c r="P8" s="48">
         <v>0</v>
       </c>
-      <c r="O8" s="91"/>
-      <c r="P8" s="48">
+      <c r="Q8" s="91"/>
+      <c r="R8" s="48">
         <v>22</v>
       </c>
-      <c r="Q8" s="48">
+      <c r="S8" s="48">
         <v>22</v>
       </c>
-      <c r="R8" s="183">
+      <c r="T8" s="183">
         <v>10</v>
       </c>
-      <c r="S8" s="48">
+      <c r="U8" s="48">
         <v>10</v>
       </c>
-      <c r="T8" s="66"/>
-    </row>
-    <row r="9" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V8" s="66"/>
+    </row>
+    <row r="9" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>40</v>
       </c>
@@ -13885,44 +13997,48 @@
       <c r="D9" s="132">
         <v>2009</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="132"/>
+      <c r="F9" s="207" t="s">
+        <v>570</v>
+      </c>
+      <c r="G9" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="F9" s="183" t="s">
+      <c r="H9" s="183" t="s">
         <v>513</v>
       </c>
-      <c r="G9" s="48"/>
-      <c r="H9" s="183" t="s">
+      <c r="I9" s="48"/>
+      <c r="J9" s="183" t="s">
         <v>346</v>
       </c>
-      <c r="I9" s="94"/>
-      <c r="J9" s="94"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="48">
+      <c r="K9" s="94"/>
+      <c r="L9" s="94"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="48">
         <v>22</v>
       </c>
-      <c r="M9" s="48">
+      <c r="O9" s="48">
         <v>20</v>
       </c>
-      <c r="N9" s="48">
+      <c r="P9" s="48">
         <v>1</v>
       </c>
-      <c r="O9" s="91"/>
-      <c r="P9" s="48">
+      <c r="Q9" s="91"/>
+      <c r="R9" s="48">
         <v>13</v>
       </c>
-      <c r="Q9" s="48">
+      <c r="S9" s="48">
         <v>13</v>
       </c>
-      <c r="R9" s="183">
+      <c r="T9" s="183">
         <v>22</v>
       </c>
-      <c r="S9" s="48">
+      <c r="U9" s="48">
         <v>22</v>
       </c>
-      <c r="T9" s="66"/>
-    </row>
-    <row r="10" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V9" s="66"/>
+    </row>
+    <row r="10" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>41</v>
       </c>
@@ -13935,44 +14051,50 @@
       <c r="D10" s="132">
         <v>2010</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="203" t="s">
+        <v>572</v>
+      </c>
+      <c r="F10" s="204" t="s">
+        <v>571</v>
+      </c>
+      <c r="G10" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="F10" s="183" t="s">
+      <c r="H10" s="183" t="s">
         <v>212</v>
       </c>
-      <c r="G10" s="48"/>
-      <c r="H10" s="183" t="s">
+      <c r="I10" s="48"/>
+      <c r="J10" s="183" t="s">
         <v>346</v>
       </c>
-      <c r="I10" s="94"/>
-      <c r="J10" s="94"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="48">
+      <c r="K10" s="94"/>
+      <c r="L10" s="94"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="48">
         <v>19</v>
       </c>
-      <c r="M10" s="48">
+      <c r="O10" s="48">
         <v>15</v>
       </c>
-      <c r="N10" s="48">
+      <c r="P10" s="48">
         <v>0</v>
       </c>
-      <c r="O10" s="91"/>
-      <c r="P10" s="48">
+      <c r="Q10" s="91"/>
+      <c r="R10" s="48">
         <v>43</v>
       </c>
-      <c r="Q10" s="48">
+      <c r="S10" s="48">
         <v>43</v>
       </c>
-      <c r="R10" s="183">
+      <c r="T10" s="183">
         <v>19</v>
       </c>
-      <c r="S10" s="48">
+      <c r="U10" s="48">
         <v>19</v>
       </c>
-      <c r="T10" s="66"/>
-    </row>
-    <row r="11" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V10" s="66"/>
+    </row>
+    <row r="11" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>42</v>
       </c>
@@ -13985,46 +14107,50 @@
       <c r="D11" s="132">
         <v>2010</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="132"/>
+      <c r="F11" s="206" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="F11" s="183" t="s">
+      <c r="H11" s="183" t="s">
         <v>514</v>
       </c>
-      <c r="G11" s="48"/>
-      <c r="H11" s="183" t="s">
+      <c r="I11" s="48"/>
+      <c r="J11" s="183" t="s">
         <v>346</v>
       </c>
-      <c r="I11" s="94"/>
-      <c r="J11" s="94"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="2">
+      <c r="K11" s="94"/>
+      <c r="L11" s="94"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="2">
         <v>147</v>
       </c>
-      <c r="M11" s="48">
+      <c r="O11" s="48">
         <v>105</v>
       </c>
-      <c r="N11" s="48">
-        <v>11</v>
-      </c>
-      <c r="O11" s="91"/>
       <c r="P11" s="48">
         <v>11</v>
       </c>
-      <c r="Q11" s="48">
+      <c r="Q11" s="91"/>
+      <c r="R11" s="48">
         <v>11</v>
       </c>
-      <c r="R11" s="183">
+      <c r="S11" s="48">
+        <v>11</v>
+      </c>
+      <c r="T11" s="183">
         <v>141</v>
       </c>
-      <c r="S11" s="183">
+      <c r="U11" s="183">
         <v>146</v>
       </c>
-      <c r="T11" s="200" t="s">
+      <c r="V11" s="200" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
         <v>43</v>
       </c>
@@ -14037,44 +14163,48 @@
       <c r="D12" s="132">
         <v>1999</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="132"/>
+      <c r="F12" s="206" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="F12" s="183" t="s">
+      <c r="H12" s="183" t="s">
         <v>515</v>
       </c>
-      <c r="G12" s="48"/>
-      <c r="H12" s="183" t="s">
+      <c r="I12" s="48"/>
+      <c r="J12" s="183" t="s">
         <v>346</v>
       </c>
-      <c r="I12" s="94"/>
-      <c r="J12" s="94"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="2">
+      <c r="K12" s="94"/>
+      <c r="L12" s="94"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="2">
         <v>56</v>
       </c>
-      <c r="M12" s="48">
+      <c r="O12" s="48">
         <v>51</v>
       </c>
-      <c r="N12" s="48">
+      <c r="P12" s="48">
         <v>1</v>
       </c>
-      <c r="O12" s="91"/>
-      <c r="P12" s="2">
+      <c r="Q12" s="91"/>
+      <c r="R12" s="2">
         <v>37</v>
       </c>
-      <c r="Q12" s="2">
+      <c r="S12" s="2">
         <v>37</v>
       </c>
-      <c r="R12" s="183">
+      <c r="T12" s="183">
         <v>55</v>
       </c>
-      <c r="S12" s="48">
+      <c r="U12" s="48">
         <v>55</v>
       </c>
-      <c r="T12" s="66"/>
-    </row>
-    <row r="13" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V12" s="66"/>
+    </row>
+    <row r="13" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
         <v>44</v>
       </c>
@@ -14082,51 +14212,55 @@
         <v>68</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>69</v>
+        <v>573</v>
       </c>
       <c r="D13" s="132">
         <v>2005</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="132"/>
+      <c r="F13" s="206" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="34" t="s">
+      <c r="I13" s="48"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="34" t="s">
         <v>346</v>
       </c>
-      <c r="J13" s="94"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="2">
+      <c r="L13" s="94"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="2">
         <v>42</v>
       </c>
-      <c r="M13" s="48">
+      <c r="O13" s="48">
         <v>39</v>
       </c>
-      <c r="N13" s="48">
+      <c r="P13" s="48">
         <v>0</v>
       </c>
-      <c r="O13" s="91"/>
-      <c r="P13" s="48">
+      <c r="Q13" s="91"/>
+      <c r="R13" s="48">
         <v>16</v>
       </c>
-      <c r="Q13" s="48">
+      <c r="S13" s="48">
         <v>16</v>
       </c>
-      <c r="R13" s="183">
+      <c r="T13" s="183">
         <v>37</v>
       </c>
-      <c r="S13" s="183">
+      <c r="U13" s="183">
         <v>41</v>
       </c>
-      <c r="T13" s="66" t="s">
+      <c r="V13" s="66" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
         <v>45</v>
       </c>
@@ -14139,44 +14273,48 @@
       <c r="D14" s="132">
         <v>2008</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="132"/>
+      <c r="F14" s="204" t="s">
+        <v>571</v>
+      </c>
+      <c r="G14" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="34" t="s">
+      <c r="I14" s="48"/>
+      <c r="J14" s="48"/>
+      <c r="K14" s="34" t="s">
         <v>346</v>
       </c>
-      <c r="J14" s="94"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="48">
+      <c r="L14" s="94"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="48">
         <v>5</v>
       </c>
-      <c r="M14" s="48">
+      <c r="O14" s="48">
         <v>4</v>
       </c>
-      <c r="N14" s="48">
+      <c r="P14" s="48">
         <v>0</v>
       </c>
-      <c r="O14" s="91"/>
-      <c r="P14" s="48">
+      <c r="Q14" s="91"/>
+      <c r="R14" s="48">
         <v>14</v>
       </c>
-      <c r="Q14" s="2">
+      <c r="S14" s="2">
         <v>14</v>
       </c>
-      <c r="R14" s="183">
+      <c r="T14" s="183">
         <v>5</v>
       </c>
-      <c r="S14" s="2">
+      <c r="U14" s="2">
         <v>5</v>
       </c>
-      <c r="T14" s="66"/>
-    </row>
-    <row r="15" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V14" s="66"/>
+    </row>
+    <row r="15" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
         <v>46</v>
       </c>
@@ -14189,44 +14327,50 @@
       <c r="D15" s="132">
         <v>2011</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="203" t="s">
+        <v>572</v>
+      </c>
+      <c r="F15" s="204" t="s">
+        <v>571</v>
+      </c>
+      <c r="G15" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="F15" s="183" t="s">
+      <c r="H15" s="183" t="s">
         <v>517</v>
       </c>
-      <c r="G15" s="48"/>
-      <c r="H15" s="183" t="s">
+      <c r="I15" s="48"/>
+      <c r="J15" s="183" t="s">
         <v>346</v>
       </c>
-      <c r="I15" s="94"/>
-      <c r="J15" s="94"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="48">
+      <c r="K15" s="94"/>
+      <c r="L15" s="94"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="48">
         <v>7</v>
       </c>
-      <c r="M15" s="48">
+      <c r="O15" s="48">
         <v>2</v>
       </c>
-      <c r="N15" s="48">
+      <c r="P15" s="48">
         <v>1</v>
       </c>
-      <c r="O15" s="91"/>
-      <c r="P15" s="48">
+      <c r="Q15" s="91"/>
+      <c r="R15" s="48">
         <v>8</v>
       </c>
-      <c r="Q15" s="48">
+      <c r="S15" s="48">
         <v>8</v>
       </c>
-      <c r="R15" s="183">
+      <c r="T15" s="183">
         <v>7</v>
       </c>
-      <c r="S15" s="48">
+      <c r="U15" s="48">
         <v>7</v>
       </c>
-      <c r="T15" s="66"/>
-    </row>
-    <row r="16" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V15" s="66"/>
+    </row>
+    <row r="16" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
         <v>47</v>
       </c>
@@ -14239,44 +14383,50 @@
       <c r="D16" s="132">
         <v>2009</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="203" t="s">
+        <v>572</v>
+      </c>
+      <c r="F16" s="204" t="s">
+        <v>571</v>
+      </c>
+      <c r="G16" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="F16" s="183" t="s">
+      <c r="H16" s="183" t="s">
         <v>215</v>
       </c>
-      <c r="G16" s="48"/>
-      <c r="H16" s="183" t="s">
+      <c r="I16" s="48"/>
+      <c r="J16" s="183" t="s">
         <v>346</v>
       </c>
-      <c r="I16" s="94"/>
-      <c r="J16" s="94"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="48">
+      <c r="K16" s="94"/>
+      <c r="L16" s="94"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="48">
         <v>5</v>
       </c>
-      <c r="M16" s="48">
+      <c r="O16" s="48">
         <v>3</v>
       </c>
-      <c r="N16" s="48">
+      <c r="P16" s="48">
         <v>0</v>
       </c>
-      <c r="O16" s="91"/>
-      <c r="P16" s="48">
+      <c r="Q16" s="91"/>
+      <c r="R16" s="48">
         <v>27</v>
       </c>
-      <c r="Q16" s="48">
+      <c r="S16" s="48">
         <v>27</v>
       </c>
-      <c r="R16" s="183">
+      <c r="T16" s="183">
         <v>5</v>
       </c>
-      <c r="S16" s="48">
+      <c r="U16" s="48">
         <v>5</v>
       </c>
-      <c r="T16" s="66"/>
-    </row>
-    <row r="17" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V16" s="66"/>
+    </row>
+    <row r="17" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
         <v>48</v>
       </c>
@@ -14289,44 +14439,50 @@
       <c r="D17" s="132">
         <v>1997</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="203" t="s">
+        <v>572</v>
+      </c>
+      <c r="F17" s="203" t="s">
+        <v>572</v>
+      </c>
+      <c r="G17" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="F17" s="183" t="s">
+      <c r="H17" s="183" t="s">
         <v>216</v>
       </c>
-      <c r="G17" s="48"/>
-      <c r="H17" s="183" t="s">
+      <c r="I17" s="48"/>
+      <c r="J17" s="183" t="s">
         <v>346</v>
       </c>
-      <c r="I17" s="94"/>
-      <c r="J17" s="94"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="48">
+      <c r="K17" s="94"/>
+      <c r="L17" s="94"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="48">
         <v>10</v>
       </c>
-      <c r="M17" s="48">
+      <c r="O17" s="48">
         <v>10</v>
       </c>
-      <c r="N17" s="48">
+      <c r="P17" s="48">
         <v>0</v>
       </c>
-      <c r="O17" s="91"/>
-      <c r="P17" s="48">
+      <c r="Q17" s="91"/>
+      <c r="R17" s="48">
         <v>14</v>
       </c>
-      <c r="Q17" s="48">
+      <c r="S17" s="48">
         <v>14</v>
       </c>
-      <c r="R17" s="183">
+      <c r="T17" s="183">
         <v>10</v>
       </c>
-      <c r="S17" s="48">
+      <c r="U17" s="48">
         <v>10</v>
       </c>
-      <c r="T17" s="66"/>
-    </row>
-    <row r="18" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V17" s="66"/>
+    </row>
+    <row r="18" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
         <v>49</v>
       </c>
@@ -14339,44 +14495,48 @@
       <c r="D18" s="132">
         <v>2010</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="E18" s="132"/>
+      <c r="F18" s="206" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="H18" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="G18" s="48"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="34" t="s">
+      <c r="I18" s="48"/>
+      <c r="J18" s="48"/>
+      <c r="K18" s="34" t="s">
         <v>346</v>
       </c>
-      <c r="J18" s="94"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="48">
+      <c r="L18" s="94"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="48">
         <v>8</v>
       </c>
-      <c r="M18" s="48">
+      <c r="O18" s="48">
         <v>7</v>
       </c>
-      <c r="N18" s="48">
+      <c r="P18" s="48">
         <v>1</v>
       </c>
-      <c r="O18" s="91"/>
-      <c r="P18" s="48">
-        <v>8</v>
-      </c>
-      <c r="Q18" s="48">
-        <v>8</v>
-      </c>
-      <c r="R18" s="183">
+      <c r="Q18" s="91"/>
+      <c r="R18" s="48">
         <v>8</v>
       </c>
       <c r="S18" s="48">
         <v>8</v>
       </c>
-      <c r="T18" s="66"/>
-    </row>
-    <row r="19" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T18" s="183">
+        <v>8</v>
+      </c>
+      <c r="U18" s="48">
+        <v>8</v>
+      </c>
+      <c r="V18" s="66"/>
+    </row>
+    <row r="19" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
         <v>50</v>
       </c>
@@ -14389,46 +14549,50 @@
       <c r="D19" s="132">
         <v>2005</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="132"/>
+      <c r="F19" s="209" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="F19" s="183" t="s">
+      <c r="H19" s="183" t="s">
         <v>519</v>
       </c>
-      <c r="G19" s="48"/>
-      <c r="H19" s="183" t="s">
+      <c r="I19" s="48"/>
+      <c r="J19" s="183" t="s">
         <v>346</v>
       </c>
-      <c r="I19" s="94"/>
-      <c r="J19" s="94"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="48">
+      <c r="K19" s="94"/>
+      <c r="L19" s="94"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="48">
         <v>17</v>
       </c>
-      <c r="M19" s="48">
+      <c r="O19" s="48">
         <v>14</v>
       </c>
-      <c r="N19" s="48">
+      <c r="P19" s="48">
         <v>0</v>
       </c>
-      <c r="O19" s="91"/>
-      <c r="P19" s="48">
+      <c r="Q19" s="91"/>
+      <c r="R19" s="48">
         <v>15</v>
       </c>
-      <c r="Q19" s="48">
+      <c r="S19" s="48">
         <v>15</v>
       </c>
-      <c r="R19" s="183">
+      <c r="T19" s="183">
         <v>15</v>
       </c>
-      <c r="S19" s="183">
+      <c r="U19" s="183">
         <v>17</v>
       </c>
-      <c r="T19" s="66" t="s">
+      <c r="V19" s="66" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
         <v>51</v>
       </c>
@@ -14441,44 +14605,48 @@
       <c r="D20" s="132">
         <v>2011</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="132"/>
+      <c r="F20" s="205" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="F20" s="183" t="s">
+      <c r="H20" s="183" t="s">
         <v>520</v>
       </c>
-      <c r="G20" s="48"/>
-      <c r="H20" s="183" t="s">
+      <c r="I20" s="48"/>
+      <c r="J20" s="183" t="s">
         <v>346</v>
       </c>
-      <c r="I20" s="94"/>
-      <c r="J20" s="94"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="48">
+      <c r="K20" s="94"/>
+      <c r="L20" s="94"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="48">
         <v>8</v>
       </c>
-      <c r="M20" s="48">
+      <c r="O20" s="48">
         <v>8</v>
       </c>
-      <c r="N20" s="48">
+      <c r="P20" s="48">
         <v>0</v>
       </c>
-      <c r="O20" s="91"/>
-      <c r="P20" s="48">
+      <c r="Q20" s="91"/>
+      <c r="R20" s="48">
         <v>18</v>
       </c>
-      <c r="Q20" s="48">
+      <c r="S20" s="48">
         <v>18</v>
       </c>
-      <c r="R20" s="183">
+      <c r="T20" s="183">
         <v>8</v>
       </c>
-      <c r="S20" s="48">
+      <c r="U20" s="48">
         <v>8</v>
       </c>
-      <c r="T20" s="66"/>
-    </row>
-    <row r="21" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V20" s="66"/>
+    </row>
+    <row r="21" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
         <v>52</v>
       </c>
@@ -14491,46 +14659,50 @@
       <c r="D21" s="132">
         <v>2008</v>
       </c>
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="132"/>
+      <c r="F21" s="205" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="F21" s="183" t="s">
+      <c r="H21" s="183" t="s">
         <v>521</v>
       </c>
-      <c r="G21" s="48"/>
-      <c r="H21" s="183" t="s">
+      <c r="I21" s="48"/>
+      <c r="J21" s="183" t="s">
         <v>346</v>
       </c>
-      <c r="I21" s="94"/>
-      <c r="J21" s="94"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="48">
+      <c r="K21" s="94"/>
+      <c r="L21" s="94"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="48">
         <v>21</v>
       </c>
-      <c r="M21" s="48">
+      <c r="O21" s="48">
         <v>17</v>
       </c>
-      <c r="N21" s="48">
+      <c r="P21" s="48">
         <v>4</v>
       </c>
-      <c r="O21" s="91"/>
-      <c r="P21" s="48">
+      <c r="Q21" s="91"/>
+      <c r="R21" s="48">
         <v>22</v>
       </c>
-      <c r="Q21" s="48">
+      <c r="S21" s="48">
         <v>22</v>
       </c>
-      <c r="R21" s="183">
+      <c r="T21" s="183">
         <v>18</v>
       </c>
-      <c r="S21" s="183">
+      <c r="U21" s="183">
         <v>21</v>
       </c>
-      <c r="T21" s="66" t="s">
+      <c r="V21" s="66" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
         <v>53</v>
       </c>
@@ -14543,44 +14715,48 @@
       <c r="D22" s="132">
         <v>2015</v>
       </c>
-      <c r="E22" s="19" t="s">
+      <c r="E22" s="132"/>
+      <c r="F22" s="205" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="G22" s="48"/>
-      <c r="H22" s="48"/>
-      <c r="I22" s="34" t="s">
+      <c r="I22" s="48"/>
+      <c r="J22" s="48"/>
+      <c r="K22" s="34" t="s">
         <v>346</v>
       </c>
-      <c r="J22" s="94"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="48">
+      <c r="L22" s="94"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="48">
         <v>4</v>
       </c>
-      <c r="M22" s="48">
+      <c r="O22" s="48">
         <v>0</v>
       </c>
-      <c r="N22" s="48">
+      <c r="P22" s="48">
         <v>0</v>
       </c>
-      <c r="O22" s="91"/>
-      <c r="P22" s="48">
+      <c r="Q22" s="91"/>
+      <c r="R22" s="48">
         <v>15</v>
       </c>
-      <c r="Q22" s="48">
+      <c r="S22" s="48">
         <v>15</v>
       </c>
-      <c r="R22" s="183">
+      <c r="T22" s="183">
         <v>4</v>
       </c>
-      <c r="S22" s="48">
+      <c r="U22" s="48">
         <v>4</v>
       </c>
-      <c r="T22" s="66"/>
-    </row>
-    <row r="23" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V22" s="66"/>
+    </row>
+    <row r="23" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
         <v>54</v>
       </c>
@@ -14593,46 +14769,50 @@
       <c r="D23" s="132">
         <v>2000</v>
       </c>
-      <c r="E23" s="19" t="s">
+      <c r="E23" s="132"/>
+      <c r="F23" s="205" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="F23" s="183" t="s">
+      <c r="H23" s="183" t="s">
         <v>523</v>
       </c>
-      <c r="G23" s="48"/>
-      <c r="H23" s="183" t="s">
+      <c r="I23" s="48"/>
+      <c r="J23" s="183" t="s">
         <v>346</v>
       </c>
-      <c r="I23" s="94"/>
-      <c r="J23" s="94"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="2">
+      <c r="K23" s="94"/>
+      <c r="L23" s="94"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="2">
         <v>95</v>
       </c>
-      <c r="M23" s="48">
+      <c r="O23" s="48">
         <v>80</v>
       </c>
-      <c r="N23" s="48">
+      <c r="P23" s="48">
         <v>0</v>
       </c>
-      <c r="O23" s="91"/>
-      <c r="P23" s="48">
+      <c r="Q23" s="91"/>
+      <c r="R23" s="48">
         <v>11</v>
       </c>
-      <c r="Q23" s="48">
+      <c r="S23" s="48">
         <v>11</v>
       </c>
-      <c r="R23" s="183">
+      <c r="T23" s="183">
         <v>85</v>
       </c>
-      <c r="S23" s="183">
+      <c r="U23" s="183">
         <v>95</v>
       </c>
-      <c r="T23" s="66" t="s">
+      <c r="V23" s="66" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
         <v>55</v>
       </c>
@@ -14645,46 +14825,50 @@
       <c r="D24" s="132">
         <v>2010</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="132"/>
+      <c r="F24" s="205" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="H24" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="G24" s="48"/>
-      <c r="H24" s="48"/>
-      <c r="I24" s="34" t="s">
+      <c r="I24" s="48"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="34" t="s">
         <v>346</v>
       </c>
-      <c r="J24" s="94"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="48">
+      <c r="L24" s="94"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="48">
         <v>29</v>
       </c>
-      <c r="M24" s="48">
+      <c r="O24" s="48">
         <v>21</v>
       </c>
-      <c r="N24" s="48">
+      <c r="P24" s="48">
         <v>5</v>
       </c>
-      <c r="O24" s="91"/>
-      <c r="P24" s="48">
+      <c r="Q24" s="91"/>
+      <c r="R24" s="48">
         <v>33</v>
       </c>
-      <c r="Q24" s="48">
+      <c r="S24" s="48">
         <v>33</v>
       </c>
-      <c r="R24" s="183">
+      <c r="T24" s="183">
         <v>27</v>
       </c>
-      <c r="S24" s="183">
+      <c r="U24" s="183">
         <v>29</v>
       </c>
-      <c r="T24" s="66" t="s">
+      <c r="V24" s="66" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="53" t="s">
         <v>359</v>
       </c>
@@ -14697,41 +14881,43 @@
       <c r="D25" s="18">
         <v>1999</v>
       </c>
-      <c r="E25" s="18" t="s">
+      <c r="E25" s="18"/>
+      <c r="F25" s="202"/>
+      <c r="G25" s="18" t="s">
         <v>357</v>
       </c>
-      <c r="F25" s="29" t="s">
+      <c r="H25" s="29" t="s">
         <v>501</v>
       </c>
-      <c r="G25" s="191" t="s">
+      <c r="I25" s="191" t="s">
         <v>545</v>
       </c>
-      <c r="H25" s="85"/>
-      <c r="I25" s="85"/>
-      <c r="J25" s="74" t="s">
+      <c r="J25" s="85"/>
+      <c r="K25" s="85"/>
+      <c r="L25" s="74" t="s">
         <v>346</v>
       </c>
-      <c r="K25" s="19" t="s">
+      <c r="M25" s="19" t="s">
         <v>568</v>
       </c>
-      <c r="L25" s="29">
+      <c r="N25" s="29">
         <v>40</v>
       </c>
-      <c r="M25" s="29">
+      <c r="O25" s="29">
         <v>33</v>
       </c>
-      <c r="N25" s="29">
+      <c r="P25" s="29">
         <v>1</v>
       </c>
-      <c r="O25" s="91"/>
-      <c r="P25" s="85" t="s">
+      <c r="Q25" s="91"/>
+      <c r="R25" s="85" t="s">
         <v>510</v>
       </c>
-      <c r="Q25" s="197">
+      <c r="S25" s="197">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="53" t="s">
         <v>360</v>
       </c>
@@ -14744,39 +14930,41 @@
       <c r="D26" s="18">
         <v>2010</v>
       </c>
-      <c r="E26" s="18" t="s">
+      <c r="E26" s="18"/>
+      <c r="F26" s="202"/>
+      <c r="G26" s="18" t="s">
         <v>361</v>
       </c>
-      <c r="F26" s="53" t="s">
+      <c r="H26" s="53" t="s">
         <v>470</v>
       </c>
-      <c r="G26" s="192" t="s">
+      <c r="I26" s="192" t="s">
         <v>530</v>
       </c>
-      <c r="H26" s="53"/>
-      <c r="I26" s="34" t="s">
+      <c r="J26" s="53"/>
+      <c r="K26" s="34" t="s">
         <v>346</v>
       </c>
-      <c r="J26" s="94"/>
-      <c r="K26" s="19"/>
-      <c r="L26" s="53">
+      <c r="L26" s="94"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="53">
         <v>8</v>
       </c>
-      <c r="M26" s="53">
+      <c r="O26" s="53">
         <v>5</v>
       </c>
-      <c r="N26" s="53">
+      <c r="P26" s="53">
         <v>1</v>
       </c>
-      <c r="O26" s="91"/>
-      <c r="P26" s="94">
+      <c r="Q26" s="91"/>
+      <c r="R26" s="94">
         <v>12</v>
       </c>
-      <c r="Q26" s="94">
+      <c r="S26" s="94">
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="53" t="s">
         <v>364</v>
       </c>
@@ -14789,41 +14977,43 @@
       <c r="D27" s="18">
         <v>2014</v>
       </c>
-      <c r="E27" s="18" t="s">
+      <c r="E27" s="18"/>
+      <c r="F27" s="202"/>
+      <c r="G27" s="18" t="s">
         <v>365</v>
       </c>
-      <c r="F27" s="29" t="s">
+      <c r="H27" s="29" t="s">
         <v>471</v>
       </c>
-      <c r="G27" s="89" t="s">
+      <c r="I27" s="89" t="s">
         <v>531</v>
       </c>
-      <c r="H27" s="85"/>
-      <c r="I27" s="85"/>
-      <c r="J27" s="74" t="s">
+      <c r="J27" s="85"/>
+      <c r="K27" s="85"/>
+      <c r="L27" s="74" t="s">
         <v>346</v>
       </c>
-      <c r="K27" s="19" t="s">
+      <c r="M27" s="19" t="s">
         <v>568</v>
       </c>
-      <c r="L27" s="29">
+      <c r="N27" s="29">
         <v>1</v>
       </c>
-      <c r="M27" s="29">
+      <c r="O27" s="29">
         <v>0</v>
       </c>
-      <c r="N27" s="29">
+      <c r="P27" s="29">
         <v>0</v>
       </c>
-      <c r="O27" s="91"/>
-      <c r="P27" s="94">
+      <c r="Q27" s="91"/>
+      <c r="R27" s="94">
         <v>10</v>
       </c>
-      <c r="Q27" s="94">
+      <c r="S27" s="94">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="53" t="s">
         <v>368</v>
       </c>
@@ -14836,39 +15026,41 @@
       <c r="D28" s="18">
         <v>2014</v>
       </c>
-      <c r="E28" s="18" t="s">
+      <c r="E28" s="18"/>
+      <c r="F28" s="202"/>
+      <c r="G28" s="18" t="s">
         <v>369</v>
       </c>
-      <c r="F28" s="53" t="s">
+      <c r="H28" s="53" t="s">
         <v>472</v>
       </c>
-      <c r="G28" s="192" t="s">
+      <c r="I28" s="192" t="s">
         <v>532</v>
       </c>
-      <c r="H28" s="53"/>
-      <c r="I28" s="34" t="s">
+      <c r="J28" s="53"/>
+      <c r="K28" s="34" t="s">
         <v>346</v>
       </c>
-      <c r="J28" s="94"/>
-      <c r="K28" s="19"/>
-      <c r="L28" s="53">
+      <c r="L28" s="94"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="53">
         <v>4</v>
       </c>
-      <c r="M28" s="53">
+      <c r="O28" s="53">
         <v>1</v>
       </c>
-      <c r="N28" s="53">
+      <c r="P28" s="53">
         <v>0</v>
       </c>
-      <c r="O28" s="91"/>
-      <c r="P28" s="94">
+      <c r="Q28" s="91"/>
+      <c r="R28" s="94">
         <v>94</v>
       </c>
-      <c r="Q28" s="94">
+      <c r="S28" s="94">
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="53" t="s">
         <v>372</v>
       </c>
@@ -14881,39 +15073,41 @@
       <c r="D29" s="18">
         <v>2002</v>
       </c>
-      <c r="E29" s="18" t="s">
+      <c r="E29" s="18"/>
+      <c r="F29" s="202"/>
+      <c r="G29" s="18" t="s">
         <v>373</v>
       </c>
-      <c r="F29" s="184" t="s">
+      <c r="H29" s="184" t="s">
         <v>476</v>
       </c>
-      <c r="G29" s="191" t="s">
+      <c r="I29" s="191" t="s">
         <v>561</v>
       </c>
-      <c r="H29" s="184" t="s">
+      <c r="J29" s="184" t="s">
         <v>346</v>
       </c>
-      <c r="I29" s="94"/>
-      <c r="J29" s="94"/>
-      <c r="K29" s="19"/>
-      <c r="L29" s="29">
+      <c r="K29" s="94"/>
+      <c r="L29" s="94"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="29">
         <v>31</v>
       </c>
-      <c r="M29" s="29">
+      <c r="O29" s="29">
         <v>30</v>
       </c>
-      <c r="N29" s="29">
+      <c r="P29" s="29">
         <v>0</v>
       </c>
-      <c r="O29" s="91"/>
-      <c r="P29" s="94">
+      <c r="Q29" s="91"/>
+      <c r="R29" s="94">
         <v>19</v>
       </c>
-      <c r="Q29" s="94">
+      <c r="S29" s="94">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="53" t="s">
         <v>378</v>
       </c>
@@ -14926,39 +15120,41 @@
       <c r="D30" s="18">
         <v>2013</v>
       </c>
-      <c r="E30" s="18" t="s">
+      <c r="E30" s="18"/>
+      <c r="F30" s="202"/>
+      <c r="G30" s="18" t="s">
         <v>376</v>
       </c>
-      <c r="F30" s="29" t="s">
+      <c r="H30" s="29" t="s">
         <v>477</v>
       </c>
-      <c r="G30" s="193" t="s">
+      <c r="I30" s="193" t="s">
         <v>533</v>
       </c>
-      <c r="H30" s="94"/>
-      <c r="I30" s="34" t="s">
+      <c r="J30" s="94"/>
+      <c r="K30" s="34" t="s">
         <v>346</v>
       </c>
-      <c r="J30" s="94"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="29">
-        <v>0</v>
-      </c>
-      <c r="M30" s="29">
-        <v>0</v>
-      </c>
+      <c r="L30" s="94"/>
+      <c r="M30" s="19"/>
       <c r="N30" s="29">
         <v>0</v>
       </c>
-      <c r="O30" s="91"/>
-      <c r="P30" s="94">
+      <c r="O30" s="29">
+        <v>0</v>
+      </c>
+      <c r="P30" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="91"/>
+      <c r="R30" s="94">
         <v>13</v>
       </c>
-      <c r="Q30" s="94">
+      <c r="S30" s="94">
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="53" t="s">
         <v>379</v>
       </c>
@@ -14971,39 +15167,41 @@
       <c r="D31" s="18">
         <v>1995</v>
       </c>
-      <c r="E31" s="18" t="s">
+      <c r="E31" s="18"/>
+      <c r="F31" s="202"/>
+      <c r="G31" s="18" t="s">
         <v>380</v>
       </c>
-      <c r="F31" s="29" t="s">
+      <c r="H31" s="29" t="s">
         <v>500</v>
       </c>
-      <c r="G31" s="191" t="s">
+      <c r="I31" s="191" t="s">
         <v>534</v>
       </c>
-      <c r="H31" s="29"/>
-      <c r="I31" s="34" t="s">
+      <c r="J31" s="29"/>
+      <c r="K31" s="34" t="s">
         <v>346</v>
       </c>
-      <c r="J31" s="94"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="29">
-        <v>1</v>
-      </c>
-      <c r="M31" s="29">
-        <v>1</v>
-      </c>
+      <c r="L31" s="94"/>
+      <c r="M31" s="19"/>
       <c r="N31" s="29">
         <v>1</v>
       </c>
-      <c r="O31" s="91"/>
-      <c r="P31" s="94">
+      <c r="O31" s="29">
+        <v>1</v>
+      </c>
+      <c r="P31" s="29">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="91"/>
+      <c r="R31" s="94">
         <v>16</v>
       </c>
-      <c r="Q31" s="94">
+      <c r="S31" s="94">
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="53" t="s">
         <v>383</v>
       </c>
@@ -15016,37 +15214,39 @@
       <c r="D32" s="18">
         <v>2010</v>
       </c>
-      <c r="E32" s="18" t="s">
+      <c r="E32" s="18"/>
+      <c r="F32" s="202"/>
+      <c r="G32" s="18" t="s">
         <v>384</v>
       </c>
-      <c r="F32" s="184" t="s">
+      <c r="H32" s="184" t="s">
         <v>479</v>
       </c>
-      <c r="G32" s="191"/>
-      <c r="H32" s="184" t="s">
+      <c r="I32" s="191"/>
+      <c r="J32" s="184" t="s">
         <v>346</v>
       </c>
-      <c r="I32" s="94"/>
-      <c r="J32" s="94"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="29">
+      <c r="K32" s="94"/>
+      <c r="L32" s="94"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="29">
         <v>50</v>
       </c>
-      <c r="M32" s="29">
+      <c r="O32" s="29">
         <v>32</v>
       </c>
-      <c r="N32" s="29">
+      <c r="P32" s="29">
         <v>0</v>
       </c>
-      <c r="O32" s="91"/>
-      <c r="P32" s="94">
+      <c r="Q32" s="91"/>
+      <c r="R32" s="94">
         <v>26</v>
       </c>
-      <c r="Q32" s="94">
+      <c r="S32" s="94">
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="53" t="s">
         <v>387</v>
       </c>
@@ -15059,39 +15259,41 @@
       <c r="D33" s="18">
         <v>2010</v>
       </c>
-      <c r="E33" s="18" t="s">
+      <c r="E33" s="18"/>
+      <c r="F33" s="202"/>
+      <c r="G33" s="18" t="s">
         <v>388</v>
       </c>
-      <c r="F33" s="184" t="s">
+      <c r="H33" s="184" t="s">
         <v>480</v>
       </c>
-      <c r="G33" s="191" t="s">
+      <c r="I33" s="191" t="s">
         <v>562</v>
       </c>
-      <c r="H33" s="184" t="s">
+      <c r="J33" s="184" t="s">
         <v>346</v>
       </c>
-      <c r="I33" s="94"/>
-      <c r="J33" s="94"/>
-      <c r="K33" s="19"/>
-      <c r="L33" s="29">
+      <c r="K33" s="94"/>
+      <c r="L33" s="94"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="29">
         <v>5</v>
       </c>
-      <c r="M33" s="29">
+      <c r="O33" s="29">
         <v>4</v>
       </c>
-      <c r="N33" s="29">
+      <c r="P33" s="29">
         <v>1</v>
       </c>
-      <c r="O33" s="91"/>
-      <c r="P33" s="94">
+      <c r="Q33" s="91"/>
+      <c r="R33" s="94">
         <v>21</v>
       </c>
-      <c r="Q33" s="94">
+      <c r="S33" s="94">
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="53" t="s">
         <v>391</v>
       </c>
@@ -15104,43 +15306,45 @@
       <c r="D34" s="18">
         <v>2000</v>
       </c>
-      <c r="E34" s="18" t="s">
+      <c r="E34" s="18"/>
+      <c r="F34" s="202"/>
+      <c r="G34" s="18" t="s">
         <v>392</v>
       </c>
-      <c r="F34" s="184" t="s">
+      <c r="H34" s="184" t="s">
         <v>499</v>
       </c>
-      <c r="G34" s="191" t="s">
+      <c r="I34" s="191" t="s">
         <v>535</v>
       </c>
-      <c r="H34" s="184" t="s">
+      <c r="J34" s="184" t="s">
         <v>346</v>
       </c>
-      <c r="I34" s="94"/>
-      <c r="J34" s="185" t="s">
+      <c r="K34" s="94"/>
+      <c r="L34" s="185" t="s">
         <v>346</v>
       </c>
-      <c r="K34" s="189" t="s">
+      <c r="M34" s="189" t="s">
         <v>528</v>
       </c>
-      <c r="L34" s="29">
+      <c r="N34" s="29">
         <v>55</v>
       </c>
-      <c r="M34" s="29">
+      <c r="O34" s="29">
         <v>51</v>
       </c>
-      <c r="N34" s="29">
+      <c r="P34" s="29">
         <v>4</v>
       </c>
-      <c r="O34" s="91"/>
-      <c r="P34" s="94">
+      <c r="Q34" s="91"/>
+      <c r="R34" s="94">
         <v>8</v>
       </c>
-      <c r="Q34" s="94">
+      <c r="S34" s="94">
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="53" t="s">
         <v>395</v>
       </c>
@@ -15153,39 +15357,41 @@
       <c r="D35" s="18">
         <v>2014</v>
       </c>
-      <c r="E35" s="18" t="s">
+      <c r="E35" s="18"/>
+      <c r="F35" s="202"/>
+      <c r="G35" s="18" t="s">
         <v>396</v>
       </c>
-      <c r="F35" s="29" t="s">
+      <c r="H35" s="29" t="s">
         <v>481</v>
       </c>
-      <c r="G35" s="193" t="s">
+      <c r="I35" s="193" t="s">
         <v>536</v>
       </c>
-      <c r="H35" s="94"/>
-      <c r="I35" s="34" t="s">
+      <c r="J35" s="94"/>
+      <c r="K35" s="34" t="s">
         <v>346</v>
       </c>
-      <c r="J35" s="94"/>
-      <c r="K35" s="19"/>
-      <c r="L35" s="29">
+      <c r="L35" s="94"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="29">
         <v>4</v>
       </c>
-      <c r="M35" s="29">
+      <c r="O35" s="29">
         <v>1</v>
       </c>
-      <c r="N35" s="29">
+      <c r="P35" s="29">
         <v>1</v>
       </c>
-      <c r="O35" s="91"/>
-      <c r="P35" s="94">
+      <c r="Q35" s="91"/>
+      <c r="R35" s="94">
         <v>18</v>
       </c>
-      <c r="Q35" s="94">
+      <c r="S35" s="94">
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="53" t="s">
         <v>400</v>
       </c>
@@ -15198,39 +15404,41 @@
       <c r="D36" s="18">
         <v>2010</v>
       </c>
-      <c r="E36" s="18" t="s">
+      <c r="E36" s="18"/>
+      <c r="F36" s="202"/>
+      <c r="G36" s="18" t="s">
         <v>401</v>
       </c>
-      <c r="F36" s="184" t="s">
+      <c r="H36" s="184" t="s">
         <v>482</v>
       </c>
-      <c r="G36" s="193" t="s">
+      <c r="I36" s="193" t="s">
         <v>537</v>
       </c>
-      <c r="H36" s="184" t="s">
+      <c r="J36" s="184" t="s">
         <v>346</v>
       </c>
-      <c r="I36" s="94"/>
-      <c r="J36" s="94"/>
-      <c r="K36" s="19"/>
-      <c r="L36" s="29">
+      <c r="K36" s="94"/>
+      <c r="L36" s="94"/>
+      <c r="M36" s="19"/>
+      <c r="N36" s="29">
         <v>5</v>
       </c>
-      <c r="M36" s="29">
+      <c r="O36" s="29">
         <v>4</v>
       </c>
-      <c r="N36" s="29">
+      <c r="P36" s="29">
         <v>1</v>
       </c>
-      <c r="O36" s="91"/>
-      <c r="P36" s="94">
+      <c r="Q36" s="91"/>
+      <c r="R36" s="94">
         <v>45</v>
       </c>
-      <c r="Q36" s="94">
+      <c r="S36" s="94">
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="53" t="s">
         <v>404</v>
       </c>
@@ -15243,39 +15451,41 @@
       <c r="D37" s="18">
         <v>2010</v>
       </c>
-      <c r="E37" s="18" t="s">
+      <c r="E37" s="18"/>
+      <c r="F37" s="202"/>
+      <c r="G37" s="18" t="s">
         <v>401</v>
       </c>
-      <c r="F37" s="184" t="s">
+      <c r="H37" s="184" t="s">
         <v>483</v>
       </c>
-      <c r="G37" s="193" t="s">
+      <c r="I37" s="193" t="s">
         <v>544</v>
       </c>
-      <c r="H37" s="184" t="s">
+      <c r="J37" s="184" t="s">
         <v>346</v>
       </c>
-      <c r="I37" s="94"/>
-      <c r="J37" s="94"/>
-      <c r="K37" s="19"/>
-      <c r="L37" s="29">
+      <c r="K37" s="94"/>
+      <c r="L37" s="94"/>
+      <c r="M37" s="19"/>
+      <c r="N37" s="29">
         <v>3</v>
       </c>
-      <c r="M37" s="29">
+      <c r="O37" s="29">
         <v>2</v>
       </c>
-      <c r="N37" s="29">
+      <c r="P37" s="29">
         <v>0</v>
       </c>
-      <c r="O37" s="91"/>
-      <c r="P37" s="94">
+      <c r="Q37" s="91"/>
+      <c r="R37" s="94">
         <v>28</v>
       </c>
-      <c r="Q37" s="94">
+      <c r="S37" s="94">
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="53" t="s">
         <v>407</v>
       </c>
@@ -15288,39 +15498,41 @@
       <c r="D38" s="18">
         <v>2005</v>
       </c>
-      <c r="E38" s="18" t="s">
+      <c r="E38" s="18"/>
+      <c r="F38" s="202"/>
+      <c r="G38" s="18" t="s">
         <v>408</v>
       </c>
-      <c r="F38" s="184" t="s">
+      <c r="H38" s="184" t="s">
         <v>484</v>
       </c>
-      <c r="G38" s="193" t="s">
+      <c r="I38" s="193" t="s">
         <v>563</v>
       </c>
-      <c r="H38" s="184" t="s">
+      <c r="J38" s="184" t="s">
         <v>346</v>
       </c>
-      <c r="I38" s="94"/>
-      <c r="J38" s="94"/>
-      <c r="K38" s="19"/>
-      <c r="L38" s="29">
+      <c r="K38" s="94"/>
+      <c r="L38" s="94"/>
+      <c r="M38" s="19"/>
+      <c r="N38" s="29">
         <v>14</v>
       </c>
-      <c r="M38" s="29">
+      <c r="O38" s="29">
         <v>15</v>
       </c>
-      <c r="N38" s="29">
+      <c r="P38" s="29">
         <v>3</v>
       </c>
-      <c r="O38" s="91"/>
-      <c r="P38" s="94">
+      <c r="Q38" s="91"/>
+      <c r="R38" s="94">
         <v>14</v>
       </c>
-      <c r="Q38" s="94">
+      <c r="S38" s="94">
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="53" t="s">
         <v>411</v>
       </c>
@@ -15333,37 +15545,39 @@
       <c r="D39" s="18">
         <v>1998</v>
       </c>
-      <c r="E39" s="18" t="s">
+      <c r="E39" s="18"/>
+      <c r="F39" s="202"/>
+      <c r="G39" s="18" t="s">
         <v>412</v>
       </c>
-      <c r="F39" s="184" t="s">
+      <c r="H39" s="184" t="s">
         <v>498</v>
       </c>
-      <c r="G39" s="191"/>
-      <c r="H39" s="184" t="s">
+      <c r="I39" s="191"/>
+      <c r="J39" s="184" t="s">
         <v>346</v>
       </c>
-      <c r="I39" s="94"/>
-      <c r="J39" s="94"/>
-      <c r="K39" s="19"/>
-      <c r="L39" s="29">
+      <c r="K39" s="94"/>
+      <c r="L39" s="94"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="29">
         <v>1</v>
       </c>
-      <c r="M39" s="29">
+      <c r="O39" s="29">
         <v>2</v>
       </c>
-      <c r="N39" s="29">
+      <c r="P39" s="29">
         <v>2</v>
       </c>
-      <c r="O39" s="91"/>
-      <c r="P39" s="94">
+      <c r="Q39" s="91"/>
+      <c r="R39" s="94">
         <v>5</v>
       </c>
-      <c r="Q39" s="94">
+      <c r="S39" s="94">
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="53" t="s">
         <v>415</v>
       </c>
@@ -15376,39 +15590,41 @@
       <c r="D40" s="18">
         <v>2007</v>
       </c>
-      <c r="E40" s="18" t="s">
+      <c r="E40" s="18"/>
+      <c r="F40" s="202"/>
+      <c r="G40" s="18" t="s">
         <v>420</v>
       </c>
-      <c r="F40" s="184" t="s">
+      <c r="H40" s="184" t="s">
         <v>485</v>
       </c>
-      <c r="G40" s="193" t="s">
+      <c r="I40" s="193" t="s">
         <v>546</v>
       </c>
-      <c r="H40" s="184" t="s">
+      <c r="J40" s="184" t="s">
         <v>346</v>
       </c>
-      <c r="I40" s="94"/>
-      <c r="J40" s="94"/>
-      <c r="K40" s="19"/>
-      <c r="L40" s="29">
+      <c r="K40" s="94"/>
+      <c r="L40" s="94"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="29">
         <v>58</v>
       </c>
-      <c r="M40" s="29">
+      <c r="O40" s="29">
         <v>39</v>
       </c>
-      <c r="N40" s="29">
+      <c r="P40" s="29">
         <v>5</v>
       </c>
-      <c r="O40" s="91"/>
-      <c r="P40" s="94">
+      <c r="Q40" s="91"/>
+      <c r="R40" s="94">
         <v>15</v>
       </c>
-      <c r="Q40" s="94">
+      <c r="S40" s="94">
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="53" t="s">
         <v>417</v>
       </c>
@@ -15421,43 +15637,45 @@
       <c r="D41" s="18">
         <v>2014</v>
       </c>
-      <c r="E41" s="18" t="s">
+      <c r="E41" s="18"/>
+      <c r="F41" s="202"/>
+      <c r="G41" s="18" t="s">
         <v>418</v>
       </c>
-      <c r="F41" s="184" t="s">
+      <c r="H41" s="184" t="s">
         <v>497</v>
       </c>
-      <c r="G41" s="191" t="s">
+      <c r="I41" s="191" t="s">
         <v>538</v>
       </c>
-      <c r="H41" s="184" t="s">
+      <c r="J41" s="184" t="s">
         <v>346</v>
       </c>
-      <c r="I41" s="94"/>
-      <c r="J41" s="185" t="s">
+      <c r="K41" s="94"/>
+      <c r="L41" s="185" t="s">
         <v>346</v>
       </c>
-      <c r="K41" s="189" t="s">
+      <c r="M41" s="189" t="s">
         <v>527</v>
       </c>
-      <c r="L41" s="29">
+      <c r="N41" s="29">
         <v>1</v>
       </c>
-      <c r="M41" s="29">
+      <c r="O41" s="29">
         <v>0</v>
       </c>
-      <c r="N41" s="29">
+      <c r="P41" s="29">
         <v>0</v>
       </c>
-      <c r="O41" s="91"/>
-      <c r="P41" s="94">
+      <c r="Q41" s="91"/>
+      <c r="R41" s="94">
         <v>70</v>
       </c>
-      <c r="Q41" s="94">
+      <c r="S41" s="94">
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="53" t="s">
         <v>423</v>
       </c>
@@ -15470,39 +15688,41 @@
       <c r="D42" s="18">
         <v>2013</v>
       </c>
-      <c r="E42" s="18" t="s">
+      <c r="E42" s="18"/>
+      <c r="F42" s="202"/>
+      <c r="G42" s="18" t="s">
         <v>424</v>
       </c>
-      <c r="F42" s="184" t="s">
+      <c r="H42" s="184" t="s">
         <v>506</v>
       </c>
-      <c r="G42" s="193" t="s">
+      <c r="I42" s="193" t="s">
         <v>539</v>
       </c>
-      <c r="H42" s="184" t="s">
+      <c r="J42" s="184" t="s">
         <v>346</v>
       </c>
-      <c r="I42" s="94"/>
-      <c r="J42" s="94"/>
-      <c r="K42" s="19"/>
-      <c r="L42" s="29">
+      <c r="K42" s="94"/>
+      <c r="L42" s="94"/>
+      <c r="M42" s="19"/>
+      <c r="N42" s="29">
         <v>17</v>
       </c>
-      <c r="M42" s="29">
+      <c r="O42" s="29">
         <v>10</v>
       </c>
-      <c r="N42" s="29">
+      <c r="P42" s="29">
         <v>2</v>
       </c>
-      <c r="O42" s="91"/>
-      <c r="P42" s="94">
+      <c r="Q42" s="91"/>
+      <c r="R42" s="94">
         <v>31</v>
       </c>
-      <c r="Q42" s="94">
+      <c r="S42" s="94">
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="53" t="s">
         <v>426</v>
       </c>
@@ -15515,39 +15735,41 @@
       <c r="D43" s="18">
         <v>2013</v>
       </c>
-      <c r="E43" s="18" t="s">
+      <c r="E43" s="18"/>
+      <c r="F43" s="202"/>
+      <c r="G43" s="18" t="s">
         <v>424</v>
       </c>
-      <c r="F43" s="98" t="s">
+      <c r="H43" s="98" t="s">
         <v>496</v>
       </c>
-      <c r="G43" s="194" t="s">
+      <c r="I43" s="194" t="s">
         <v>540</v>
       </c>
-      <c r="H43" s="98"/>
-      <c r="I43" s="34" t="s">
+      <c r="J43" s="98"/>
+      <c r="K43" s="34" t="s">
         <v>346</v>
       </c>
-      <c r="J43" s="94"/>
-      <c r="K43" s="19"/>
-      <c r="L43" s="195">
+      <c r="L43" s="94"/>
+      <c r="M43" s="19"/>
+      <c r="N43" s="195">
         <v>6</v>
       </c>
-      <c r="M43" s="98">
+      <c r="O43" s="98">
         <v>1</v>
       </c>
-      <c r="N43" s="98">
+      <c r="P43" s="98">
         <v>1</v>
       </c>
-      <c r="O43" s="91"/>
-      <c r="P43" s="94">
+      <c r="Q43" s="91"/>
+      <c r="R43" s="94">
         <v>15</v>
       </c>
-      <c r="Q43" s="94">
+      <c r="S43" s="94">
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="53" t="s">
         <v>429</v>
       </c>
@@ -15560,37 +15782,39 @@
       <c r="D44" s="18">
         <v>2007</v>
       </c>
-      <c r="E44" s="18" t="s">
+      <c r="E44" s="18"/>
+      <c r="F44" s="202"/>
+      <c r="G44" s="18" t="s">
         <v>430</v>
       </c>
-      <c r="F44" s="184" t="s">
+      <c r="H44" s="184" t="s">
         <v>486</v>
       </c>
-      <c r="G44" s="6"/>
-      <c r="H44" s="184" t="s">
+      <c r="I44" s="6"/>
+      <c r="J44" s="184" t="s">
         <v>346</v>
       </c>
-      <c r="I44" s="94"/>
-      <c r="J44" s="94"/>
-      <c r="K44" s="19"/>
-      <c r="L44" s="190">
+      <c r="K44" s="94"/>
+      <c r="L44" s="94"/>
+      <c r="M44" s="19"/>
+      <c r="N44" s="190">
         <v>69</v>
       </c>
-      <c r="M44" s="29">
+      <c r="O44" s="29">
         <v>51</v>
       </c>
-      <c r="N44" s="29">
+      <c r="P44" s="29">
         <v>5</v>
       </c>
-      <c r="O44" s="91"/>
-      <c r="P44" s="94">
+      <c r="Q44" s="91"/>
+      <c r="R44" s="94">
         <v>7</v>
       </c>
-      <c r="Q44" s="94">
+      <c r="S44" s="94">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="53" t="s">
         <v>433</v>
       </c>
@@ -15603,39 +15827,41 @@
       <c r="D45" s="18">
         <v>2011</v>
       </c>
-      <c r="E45" s="18" t="s">
+      <c r="E45" s="18"/>
+      <c r="F45" s="202"/>
+      <c r="G45" s="18" t="s">
         <v>434</v>
       </c>
-      <c r="F45" s="29" t="s">
+      <c r="H45" s="29" t="s">
         <v>487</v>
       </c>
-      <c r="G45" s="193" t="s">
+      <c r="I45" s="193" t="s">
         <v>541</v>
       </c>
-      <c r="H45" s="94"/>
-      <c r="I45" s="34" t="s">
+      <c r="J45" s="94"/>
+      <c r="K45" s="34" t="s">
         <v>346</v>
       </c>
-      <c r="J45" s="94"/>
-      <c r="K45" s="19"/>
-      <c r="L45" s="29">
+      <c r="L45" s="94"/>
+      <c r="M45" s="19"/>
+      <c r="N45" s="29">
         <v>17</v>
       </c>
-      <c r="M45" s="29">
+      <c r="O45" s="29">
         <v>10</v>
       </c>
-      <c r="N45" s="29">
+      <c r="P45" s="29">
         <v>2</v>
       </c>
-      <c r="O45" s="91"/>
-      <c r="P45" s="94">
+      <c r="Q45" s="91"/>
+      <c r="R45" s="94">
         <v>7</v>
       </c>
-      <c r="Q45" s="94">
+      <c r="S45" s="94">
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="53" t="s">
         <v>437</v>
       </c>
@@ -15648,39 +15874,41 @@
       <c r="D46" s="18">
         <v>2007</v>
       </c>
-      <c r="E46" s="18" t="s">
+      <c r="E46" s="18"/>
+      <c r="F46" s="202"/>
+      <c r="G46" s="18" t="s">
         <v>438</v>
       </c>
-      <c r="F46" s="29" t="s">
+      <c r="H46" s="29" t="s">
         <v>495</v>
       </c>
-      <c r="G46" s="191" t="s">
+      <c r="I46" s="191" t="s">
         <v>548</v>
       </c>
-      <c r="H46" s="29"/>
-      <c r="I46" s="34" t="s">
+      <c r="J46" s="29"/>
+      <c r="K46" s="34" t="s">
         <v>346</v>
       </c>
-      <c r="J46" s="94"/>
-      <c r="K46" s="19"/>
-      <c r="L46" s="29">
+      <c r="L46" s="94"/>
+      <c r="M46" s="19"/>
+      <c r="N46" s="29">
         <v>15</v>
       </c>
-      <c r="M46" s="29">
+      <c r="O46" s="29">
         <v>14</v>
       </c>
-      <c r="N46" s="29">
+      <c r="P46" s="29">
         <v>2</v>
       </c>
-      <c r="O46" s="91"/>
-      <c r="P46" s="94">
+      <c r="Q46" s="91"/>
+      <c r="R46" s="94">
         <v>14</v>
       </c>
-      <c r="Q46" s="94">
+      <c r="S46" s="94">
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="53" t="s">
         <v>440</v>
       </c>
@@ -15693,39 +15921,41 @@
       <c r="D47" s="18">
         <v>2010</v>
       </c>
-      <c r="E47" s="18" t="s">
+      <c r="E47" s="18"/>
+      <c r="F47" s="202"/>
+      <c r="G47" s="18" t="s">
         <v>441</v>
       </c>
-      <c r="F47" s="29" t="s">
+      <c r="H47" s="29" t="s">
         <v>494</v>
       </c>
-      <c r="G47" s="191" t="s">
+      <c r="I47" s="191" t="s">
         <v>533</v>
       </c>
-      <c r="H47" s="29"/>
-      <c r="I47" s="34" t="s">
+      <c r="J47" s="29"/>
+      <c r="K47" s="34" t="s">
         <v>346</v>
       </c>
-      <c r="J47" s="94"/>
-      <c r="K47" s="19"/>
-      <c r="L47" s="29">
-        <v>0</v>
-      </c>
-      <c r="M47" s="29">
-        <v>0</v>
-      </c>
+      <c r="L47" s="94"/>
+      <c r="M47" s="19"/>
       <c r="N47" s="29">
         <v>0</v>
       </c>
-      <c r="O47" s="91"/>
-      <c r="P47" s="94">
+      <c r="O47" s="29">
+        <v>0</v>
+      </c>
+      <c r="P47" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="91"/>
+      <c r="R47" s="94">
         <v>27</v>
       </c>
-      <c r="Q47" s="94">
+      <c r="S47" s="94">
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="53" t="s">
         <v>444</v>
       </c>
@@ -15738,41 +15968,43 @@
       <c r="D48" s="18">
         <v>2006</v>
       </c>
-      <c r="E48" s="18" t="s">
+      <c r="E48" s="18"/>
+      <c r="F48" s="202"/>
+      <c r="G48" s="18" t="s">
         <v>408</v>
       </c>
-      <c r="F48" s="29" t="s">
+      <c r="H48" s="29" t="s">
         <v>488</v>
       </c>
-      <c r="G48" s="193" t="s">
+      <c r="I48" s="193" t="s">
         <v>544</v>
       </c>
-      <c r="H48" s="85"/>
-      <c r="I48" s="85"/>
-      <c r="J48" s="85" t="s">
+      <c r="J48" s="85"/>
+      <c r="K48" s="85"/>
+      <c r="L48" s="85" t="s">
         <v>346</v>
       </c>
-      <c r="K48" s="19" t="s">
+      <c r="M48" s="19" t="s">
         <v>568</v>
       </c>
-      <c r="L48" s="29">
+      <c r="N48" s="29">
         <v>11</v>
       </c>
-      <c r="M48" s="29">
+      <c r="O48" s="29">
         <v>10</v>
       </c>
-      <c r="N48" s="29">
+      <c r="P48" s="29">
         <v>2</v>
       </c>
-      <c r="O48" s="91"/>
-      <c r="P48" s="94">
+      <c r="Q48" s="91"/>
+      <c r="R48" s="94">
         <v>19</v>
       </c>
-      <c r="Q48" s="94">
+      <c r="S48" s="94">
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="53" t="s">
         <v>447</v>
       </c>
@@ -15785,39 +16017,41 @@
       <c r="D49" s="18">
         <v>2011</v>
       </c>
-      <c r="E49" s="18" t="s">
+      <c r="E49" s="18"/>
+      <c r="F49" s="202"/>
+      <c r="G49" s="18" t="s">
         <v>448</v>
       </c>
-      <c r="F49" s="29" t="s">
+      <c r="H49" s="29" t="s">
         <v>489</v>
       </c>
-      <c r="G49" s="191" t="s">
+      <c r="I49" s="191" t="s">
         <v>542</v>
       </c>
-      <c r="H49" s="29"/>
-      <c r="I49" s="34" t="s">
+      <c r="J49" s="29"/>
+      <c r="K49" s="34" t="s">
         <v>346</v>
       </c>
-      <c r="J49" s="94"/>
-      <c r="K49" s="19"/>
-      <c r="L49" s="29">
+      <c r="L49" s="94"/>
+      <c r="M49" s="19"/>
+      <c r="N49" s="29">
         <v>4</v>
       </c>
-      <c r="M49" s="29">
+      <c r="O49" s="29">
         <v>3</v>
       </c>
-      <c r="N49" s="29">
+      <c r="P49" s="29">
         <v>0</v>
       </c>
-      <c r="O49" s="91"/>
-      <c r="P49" s="94">
+      <c r="Q49" s="91"/>
+      <c r="R49" s="94">
         <v>19</v>
       </c>
-      <c r="Q49" s="94">
+      <c r="S49" s="94">
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="53" t="s">
         <v>451</v>
       </c>
@@ -15830,39 +16064,41 @@
       <c r="D50" s="18">
         <v>2004</v>
       </c>
-      <c r="E50" s="18" t="s">
+      <c r="E50" s="18"/>
+      <c r="F50" s="202"/>
+      <c r="G50" s="18" t="s">
         <v>455</v>
       </c>
-      <c r="F50" s="184" t="s">
+      <c r="H50" s="184" t="s">
         <v>490</v>
       </c>
-      <c r="G50" s="191" t="s">
+      <c r="I50" s="191" t="s">
         <v>534</v>
       </c>
-      <c r="H50" s="184" t="s">
+      <c r="J50" s="184" t="s">
         <v>346</v>
       </c>
-      <c r="I50" s="94"/>
-      <c r="J50" s="94"/>
-      <c r="K50" s="19"/>
-      <c r="L50" s="29">
+      <c r="K50" s="94"/>
+      <c r="L50" s="94"/>
+      <c r="M50" s="19"/>
+      <c r="N50" s="29">
         <v>1</v>
       </c>
-      <c r="M50" s="29">
+      <c r="O50" s="29">
         <v>1</v>
       </c>
-      <c r="N50" s="29">
+      <c r="P50" s="29">
         <v>0</v>
       </c>
-      <c r="O50" s="91"/>
-      <c r="P50" s="94">
+      <c r="Q50" s="91"/>
+      <c r="R50" s="94">
         <v>13</v>
       </c>
-      <c r="Q50" s="94">
+      <c r="S50" s="94">
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="53" t="s">
         <v>452</v>
       </c>
@@ -15875,37 +16111,39 @@
       <c r="D51" s="18">
         <v>2010</v>
       </c>
-      <c r="E51" s="18" t="s">
+      <c r="E51" s="18"/>
+      <c r="F51" s="202"/>
+      <c r="G51" s="18" t="s">
         <v>457</v>
       </c>
-      <c r="F51" s="184" t="s">
+      <c r="H51" s="184" t="s">
         <v>493</v>
       </c>
-      <c r="G51" s="191"/>
-      <c r="H51" s="184" t="s">
+      <c r="I51" s="191"/>
+      <c r="J51" s="184" t="s">
         <v>346</v>
       </c>
-      <c r="I51" s="94"/>
-      <c r="J51" s="94"/>
-      <c r="K51" s="19"/>
-      <c r="L51" s="29">
+      <c r="K51" s="94"/>
+      <c r="L51" s="94"/>
+      <c r="M51" s="19"/>
+      <c r="N51" s="29">
         <v>5</v>
       </c>
-      <c r="M51" s="29">
+      <c r="O51" s="29">
         <v>4</v>
       </c>
-      <c r="N51" s="29">
+      <c r="P51" s="29">
         <v>2</v>
       </c>
-      <c r="O51" s="91"/>
-      <c r="P51" s="94">
+      <c r="Q51" s="91"/>
+      <c r="R51" s="94">
         <v>8</v>
       </c>
-      <c r="Q51" s="94">
+      <c r="S51" s="94">
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="53" t="s">
         <v>453</v>
       </c>
@@ -15918,39 +16156,41 @@
       <c r="D52" s="18">
         <v>2003</v>
       </c>
-      <c r="E52" s="18" t="s">
+      <c r="E52" s="18"/>
+      <c r="F52" s="202"/>
+      <c r="G52" s="18" t="s">
         <v>460</v>
       </c>
-      <c r="F52" s="29" t="s">
+      <c r="H52" s="29" t="s">
         <v>491</v>
       </c>
-      <c r="G52" s="191" t="s">
+      <c r="I52" s="191" t="s">
         <v>543</v>
       </c>
-      <c r="H52" s="29"/>
-      <c r="I52" s="34" t="s">
+      <c r="J52" s="29"/>
+      <c r="K52" s="34" t="s">
         <v>346</v>
       </c>
-      <c r="J52" s="94"/>
-      <c r="K52" s="19"/>
-      <c r="L52" s="29">
+      <c r="L52" s="94"/>
+      <c r="M52" s="19"/>
+      <c r="N52" s="29">
         <v>84</v>
       </c>
-      <c r="M52" s="29">
+      <c r="O52" s="29">
         <v>66</v>
       </c>
-      <c r="N52" s="29">
+      <c r="P52" s="29">
         <v>2</v>
       </c>
-      <c r="O52" s="91"/>
-      <c r="P52" s="94">
+      <c r="Q52" s="91"/>
+      <c r="R52" s="94">
         <v>13</v>
       </c>
-      <c r="Q52" s="94">
+      <c r="S52" s="94">
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="53" t="s">
         <v>454</v>
       </c>
@@ -15963,41 +16203,43 @@
       <c r="D53" s="18">
         <v>2007</v>
       </c>
-      <c r="E53" s="18" t="s">
+      <c r="E53" s="18"/>
+      <c r="F53" s="202"/>
+      <c r="G53" s="18" t="s">
         <v>420</v>
       </c>
-      <c r="F53" s="184" t="s">
+      <c r="H53" s="184" t="s">
         <v>492</v>
       </c>
-      <c r="G53" s="191" t="s">
+      <c r="I53" s="191" t="s">
         <v>547</v>
       </c>
-      <c r="H53" s="184" t="s">
+      <c r="J53" s="184" t="s">
         <v>346</v>
       </c>
-      <c r="I53" s="94"/>
-      <c r="J53" s="94"/>
-      <c r="K53" s="19"/>
-      <c r="L53" s="29">
+      <c r="K53" s="94"/>
+      <c r="L53" s="94"/>
+      <c r="M53" s="19"/>
+      <c r="N53" s="29">
         <v>37</v>
       </c>
-      <c r="M53" s="29">
+      <c r="O53" s="29">
         <v>28</v>
       </c>
-      <c r="N53" s="29">
+      <c r="P53" s="29">
         <v>4</v>
       </c>
-      <c r="O53" s="91"/>
-      <c r="P53" s="94">
+      <c r="Q53" s="91"/>
+      <c r="R53" s="94">
         <v>10</v>
       </c>
-      <c r="Q53" s="94">
+      <c r="S53" s="94">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="A1:S1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -16008,8 +16250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S54"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16024,43 +16266,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="226" t="s">
+      <c r="A1" s="227" t="s">
         <v>230</v>
       </c>
-      <c r="B1" s="227"/>
-      <c r="C1" s="227"/>
-      <c r="D1" s="227"/>
-      <c r="E1" s="227"/>
-      <c r="F1" s="227"/>
-      <c r="G1" s="227"/>
-      <c r="H1" s="227"/>
-      <c r="I1" s="227"/>
+      <c r="B1" s="228"/>
+      <c r="C1" s="228"/>
+      <c r="D1" s="228"/>
+      <c r="E1" s="228"/>
+      <c r="F1" s="228"/>
+      <c r="G1" s="228"/>
+      <c r="H1" s="228"/>
+      <c r="I1" s="228"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="225" t="s">
+      <c r="A2" s="230" t="s">
         <v>229</v>
       </c>
-      <c r="B2" s="225"/>
-      <c r="C2" s="225"/>
-      <c r="D2" s="225"/>
-      <c r="E2" s="225"/>
-      <c r="F2" s="225"/>
-      <c r="G2" s="225"/>
-      <c r="H2" s="225"/>
-      <c r="I2" s="225"/>
+      <c r="B2" s="230"/>
+      <c r="C2" s="230"/>
+      <c r="D2" s="230"/>
+      <c r="E2" s="230"/>
+      <c r="F2" s="230"/>
+      <c r="G2" s="230"/>
+      <c r="H2" s="230"/>
+      <c r="I2" s="230"/>
     </row>
     <row r="3" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="218" t="s">
+      <c r="A3" s="231" t="s">
         <v>337</v>
       </c>
-      <c r="B3" s="218"/>
-      <c r="C3" s="218"/>
-      <c r="D3" s="218"/>
-      <c r="E3" s="218"/>
-      <c r="F3" s="218"/>
-      <c r="G3" s="218"/>
-      <c r="H3" s="218"/>
-      <c r="I3" s="218"/>
+      <c r="B3" s="231"/>
+      <c r="C3" s="231"/>
+      <c r="D3" s="231"/>
+      <c r="E3" s="231"/>
+      <c r="F3" s="231"/>
+      <c r="G3" s="231"/>
+      <c r="H3" s="231"/>
+      <c r="I3" s="231"/>
       <c r="J3" s="71"/>
       <c r="K3" s="71"/>
       <c r="L3" s="71"/>
@@ -16073,12 +16315,12 @@
       <c r="S3" s="71"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="228" t="s">
+      <c r="A4" s="229" t="s">
         <v>253</v>
       </c>
-      <c r="B4" s="228"/>
-      <c r="C4" s="228"/>
-      <c r="D4" s="228"/>
+      <c r="B4" s="229"/>
+      <c r="C4" s="229"/>
+      <c r="D4" s="229"/>
     </row>
     <row r="5" spans="1:19" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="69" t="s">
@@ -16104,7 +16346,7 @@
       <c r="C6" s="49" t="s">
         <v>196</v>
       </c>
-      <c r="D6" s="222" t="s">
+      <c r="D6" s="240" t="s">
         <v>339</v>
       </c>
       <c r="E6" t="e">
@@ -16123,7 +16365,7 @@
       <c r="C7" s="49" t="s">
         <v>228</v>
       </c>
-      <c r="D7" s="223"/>
+      <c r="D7" s="241"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="78" t="s">
@@ -16135,7 +16377,7 @@
       <c r="C8" s="49" t="s">
         <v>235</v>
       </c>
-      <c r="D8" s="223"/>
+      <c r="D8" s="241"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="78" t="s">
@@ -16147,7 +16389,7 @@
       <c r="C9" s="49" t="s">
         <v>236</v>
       </c>
-      <c r="D9" s="223"/>
+      <c r="D9" s="241"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="78" t="s">
@@ -16159,7 +16401,7 @@
       <c r="C10" s="49" t="s">
         <v>237</v>
       </c>
-      <c r="D10" s="223"/>
+      <c r="D10" s="241"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="78" t="s">
@@ -16171,7 +16413,7 @@
       <c r="C11" s="49" t="s">
         <v>237</v>
       </c>
-      <c r="D11" s="223"/>
+      <c r="D11" s="241"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="78" t="s">
@@ -16183,7 +16425,7 @@
       <c r="C12" s="49" t="s">
         <v>266</v>
       </c>
-      <c r="D12" s="223"/>
+      <c r="D12" s="241"/>
     </row>
     <row r="13" spans="1:19" s="77" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="145" t="s">
@@ -16195,7 +16437,7 @@
       <c r="C13" s="136" t="s">
         <v>273</v>
       </c>
-      <c r="D13" s="224"/>
+      <c r="D13" s="242"/>
     </row>
     <row r="14" spans="1:19" s="77" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="146" t="s">
@@ -16212,30 +16454,30 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="225" t="s">
+      <c r="A15" s="230" t="s">
         <v>261</v>
       </c>
-      <c r="B15" s="225"/>
-      <c r="C15" s="225"/>
-      <c r="D15" s="225"/>
-      <c r="E15" s="225"/>
-      <c r="F15" s="225"/>
-      <c r="G15" s="225"/>
-      <c r="H15" s="225"/>
-      <c r="I15" s="225"/>
+      <c r="B15" s="230"/>
+      <c r="C15" s="230"/>
+      <c r="D15" s="230"/>
+      <c r="E15" s="230"/>
+      <c r="F15" s="230"/>
+      <c r="G15" s="230"/>
+      <c r="H15" s="230"/>
+      <c r="I15" s="230"/>
     </row>
     <row r="16" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="218" t="s">
+      <c r="A16" s="231" t="s">
         <v>238</v>
       </c>
-      <c r="B16" s="218"/>
-      <c r="C16" s="218"/>
-      <c r="D16" s="218"/>
-      <c r="E16" s="218"/>
-      <c r="F16" s="218"/>
-      <c r="G16" s="218"/>
-      <c r="H16" s="218"/>
-      <c r="I16" s="218"/>
+      <c r="B16" s="231"/>
+      <c r="C16" s="231"/>
+      <c r="D16" s="231"/>
+      <c r="E16" s="231"/>
+      <c r="F16" s="231"/>
+      <c r="G16" s="231"/>
+      <c r="H16" s="231"/>
+      <c r="I16" s="231"/>
       <c r="J16" s="71"/>
       <c r="K16" s="71"/>
       <c r="L16" s="71"/>
@@ -16248,14 +16490,14 @@
       <c r="S16" s="71"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="228" t="s">
+      <c r="A17" s="229" t="s">
         <v>259</v>
       </c>
-      <c r="B17" s="228"/>
-      <c r="C17" s="228"/>
-      <c r="D17" s="228"/>
-      <c r="E17" s="228"/>
-      <c r="F17" s="228"/>
+      <c r="B17" s="229"/>
+      <c r="C17" s="229"/>
+      <c r="D17" s="229"/>
+      <c r="E17" s="229"/>
+      <c r="F17" s="229"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="69" t="s">
@@ -16422,30 +16664,30 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="225" t="s">
+      <c r="A25" s="230" t="s">
         <v>260</v>
       </c>
-      <c r="B25" s="225"/>
-      <c r="C25" s="225"/>
-      <c r="D25" s="225"/>
-      <c r="E25" s="225"/>
-      <c r="F25" s="225"/>
-      <c r="G25" s="225"/>
-      <c r="H25" s="225"/>
-      <c r="I25" s="225"/>
+      <c r="B25" s="230"/>
+      <c r="C25" s="230"/>
+      <c r="D25" s="230"/>
+      <c r="E25" s="230"/>
+      <c r="F25" s="230"/>
+      <c r="G25" s="230"/>
+      <c r="H25" s="230"/>
+      <c r="I25" s="230"/>
     </row>
     <row r="26" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="218" t="s">
+      <c r="A26" s="231" t="s">
         <v>338</v>
       </c>
-      <c r="B26" s="218"/>
-      <c r="C26" s="218"/>
-      <c r="D26" s="218"/>
-      <c r="E26" s="218"/>
-      <c r="F26" s="218"/>
-      <c r="G26" s="218"/>
-      <c r="H26" s="218"/>
-      <c r="I26" s="218"/>
+      <c r="B26" s="231"/>
+      <c r="C26" s="231"/>
+      <c r="D26" s="231"/>
+      <c r="E26" s="231"/>
+      <c r="F26" s="231"/>
+      <c r="G26" s="231"/>
+      <c r="H26" s="231"/>
+      <c r="I26" s="231"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="69" t="s">
@@ -16457,12 +16699,12 @@
       <c r="C27" s="69" t="s">
         <v>201</v>
       </c>
-      <c r="D27" s="232" t="s">
+      <c r="D27" s="235" t="s">
         <v>292</v>
       </c>
-      <c r="E27" s="232"/>
-      <c r="F27" s="232"/>
-      <c r="G27" s="232"/>
+      <c r="E27" s="235"/>
+      <c r="F27" s="235"/>
+      <c r="G27" s="235"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="52" t="s">
@@ -16474,12 +16716,12 @@
       <c r="C28" s="72">
         <v>0.59</v>
       </c>
-      <c r="D28" s="219" t="s">
+      <c r="D28" s="237" t="s">
         <v>285</v>
       </c>
-      <c r="E28" s="220"/>
-      <c r="F28" s="220"/>
-      <c r="G28" s="221"/>
+      <c r="E28" s="238"/>
+      <c r="F28" s="238"/>
+      <c r="G28" s="239"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="52" t="s">
@@ -16491,12 +16733,12 @@
       <c r="C29" s="72">
         <v>0.77</v>
       </c>
-      <c r="D29" s="229" t="s">
+      <c r="D29" s="232" t="s">
         <v>286</v>
       </c>
-      <c r="E29" s="230"/>
-      <c r="F29" s="230"/>
-      <c r="G29" s="231"/>
+      <c r="E29" s="233"/>
+      <c r="F29" s="233"/>
+      <c r="G29" s="234"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="52" t="s">
@@ -16508,12 +16750,12 @@
       <c r="C30" s="72">
         <v>0.41</v>
       </c>
-      <c r="D30" s="229" t="s">
+      <c r="D30" s="232" t="s">
         <v>287</v>
       </c>
-      <c r="E30" s="230"/>
-      <c r="F30" s="230"/>
-      <c r="G30" s="231"/>
+      <c r="E30" s="233"/>
+      <c r="F30" s="233"/>
+      <c r="G30" s="234"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="52" t="s">
@@ -16525,12 +16767,12 @@
       <c r="C31" s="72">
         <v>0.59</v>
       </c>
-      <c r="D31" s="229" t="s">
+      <c r="D31" s="232" t="s">
         <v>289</v>
       </c>
-      <c r="E31" s="230"/>
-      <c r="F31" s="230"/>
-      <c r="G31" s="231"/>
+      <c r="E31" s="233"/>
+      <c r="F31" s="233"/>
+      <c r="G31" s="234"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="52" t="s">
@@ -16542,12 +16784,12 @@
       <c r="C32" s="72">
         <v>0.5</v>
       </c>
-      <c r="D32" s="229" t="s">
+      <c r="D32" s="232" t="s">
         <v>288</v>
       </c>
-      <c r="E32" s="230"/>
-      <c r="F32" s="230"/>
-      <c r="G32" s="231"/>
+      <c r="E32" s="233"/>
+      <c r="F32" s="233"/>
+      <c r="G32" s="234"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="52" t="s">
@@ -16559,12 +16801,12 @@
       <c r="C33" s="72">
         <v>0.59</v>
       </c>
-      <c r="D33" s="229" t="s">
+      <c r="D33" s="232" t="s">
         <v>290</v>
       </c>
-      <c r="E33" s="230"/>
-      <c r="F33" s="230"/>
-      <c r="G33" s="231"/>
+      <c r="E33" s="233"/>
+      <c r="F33" s="233"/>
+      <c r="G33" s="234"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="52" t="s">
@@ -16576,25 +16818,25 @@
       <c r="C34" s="72">
         <v>0.54</v>
       </c>
-      <c r="D34" s="229" t="s">
+      <c r="D34" s="232" t="s">
         <v>291</v>
       </c>
-      <c r="E34" s="230"/>
-      <c r="F34" s="230"/>
-      <c r="G34" s="231"/>
+      <c r="E34" s="233"/>
+      <c r="F34" s="233"/>
+      <c r="G34" s="234"/>
     </row>
     <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="225" t="s">
+      <c r="A36" s="230" t="s">
         <v>315</v>
       </c>
-      <c r="B36" s="225"/>
-      <c r="C36" s="225"/>
-      <c r="D36" s="225"/>
-      <c r="E36" s="225"/>
-      <c r="F36" s="225"/>
-      <c r="G36" s="225"/>
-      <c r="H36" s="225"/>
-      <c r="I36" s="225"/>
+      <c r="B36" s="230"/>
+      <c r="C36" s="230"/>
+      <c r="D36" s="230"/>
+      <c r="E36" s="230"/>
+      <c r="F36" s="230"/>
+      <c r="G36" s="230"/>
+      <c r="H36" s="230"/>
+      <c r="I36" s="230"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="87" t="s">
@@ -16661,12 +16903,12 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="217" t="s">
+      <c r="A46" s="236" t="s">
         <v>318</v>
       </c>
-      <c r="B46" s="217"/>
-      <c r="C46" s="217"/>
-      <c r="D46" s="217"/>
+      <c r="B46" s="236"/>
+      <c r="C46" s="236"/>
+      <c r="D46" s="236"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="88" t="s">
@@ -16817,6 +17059,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="D6:D13"/>
+    <mergeCell ref="A2:I2"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="A25:I25"/>
@@ -16832,11 +17079,6 @@
     <mergeCell ref="D30:G30"/>
     <mergeCell ref="D31:G31"/>
     <mergeCell ref="D32:G32"/>
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="D28:G28"/>
-    <mergeCell ref="D6:D13"/>
-    <mergeCell ref="A2:I2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -16868,15 +17110,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="238" t="s">
+      <c r="A1" s="248" t="s">
         <v>347</v>
       </c>
-      <c r="B1" s="238"/>
-      <c r="C1" s="238"/>
-      <c r="D1" s="238"/>
-      <c r="E1" s="238"/>
-      <c r="F1" s="238"/>
-      <c r="G1" s="238"/>
+      <c r="B1" s="248"/>
+      <c r="C1" s="248"/>
+      <c r="D1" s="248"/>
+      <c r="E1" s="248"/>
+      <c r="F1" s="248"/>
+      <c r="G1" s="248"/>
     </row>
     <row r="2" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="158" t="s">
@@ -16900,11 +17142,11 @@
       <c r="G2" s="158" t="s">
         <v>344</v>
       </c>
-      <c r="I2" s="237" t="s">
+      <c r="I2" s="247" t="s">
         <v>197</v>
       </c>
-      <c r="J2" s="237"/>
-      <c r="K2" s="237"/>
+      <c r="J2" s="247"/>
+      <c r="K2" s="247"/>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
@@ -17357,20 +17599,20 @@
       <c r="J22" s="115" t="s">
         <v>217</v>
       </c>
-      <c r="K22" s="239" t="s">
+      <c r="K22" s="249" t="s">
         <v>307</v>
       </c>
-      <c r="L22" s="239"/>
-      <c r="M22" s="239"/>
-      <c r="N22" s="239"/>
-      <c r="O22" s="239"/>
-      <c r="P22" s="239"/>
-      <c r="Q22" s="239"/>
-      <c r="R22" s="239"/>
-      <c r="S22" s="239"/>
-      <c r="T22" s="239"/>
-      <c r="U22" s="239"/>
-      <c r="V22" s="239"/>
+      <c r="L22" s="249"/>
+      <c r="M22" s="249"/>
+      <c r="N22" s="249"/>
+      <c r="O22" s="249"/>
+      <c r="P22" s="249"/>
+      <c r="Q22" s="249"/>
+      <c r="R22" s="249"/>
+      <c r="S22" s="249"/>
+      <c r="T22" s="249"/>
+      <c r="U22" s="249"/>
+      <c r="V22" s="249"/>
     </row>
     <row r="23" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="36" t="s">
@@ -17476,10 +17718,10 @@
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="241"/>
-      <c r="B29" s="242"/>
-      <c r="C29" s="242"/>
-      <c r="D29" s="243"/>
+      <c r="A29" s="251"/>
+      <c r="B29" s="252"/>
+      <c r="C29" s="252"/>
+      <c r="D29" s="253"/>
       <c r="I29" s="43" t="s">
         <v>187</v>
       </c>
@@ -17496,10 +17738,10 @@
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" s="244" t="s">
+      <c r="A31" s="254" t="s">
         <v>181</v>
       </c>
-      <c r="B31" s="245"/>
+      <c r="B31" s="255"/>
       <c r="C31" s="68"/>
       <c r="I31" s="43" t="s">
         <v>189</v>
@@ -17521,20 +17763,20 @@
       <c r="J32" s="116" t="s">
         <v>308</v>
       </c>
-      <c r="K32" s="240" t="s">
+      <c r="K32" s="250" t="s">
         <v>306</v>
       </c>
-      <c r="L32" s="240"/>
-      <c r="M32" s="240"/>
-      <c r="N32" s="240"/>
-      <c r="O32" s="240"/>
-      <c r="P32" s="240"/>
-      <c r="Q32" s="240"/>
-      <c r="R32" s="240"/>
-      <c r="S32" s="240"/>
-      <c r="T32" s="240"/>
-      <c r="U32" s="240"/>
-      <c r="V32" s="240"/>
+      <c r="L32" s="250"/>
+      <c r="M32" s="250"/>
+      <c r="N32" s="250"/>
+      <c r="O32" s="250"/>
+      <c r="P32" s="250"/>
+      <c r="Q32" s="250"/>
+      <c r="R32" s="250"/>
+      <c r="S32" s="250"/>
+      <c r="T32" s="250"/>
+      <c r="U32" s="250"/>
+      <c r="V32" s="250"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="84" t="s">
@@ -17567,10 +17809,10 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="233" t="s">
+      <c r="A35" s="243" t="s">
         <v>184</v>
       </c>
-      <c r="B35" s="235" t="s">
+      <c r="B35" s="245" t="s">
         <v>219</v>
       </c>
       <c r="D35" s="90"/>
@@ -17580,8 +17822,8 @@
       <c r="J35" s="41"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="234"/>
-      <c r="B36" s="236"/>
+      <c r="A36" s="244"/>
+      <c r="B36" s="246"/>
       <c r="D36" s="90"/>
       <c r="I36" s="105" t="s">
         <v>296</v>
@@ -17700,15 +17942,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="238" t="s">
+      <c r="A1" s="248" t="s">
         <v>347</v>
       </c>
-      <c r="B1" s="238"/>
-      <c r="C1" s="238"/>
-      <c r="D1" s="238"/>
-      <c r="E1" s="238"/>
-      <c r="F1" s="238"/>
-      <c r="G1" s="238"/>
+      <c r="B1" s="248"/>
+      <c r="C1" s="248"/>
+      <c r="D1" s="248"/>
+      <c r="E1" s="248"/>
+      <c r="F1" s="248"/>
+      <c r="G1" s="248"/>
     </row>
     <row r="2" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="158" t="s">
@@ -17732,11 +17974,11 @@
       <c r="G2" s="158" t="s">
         <v>344</v>
       </c>
-      <c r="I2" s="237" t="s">
+      <c r="I2" s="247" t="s">
         <v>197</v>
       </c>
-      <c r="J2" s="237"/>
-      <c r="K2" s="237"/>
+      <c r="J2" s="247"/>
+      <c r="K2" s="247"/>
       <c r="O2" s="170" t="s">
         <v>351</v>
       </c>
@@ -18237,20 +18479,20 @@
       <c r="J22" s="115" t="s">
         <v>217</v>
       </c>
-      <c r="K22" s="239" t="s">
+      <c r="K22" s="249" t="s">
         <v>307</v>
       </c>
-      <c r="L22" s="239"/>
-      <c r="M22" s="239"/>
-      <c r="N22" s="239"/>
-      <c r="O22" s="239"/>
-      <c r="P22" s="239"/>
-      <c r="Q22" s="239"/>
-      <c r="R22" s="239"/>
-      <c r="S22" s="239"/>
-      <c r="T22" s="239"/>
-      <c r="U22" s="239"/>
-      <c r="V22" s="239"/>
+      <c r="L22" s="249"/>
+      <c r="M22" s="249"/>
+      <c r="N22" s="249"/>
+      <c r="O22" s="249"/>
+      <c r="P22" s="249"/>
+      <c r="Q22" s="249"/>
+      <c r="R22" s="249"/>
+      <c r="S22" s="249"/>
+      <c r="T22" s="249"/>
+      <c r="U22" s="249"/>
+      <c r="V22" s="249"/>
     </row>
     <row r="23" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="36" t="s">
@@ -18356,10 +18598,10 @@
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="241"/>
-      <c r="B29" s="242"/>
-      <c r="C29" s="242"/>
-      <c r="D29" s="243"/>
+      <c r="A29" s="251"/>
+      <c r="B29" s="252"/>
+      <c r="C29" s="252"/>
+      <c r="D29" s="253"/>
       <c r="I29" s="43" t="s">
         <v>187</v>
       </c>
@@ -18376,10 +18618,10 @@
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" s="244" t="s">
+      <c r="A31" s="254" t="s">
         <v>181</v>
       </c>
-      <c r="B31" s="245"/>
+      <c r="B31" s="255"/>
       <c r="C31" s="68"/>
       <c r="I31" s="43" t="s">
         <v>189</v>
@@ -18401,20 +18643,20 @@
       <c r="J32" s="116" t="s">
         <v>308</v>
       </c>
-      <c r="K32" s="240" t="s">
+      <c r="K32" s="250" t="s">
         <v>306</v>
       </c>
-      <c r="L32" s="240"/>
-      <c r="M32" s="240"/>
-      <c r="N32" s="240"/>
-      <c r="O32" s="240"/>
-      <c r="P32" s="240"/>
-      <c r="Q32" s="240"/>
-      <c r="R32" s="240"/>
-      <c r="S32" s="240"/>
-      <c r="T32" s="240"/>
-      <c r="U32" s="240"/>
-      <c r="V32" s="240"/>
+      <c r="L32" s="250"/>
+      <c r="M32" s="250"/>
+      <c r="N32" s="250"/>
+      <c r="O32" s="250"/>
+      <c r="P32" s="250"/>
+      <c r="Q32" s="250"/>
+      <c r="R32" s="250"/>
+      <c r="S32" s="250"/>
+      <c r="T32" s="250"/>
+      <c r="U32" s="250"/>
+      <c r="V32" s="250"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="84" t="s">
@@ -18445,10 +18687,10 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="233" t="s">
+      <c r="A35" s="243" t="s">
         <v>184</v>
       </c>
-      <c r="B35" s="235" t="s">
+      <c r="B35" s="245" t="s">
         <v>219</v>
       </c>
       <c r="I35" s="43" t="s">
@@ -18457,8 +18699,8 @@
       <c r="J35" s="41"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="234"/>
-      <c r="B36" s="236"/>
+      <c r="A36" s="244"/>
+      <c r="B36" s="246"/>
       <c r="I36" s="105" t="s">
         <v>296</v>
       </c>
@@ -18560,18 +18802,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="246" t="s">
+      <c r="A1" s="256" t="s">
         <v>464</v>
       </c>
-      <c r="B1" s="246"/>
-      <c r="C1" s="246"/>
-      <c r="D1" s="246"/>
-      <c r="E1" s="246"/>
-      <c r="F1" s="246"/>
-      <c r="G1" s="246"/>
-      <c r="H1" s="246"/>
-      <c r="I1" s="246"/>
-      <c r="J1" s="246"/>
+      <c r="B1" s="256"/>
+      <c r="C1" s="256"/>
+      <c r="D1" s="256"/>
+      <c r="E1" s="256"/>
+      <c r="F1" s="256"/>
+      <c r="G1" s="256"/>
+      <c r="H1" s="256"/>
+      <c r="I1" s="256"/>
+      <c r="J1" s="256"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="173" t="s">

</xml_diff>